<commit_message>
Add formula to drug table to get class name for row
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3691EB-02CC-4902-92EC-AA09BDD8EE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE3BED-8670-4FC9-89BA-B03ADFF101AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -117,15 +117,6 @@
   </si>
   <si>
     <t>E. coli</t>
-  </si>
-  <si>
-    <t>Amox-clav</t>
-  </si>
-  <si>
-    <t>Amp-sul</t>
-  </si>
-  <si>
-    <t>Amp/Amox</t>
   </si>
   <si>
     <t>Nitroimidazoles</t>
@@ -898,6 +889,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -999,7 +991,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="Table1" displayName="Table1" ref="O2:Q26" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="O2:Q26" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="0">
+      <calculatedColumnFormula>IF(A3=0,O2,A3)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="3"/>
   </tableColumns>
@@ -1277,7 +1271,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E33" sqref="E33"/>
+      <selection pane="topRight" activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1284,7 @@
     <col min="8" max="8" width="14.375" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.875" style="2"/>
     <col min="10" max="10" width="15.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" style="2" customWidth="1"/>
     <col min="13" max="13" width="16.5" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
@@ -1327,7 +1321,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="82" t="s">
         <v>1</v>
@@ -1336,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="85" t="s">
         <v>25</v>
@@ -1345,7 +1339,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="86" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H2" s="86" t="s">
         <v>4</v>
@@ -1357,20 +1351,20 @@
         <v>9</v>
       </c>
       <c r="K2" s="89" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L2" s="9"/>
       <c r="M2" s="90" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1392,17 +1386,18 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
       <c r="M3" s="19"/>
-      <c r="O3" s="6" t="s">
-        <v>23</v>
+      <c r="O3" s="6" t="str">
+        <f t="shared" ref="O3:O26" si="0">IF(A3=0,O2,A3)</f>
+        <v>Penicillin</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="21" t="str">
@@ -1419,17 +1414,18 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
-      <c r="O4" s="6" t="s">
-        <v>33</v>
+      <c r="O4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Anti-staphylococcal penicillins</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1443,22 +1439,24 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="24" t="s">
-        <v>28</v>
+      <c r="K5" s="24" t="str">
+        <f>$P5</f>
+        <v>Ampicillin, Amoxicillin</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
-      <c r="O5" s="6" t="s">
-        <v>34</v>
+      <c r="O5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aminopenicillins</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="25" t="str">
@@ -1475,17 +1473,18 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
       <c r="M6" s="28"/>
-      <c r="O6" s="6" t="s">
-        <v>35</v>
+      <c r="O6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1st-gen cephalosporin</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="25" t="str">
@@ -1505,8 +1504,9 @@
         <v>Cephotetan, Cefoxitin</v>
       </c>
       <c r="M7" s="28"/>
-      <c r="O7" s="6" t="s">
-        <v>36</v>
+      <c r="O7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2nd-gen cephalosporin</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>7</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="25" t="str">
@@ -1535,8 +1535,9 @@
       <c r="K8" s="27"/>
       <c r="L8" s="19"/>
       <c r="M8" s="28"/>
-      <c r="O8" s="6" t="s">
-        <v>37</v>
+      <c r="O8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>3rd-gen cephalosporin</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>8</v>
@@ -1560,8 +1561,9 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="28"/>
-      <c r="O9" s="6" t="s">
-        <v>37</v>
+      <c r="O9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>3rd-gen cephalosporin</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>11</v>
@@ -1570,7 +1572,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="31" t="str">
@@ -1587,8 +1589,9 @@
       <c r="K10" s="27"/>
       <c r="L10" s="19"/>
       <c r="M10" s="28"/>
-      <c r="O10" s="6" t="s">
-        <v>38</v>
+      <c r="O10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>4th-gen cephalosporin</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>10</v>
@@ -1597,7 +1600,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="33" t="str">
@@ -1612,18 +1615,20 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-      <c r="L11" s="36" t="s">
-        <v>26</v>
+      <c r="L11" s="36" t="str">
+        <f>$P11</f>
+        <v>Amoxicillin-Clavulanic Acid</v>
       </c>
       <c r="M11" s="19"/>
-      <c r="O11" s="6" t="s">
-        <v>39</v>
+      <c r="O11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1641,18 +1646,20 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
-      <c r="L12" s="36" t="s">
-        <v>27</v>
+      <c r="L12" s="36" t="str">
+        <f>$P12</f>
+        <v>Ampicillin/Sulbactam</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="6" t="s">
-        <v>39</v>
+      <c r="O12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1675,19 +1682,20 @@
       </c>
       <c r="L13" s="39"/>
       <c r="M13" s="19"/>
-      <c r="O13" s="6" t="s">
-        <v>39</v>
+      <c r="O13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="40" t="str">
@@ -1707,8 +1715,9 @@
       <c r="K14" s="41"/>
       <c r="L14" s="42"/>
       <c r="M14" s="19"/>
-      <c r="O14" s="6" t="s">
-        <v>47</v>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Carbapenems</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>12</v>
@@ -1732,8 +1741,9 @@
       <c r="K15" s="41"/>
       <c r="L15" s="42"/>
       <c r="M15" s="19"/>
-      <c r="O15" s="6" t="s">
-        <v>47</v>
+      <c r="O15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Carbapenems</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>13</v>
@@ -1748,7 +1758,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
@@ -1758,17 +1768,18 @@
       <c r="K16" s="45"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
-      <c r="O16" s="6" t="s">
-        <v>14</v>
+      <c r="O16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Monobactams</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="46" t="str">
@@ -1788,11 +1799,12 @@
       <c r="K17" s="49"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
-      <c r="O17" s="6" t="s">
-        <v>43</v>
+      <c r="O17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Quinolones</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="6"/>
     </row>
@@ -1816,8 +1828,9 @@
         <f>$P18</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="O18" s="6" t="s">
-        <v>43</v>
+      <c r="O18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Quinolones</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>15</v>
@@ -1844,8 +1857,9 @@
       <c r="K19" s="53"/>
       <c r="L19" s="53"/>
       <c r="M19" s="54"/>
-      <c r="O19" s="6" t="s">
-        <v>43</v>
+      <c r="O19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Quinolones</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>16</v>
@@ -1854,7 +1868,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -1871,11 +1885,12 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="O20" s="6" t="s">
-        <v>40</v>
+      <c r="O20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aminoglycosides</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Q20" s="6"/>
     </row>
@@ -1901,11 +1916,12 @@
         <v>Clindamycin</v>
       </c>
       <c r="M21" s="63"/>
-      <c r="O21" s="6" t="s">
-        <v>21</v>
+      <c r="O21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Lincosamide</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Q21" s="6"/>
     </row>
@@ -1934,11 +1950,12 @@
         <f>$P22</f>
         <v>Azithromycin</v>
       </c>
-      <c r="O22" s="6" t="s">
-        <v>19</v>
+      <c r="O22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Macrolides</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q22" s="6"/>
     </row>
@@ -1967,17 +1984,18 @@
         <f>$P23</f>
         <v>Doxycycline</v>
       </c>
-      <c r="O23" s="6" t="s">
-        <v>18</v>
+      <c r="O23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Tetracyclines</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="72" t="str">
         <f>$P24</f>
@@ -1994,17 +2012,18 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="O24" s="6" t="s">
-        <v>41</v>
+      <c r="O24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Glycopeptides</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="75" t="str">
         <f>$P25</f>
@@ -2025,19 +2044,20 @@
       </c>
       <c r="L25" s="19"/>
       <c r="M25" s="28"/>
-      <c r="O25" s="6" t="s">
-        <v>42</v>
+      <c r="O25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Antimetabolite</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>20</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" s="79"/>
       <c r="C26" s="79"/>
@@ -2054,17 +2074,18 @@
         <v>Metronidazole</v>
       </c>
       <c r="M26" s="79"/>
-      <c r="O26" s="6" t="s">
-        <v>29</v>
+      <c r="O26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Nitroimidazoles</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="6"/>
     </row>
     <row r="27" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>

</xml_diff>

<commit_message>
Move drug information to separate worksheet
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE3BED-8670-4FC9-89BA-B03ADFF101AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5F5680-A5DA-43FF-95F2-2F3F81ECA48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Antibiogram" sheetId="1" r:id="rId1"/>
+    <sheet name="Drug Information" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -889,7 +890,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -926,6 +926,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -988,16 +989,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="Table1" displayName="Table1" ref="O2:Q26" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="O2:Q26" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C25" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="0">
-      <calculatedColumnFormula>IF(A3=0,O2,A3)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="2">
+      <calculatedColumnFormula>IF(Antibiogram!A3=0,A1,Antibiogram!A3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1267,11 +1268,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P29" sqref="P29"/>
+      <selection pane="topRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1295,7 @@
     <col min="18" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -1319,7 +1320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>65</v>
       </c>
@@ -1357,24 +1358,15 @@
       <c r="M2" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="str">
-        <f>$P3</f>
+        <f>'Drug Information'!$B2</f>
         <v>Benzylpenicillin</v>
       </c>
       <c r="E3" s="19"/>
@@ -1386,22 +1378,14 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
       <c r="M3" s="19"/>
-      <c r="O3" s="6" t="str">
-        <f t="shared" ref="O3:O26" si="0">IF(A3=0,O2,A3)</f>
-        <v>Penicillin</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="21" t="str">
-        <f>$P4</f>
+        <f>'Drug Information'!$B3</f>
         <v>Naficillin, Oxacillin, Flucloxacillin</v>
       </c>
       <c r="D4" s="22"/>
@@ -1414,23 +1398,15 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
-      <c r="O4" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Anti-staphylococcal penicillins</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="21" t="str">
-        <f>$P5</f>
+        <f>'Drug Information'!$B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
       <c r="E5" s="23"/>
@@ -1440,27 +1416,19 @@
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="24" t="str">
-        <f>$P5</f>
+        <f>'Drug Information'!$B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
-      <c r="O5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Aminopenicillins</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="25" t="str">
-        <f>$P6</f>
+        <f>'Drug Information'!$B5</f>
         <v>Cefazolin, Cefalexin</v>
       </c>
       <c r="D6" s="26"/>
@@ -1473,22 +1441,14 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
       <c r="M6" s="28"/>
-      <c r="O6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>1st-gen cephalosporin</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="25" t="str">
-        <f>$P7</f>
+        <f>'Drug Information'!$B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
       <c r="D7" s="29"/>
@@ -1500,26 +1460,18 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="30" t="str">
-        <f>$P7</f>
+        <f>'Drug Information'!$B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
       <c r="M7" s="28"/>
-      <c r="O7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>2nd-gen cephalosporin</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="25" t="str">
-        <f>$P8</f>
+        <f>'Drug Information'!$B7</f>
         <v>Ceftriaxone</v>
       </c>
       <c r="D8" s="29"/>
@@ -1528,28 +1480,20 @@
       <c r="G8" s="27"/>
       <c r="H8" s="19"/>
       <c r="I8" s="25" t="str">
-        <f>$P8</f>
+        <f>'Drug Information'!$B7</f>
         <v>Ceftriaxone</v>
       </c>
       <c r="J8" s="29"/>
       <c r="K8" s="27"/>
       <c r="L8" s="19"/>
       <c r="M8" s="28"/>
-      <c r="O8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>3rd-gen cephalosporin</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="25" t="str">
-        <f>$P9</f>
+        <f>'Drug Information'!$B8</f>
         <v>Ceftazidime</v>
       </c>
       <c r="E9" s="29"/>
@@ -1561,22 +1505,14 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="28"/>
-      <c r="O9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>3rd-gen cephalosporin</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="31" t="str">
-        <f>$P10</f>
+        <f>'Drug Information'!$B9</f>
         <v>Cefepime</v>
       </c>
       <c r="D10" s="32"/>
@@ -1589,22 +1525,14 @@
       <c r="K10" s="27"/>
       <c r="L10" s="19"/>
       <c r="M10" s="28"/>
-      <c r="O10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>4th-gen cephalosporin</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="33" t="str">
-        <f>$P11</f>
+        <f>'Drug Information'!$B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
       <c r="D11" s="34"/>
@@ -1616,26 +1544,16 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="36" t="str">
-        <f>$P11</f>
+        <f>'Drug Information'!$B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
       <c r="M11" s="19"/>
-      <c r="O11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Aminopenicillins with beta-lactamase inhibitors</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="19"/>
       <c r="C12" s="33" t="str">
-        <f>$P12</f>
+        <f>'Drug Information'!$B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
       <c r="D12" s="34"/>
@@ -1647,26 +1565,16 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="36" t="str">
-        <f>$P12</f>
+        <f>'Drug Information'!$B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Aminopenicillins with beta-lactamase inhibitors</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="19"/>
       <c r="C13" s="37" t="str">
-        <f>$P13</f>
+        <f>'Drug Information'!$B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
       <c r="D13" s="38"/>
@@ -1677,29 +1585,19 @@
       <c r="I13" s="39"/>
       <c r="J13" s="19"/>
       <c r="K13" s="37" t="str">
-        <f>$P13</f>
+        <f>'Drug Information'!$B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
       <c r="L13" s="39"/>
       <c r="M13" s="19"/>
-      <c r="O13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Aminopenicillins with beta-lactamase inhibitors</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="40" t="str">
-        <f>$P14</f>
+        <f>'Drug Information'!$B13</f>
         <v>Ertapenem</v>
       </c>
       <c r="D14" s="41"/>
@@ -1708,27 +1606,19 @@
       <c r="G14" s="42"/>
       <c r="H14" s="19"/>
       <c r="I14" s="40" t="str">
-        <f>$P14</f>
+        <f>'Drug Information'!$B13</f>
         <v>Ertapenem</v>
       </c>
       <c r="J14" s="41"/>
       <c r="K14" s="41"/>
       <c r="L14" s="42"/>
       <c r="M14" s="19"/>
-      <c r="O14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Carbapenems</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="19"/>
       <c r="C15" s="40" t="str">
-        <f>$P15</f>
+        <f>'Drug Information'!$B14</f>
         <v>Imipenem, Meropenem</v>
       </c>
       <c r="D15" s="41"/>
@@ -1741,16 +1631,8 @@
       <c r="K15" s="41"/>
       <c r="L15" s="42"/>
       <c r="M15" s="19"/>
-      <c r="O15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Carbapenems</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1768,27 +1650,19 @@
       <c r="K16" s="45"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
-      <c r="O16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Monobactams</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="46" t="str">
-        <f>$P17</f>
+        <f>'Drug Information'!$B16</f>
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="47" t="str">
-        <f>$P17</f>
+        <f>'Drug Information'!$B16</f>
         <v>Ciprofloxacin</v>
       </c>
       <c r="F17" s="48"/>
@@ -1799,20 +1673,12 @@
       <c r="K17" s="49"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
-      <c r="O17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Quinolones</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="19"/>
       <c r="C18" s="47" t="str">
-        <f>$P18</f>
+        <f>'Drug Information'!$B17</f>
         <v>Levofloxacin</v>
       </c>
       <c r="D18" s="48"/>
@@ -1825,23 +1691,15 @@
       <c r="K18" s="51"/>
       <c r="L18" s="19"/>
       <c r="M18" s="46" t="str">
-        <f>$P18</f>
+        <f>'Drug Information'!$B17</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="O18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Quinolones</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="28"/>
       <c r="C19" s="52" t="str">
-        <f>$P19</f>
+        <f>'Drug Information'!$B18</f>
         <v>Moxifloxacin</v>
       </c>
       <c r="D19" s="53"/>
@@ -1850,23 +1708,15 @@
       <c r="G19" s="54"/>
       <c r="H19" s="28"/>
       <c r="I19" s="52" t="str">
-        <f>$P19</f>
+        <f>'Drug Information'!$B18</f>
         <v>Moxifloxacin</v>
       </c>
       <c r="J19" s="53"/>
       <c r="K19" s="53"/>
       <c r="L19" s="53"/>
       <c r="M19" s="54"/>
-      <c r="O19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Quinolones</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="6"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -1874,7 +1724,7 @@
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="55" t="str">
-        <f>$P20</f>
+        <f>'Drug Information'!$B19</f>
         <v>Gentamicin, Tobramycin, Amikacin</v>
       </c>
       <c r="F20" s="56"/>
@@ -1885,21 +1735,13 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="O20" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Aminoglycosides</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="59" t="str">
-        <f>$P21</f>
+        <f>'Drug Information'!$B20</f>
         <v>Clindamycin</v>
       </c>
       <c r="C21" s="60"/>
@@ -1912,26 +1754,18 @@
       <c r="J21" s="28"/>
       <c r="K21" s="28"/>
       <c r="L21" s="62" t="str">
-        <f>$P21</f>
+        <f>'Drug Information'!$B20</f>
         <v>Clindamycin</v>
       </c>
       <c r="M21" s="63"/>
-      <c r="O21" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Lincosamide</v>
-      </c>
-      <c r="P21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="64" t="str">
-        <f>$P22</f>
+        <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
       <c r="D22" s="65"/>
@@ -1942,29 +1776,21 @@
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
       <c r="K22" s="66" t="str">
-        <f>$P22</f>
+        <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
       <c r="L22" s="28"/>
       <c r="M22" s="67" t="str">
-        <f>$P22</f>
+        <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
-      <c r="O22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Macrolides</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="68" t="str">
-        <f>$P23</f>
+        <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
       <c r="C23" s="69"/>
@@ -1976,29 +1802,21 @@
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
       <c r="K23" s="71" t="str">
-        <f>$P23</f>
+        <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
       <c r="L23" s="28"/>
       <c r="M23" s="71" t="str">
-        <f>$P23</f>
+        <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
-      <c r="O23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Tetracyclines</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="72" t="str">
-        <f>$P24</f>
+        <f>'Drug Information'!$B23</f>
         <v>Vancomycin</v>
       </c>
       <c r="C24" s="73"/>
@@ -2012,21 +1830,13 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="O24" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Glycopeptides</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="75" t="str">
-        <f>$P25</f>
+        <f>'Drug Information'!$B24</f>
         <v>TMP/SMX</v>
       </c>
       <c r="C25" s="76"/>
@@ -2044,18 +1854,8 @@
       </c>
       <c r="L25" s="19"/>
       <c r="M25" s="28"/>
-      <c r="O25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Antimetabolite</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -2070,20 +1870,12 @@
       <c r="J26" s="79"/>
       <c r="K26" s="79"/>
       <c r="L26" s="80" t="str">
-        <f>$P26</f>
+        <f>'Drug Information'!$B25</f>
         <v>Metronidazole</v>
       </c>
       <c r="M26" s="79"/>
-      <c r="O26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Nitroimidazoles</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>49</v>
       </c>
@@ -2140,9 +1932,291 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="57" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5474896F-AAD3-451A-94EF-CDE00ADCB149}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="str">
+        <f>IF(Antibiogram!A3=0,A1,Antibiogram!A3)</f>
+        <v>Penicillin</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="str">
+        <f>IF(Antibiogram!A4=0,A2,Antibiogram!A4)</f>
+        <v>Anti-staphylococcal penicillins</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="str">
+        <f>IF(Antibiogram!A5=0,A3,Antibiogram!A5)</f>
+        <v>Aminopenicillins</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="str">
+        <f>IF(Antibiogram!A6=0,A4,Antibiogram!A6)</f>
+        <v>1st-gen cephalosporin</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
+        <f>IF(Antibiogram!A7=0,A5,Antibiogram!A7)</f>
+        <v>2nd-gen cephalosporin</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="str">
+        <f>IF(Antibiogram!A8=0,A6,Antibiogram!A8)</f>
+        <v>3rd-gen cephalosporin</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="str">
+        <f>IF(Antibiogram!A9=0,A7,Antibiogram!A9)</f>
+        <v>3rd-gen cephalosporin</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="str">
+        <f>IF(Antibiogram!A10=0,A8,Antibiogram!A10)</f>
+        <v>4th-gen cephalosporin</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="str">
+        <f>IF(Antibiogram!A11=0,A9,Antibiogram!A11)</f>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="str">
+        <f>IF(Antibiogram!A12=0,A10,Antibiogram!A12)</f>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="str">
+        <f>IF(Antibiogram!A13=0,A11,Antibiogram!A13)</f>
+        <v>Aminopenicillins with beta-lactamase inhibitors</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="str">
+        <f>IF(Antibiogram!A14=0,A12,Antibiogram!A14)</f>
+        <v>Carbapenems</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="str">
+        <f>IF(Antibiogram!A15=0,A13,Antibiogram!A15)</f>
+        <v>Carbapenems</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="str">
+        <f>IF(Antibiogram!A16=0,A14,Antibiogram!A16)</f>
+        <v>Monobactams</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="str">
+        <f>IF(Antibiogram!A17=0,A15,Antibiogram!A17)</f>
+        <v>Quinolones</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="str">
+        <f>IF(Antibiogram!A18=0,A16,Antibiogram!A18)</f>
+        <v>Quinolones</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="str">
+        <f>IF(Antibiogram!A19=0,A17,Antibiogram!A19)</f>
+        <v>Quinolones</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="str">
+        <f>IF(Antibiogram!A20=0,A18,Antibiogram!A20)</f>
+        <v>Aminoglycosides</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="str">
+        <f>IF(Antibiogram!A21=0,A19,Antibiogram!A21)</f>
+        <v>Lincosamide</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="str">
+        <f>IF(Antibiogram!A22=0,A20,Antibiogram!A22)</f>
+        <v>Macrolides</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="str">
+        <f>IF(Antibiogram!A23=0,A21,Antibiogram!A23)</f>
+        <v>Tetracyclines</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="str">
+        <f>IF(Antibiogram!A24=0,A22,Antibiogram!A24)</f>
+        <v>Glycopeptides</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="str">
+        <f>IF(Antibiogram!A25=0,A23,Antibiogram!A25)</f>
+        <v>Antimetabolite</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="str">
+        <f>IF(Antibiogram!A26=0,A24,Antibiogram!A26)</f>
+        <v>Nitroimidazoles</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add coverage to drug information table (1=Yes, 0=No) & create test antibiogram using formulae
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5F5680-A5DA-43FF-95F2-2F3F81ECA48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F054E16-CE1E-455A-A5E0-C2C4CE8BBEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="1" r:id="rId1"/>
     <sheet name="Drug Information" sheetId="2" r:id="rId2"/>
+    <sheet name="test antibiogram with formulae" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'test antibiogram with formulae'!$A$1:$N$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -239,6 +241,9 @@
   </si>
   <si>
     <t>Drug Class</t>
+  </si>
+  <si>
+    <t>Drug Name</t>
   </si>
 </sst>
 </file>
@@ -602,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -617,7 +622,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -865,6 +869,18 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -872,24 +888,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="19">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -908,6 +926,292 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -927,42 +1231,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -989,14 +1258,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C25" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
-  <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:O25" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:O25" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
+  <tableColumns count="15">
+    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="18">
       <calculatedColumnFormula>IF(Antibiogram!A3=0,A1,Antibiogram!A3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1266,13 +1547,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I33" sqref="I33"/>
+      <selection pane="topRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1297,23 +1579,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="11" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1321,41 +1603,41 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="I2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="88" t="s">
+      <c r="J2" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="90" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="89" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1363,424 +1645,424 @@
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20" t="str">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="str">
         <f>'Drug Information'!$B2</f>
         <v>Benzylpenicillin</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21" t="str">
+      <c r="B4" s="18"/>
+      <c r="C4" s="20" t="str">
         <f>'Drug Information'!$B3</f>
         <v>Naficillin, Oxacillin, Flucloxacillin</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="21" t="str">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="20" t="str">
         <f>'Drug Information'!$B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="24" t="str">
+      <c r="E5" s="22"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="23" t="str">
         <f>'Drug Information'!$B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="25" t="str">
+      <c r="B6" s="18"/>
+      <c r="C6" s="24" t="str">
         <f>'Drug Information'!$B5</f>
         <v>Cefazolin, Cefalexin</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="28"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="27"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="25" t="str">
+      <c r="B7" s="18"/>
+      <c r="C7" s="24" t="str">
         <f>'Drug Information'!$B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="30" t="str">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="29" t="str">
         <f>'Drug Information'!$B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="M7" s="28"/>
+      <c r="M7" s="27"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="25" t="str">
+      <c r="B8" s="18"/>
+      <c r="C8" s="24" t="str">
         <f>'Drug Information'!$B7</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="25" t="str">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="24" t="str">
         <f>'Drug Information'!$B7</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="27"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="25" t="str">
+      <c r="A9" s="6"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="24" t="str">
         <f>'Drug Information'!$B8</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="27"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="31" t="str">
+      <c r="B10" s="18"/>
+      <c r="C10" s="30" t="str">
         <f>'Drug Information'!$B9</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="28"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="27"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="33" t="str">
+      <c r="B11" s="18"/>
+      <c r="C11" s="32" t="str">
         <f>'Drug Information'!$B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="36" t="str">
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="35" t="str">
         <f>'Drug Information'!$B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="M11" s="19"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="33" t="str">
+      <c r="A12" s="6"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="32" t="str">
         <f>'Drug Information'!$B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="36" t="str">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="35" t="str">
         <f>'Drug Information'!$B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="M12" s="19"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="37" t="str">
+      <c r="A13" s="6"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="36" t="str">
         <f>'Drug Information'!$B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="37" t="str">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="36" t="str">
         <f>'Drug Information'!$B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="19"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="40" t="str">
+      <c r="B14" s="18"/>
+      <c r="C14" s="39" t="str">
         <f>'Drug Information'!$B13</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="40" t="str">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="39" t="str">
         <f>'Drug Information'!$B13</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="19"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="40" t="str">
+      <c r="A15" s="6"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="39" t="str">
         <f>'Drug Information'!$B14</f>
         <v>Imipenem, Meropenem</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="19"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="43" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="46" t="str">
+      <c r="B17" s="18"/>
+      <c r="C17" s="45" t="str">
         <f>'Drug Information'!$B16</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="47" t="str">
+      <c r="D17" s="18"/>
+      <c r="E17" s="46" t="str">
         <f>'Drug Information'!$B16</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="47" t="str">
+      <c r="A18" s="6"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="46" t="str">
         <f>'Drug Information'!$B17</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="46" t="str">
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="45" t="str">
         <f>'Drug Information'!$B17</f>
         <v>Levofloxacin</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="52" t="str">
+      <c r="A19" s="6"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="51" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="52" t="str">
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="51" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="54"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="53"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="55" t="str">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="54" t="str">
         <f>'Drug Information'!$B19</f>
         <v>Gentamicin, Tobramycin, Amikacin</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="59" t="str">
+      <c r="B21" s="58" t="str">
         <f>'Drug Information'!$B20</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="62" t="str">
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="61" t="str">
         <f>'Drug Information'!$B20</f>
         <v>Clindamycin</v>
       </c>
-      <c r="M21" s="63"/>
+      <c r="M21" s="62"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="64" t="str">
+      <c r="B22" s="27"/>
+      <c r="C22" s="63" t="str">
         <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="65"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="66" t="str">
+      <c r="D22" s="64"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="65" t="str">
         <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="67" t="str">
+      <c r="L22" s="27"/>
+      <c r="M22" s="66" t="str">
         <f>'Drug Information'!$B21</f>
         <v>Azithromycin</v>
       </c>
@@ -1789,24 +2071,24 @@
       <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="68" t="str">
+      <c r="B23" s="67" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="71" t="str">
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="70" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="71" t="str">
+      <c r="L23" s="27"/>
+      <c r="M23" s="70" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Doxycycline</v>
       </c>
@@ -1815,82 +2097,82 @@
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="72" t="str">
+      <c r="B24" s="71" t="str">
         <f>'Drug Information'!$B23</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="75" t="str">
+      <c r="B25" s="74" t="str">
         <f>'Drug Information'!$B24</f>
         <v>TMP/SMX</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="78" t="s">
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="78" t="s">
+      <c r="J25" s="27"/>
+      <c r="K25" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="28"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="27"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="80" t="str">
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="79" t="str">
         <f>'Drug Information'!$B25</f>
         <v>Metronidazole</v>
       </c>
-      <c r="M26" s="79"/>
+      <c r="M26" s="78"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -1941,277 +2223,906 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H20"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="93" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="92" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="92" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="92" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="92" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="92" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="92" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.125" style="92" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.125" style="92" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.125" style="92" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.375" style="92" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="92" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" style="92" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="92"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="91" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="str">
+      <c r="D1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="91" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="90" t="str">
         <f>IF(Antibiogram!A3=0,A1,Antibiogram!A3)</f>
         <v>Penicillin</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="str">
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91">
+        <v>1</v>
+      </c>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="90" t="str">
         <f>IF(Antibiogram!A4=0,A2,Antibiogram!A4)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="str">
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91">
+        <v>1</v>
+      </c>
+      <c r="F3" s="91">
+        <v>1</v>
+      </c>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="90" t="str">
         <f>IF(Antibiogram!A5=0,A3,Antibiogram!A5)</f>
         <v>Aminopenicillins</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="str">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91">
+        <v>1</v>
+      </c>
+      <c r="G4" s="91">
+        <v>1</v>
+      </c>
+      <c r="H4" s="91">
+        <v>1</v>
+      </c>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91">
+        <v>1</v>
+      </c>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="90" t="str">
         <f>IF(Antibiogram!A6=0,A4,Antibiogram!A6)</f>
         <v>1st-gen cephalosporin</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="str">
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91">
+        <v>1</v>
+      </c>
+      <c r="F5" s="91">
+        <v>1</v>
+      </c>
+      <c r="G5" s="91">
+        <v>1</v>
+      </c>
+      <c r="H5" s="91">
+        <v>1</v>
+      </c>
+      <c r="I5" s="91">
+        <v>1</v>
+      </c>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="90" t="str">
         <f>IF(Antibiogram!A7=0,A5,Antibiogram!A7)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="str">
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91">
+        <v>1</v>
+      </c>
+      <c r="F6" s="91">
+        <v>1</v>
+      </c>
+      <c r="G6" s="91">
+        <v>1</v>
+      </c>
+      <c r="H6" s="91">
+        <v>1</v>
+      </c>
+      <c r="I6" s="91">
+        <v>1</v>
+      </c>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91">
+        <v>1</v>
+      </c>
+      <c r="O6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="90" t="str">
         <f>IF(Antibiogram!A8=0,A6,Antibiogram!A8)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="str">
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91">
+        <v>1</v>
+      </c>
+      <c r="F7" s="91">
+        <v>1</v>
+      </c>
+      <c r="G7" s="91">
+        <v>1</v>
+      </c>
+      <c r="H7" s="91">
+        <v>1</v>
+      </c>
+      <c r="I7" s="91">
+        <v>1</v>
+      </c>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91">
+        <v>1</v>
+      </c>
+      <c r="L7" s="91">
+        <v>1</v>
+      </c>
+      <c r="M7" s="91">
+        <v>1</v>
+      </c>
+      <c r="N7" s="91"/>
+      <c r="O7" s="91"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="90" t="str">
         <f>IF(Antibiogram!A9=0,A7,Antibiogram!A9)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="str">
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91">
+        <v>1</v>
+      </c>
+      <c r="G8" s="91">
+        <v>1</v>
+      </c>
+      <c r="H8" s="91">
+        <v>1</v>
+      </c>
+      <c r="I8" s="91">
+        <v>1</v>
+      </c>
+      <c r="J8" s="91">
+        <v>1</v>
+      </c>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="91"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="90" t="str">
         <f>IF(Antibiogram!A10=0,A8,Antibiogram!A10)</f>
         <v>4th-gen cephalosporin</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="str">
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91">
+        <v>1</v>
+      </c>
+      <c r="F9" s="91">
+        <v>1</v>
+      </c>
+      <c r="G9" s="91">
+        <v>1</v>
+      </c>
+      <c r="H9" s="91">
+        <v>1</v>
+      </c>
+      <c r="I9" s="91">
+        <v>1</v>
+      </c>
+      <c r="J9" s="91">
+        <v>1</v>
+      </c>
+      <c r="K9" s="91">
+        <v>1</v>
+      </c>
+      <c r="L9" s="91">
+        <v>1</v>
+      </c>
+      <c r="M9" s="91">
+        <v>1</v>
+      </c>
+      <c r="N9" s="91"/>
+      <c r="O9" s="91"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="90" t="str">
         <f>IF(Antibiogram!A11=0,A9,Antibiogram!A11)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="91" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="str">
+      <c r="D10" s="91"/>
+      <c r="E10" s="91">
+        <v>1</v>
+      </c>
+      <c r="F10" s="91">
+        <v>1</v>
+      </c>
+      <c r="G10" s="91">
+        <v>1</v>
+      </c>
+      <c r="H10" s="91">
+        <v>1</v>
+      </c>
+      <c r="I10" s="91">
+        <v>1</v>
+      </c>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91">
+        <v>1</v>
+      </c>
+      <c r="O10" s="91"/>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="90" t="str">
         <f>IF(Antibiogram!A12=0,A10,Antibiogram!A12)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="91" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="str">
+      <c r="D11" s="91"/>
+      <c r="E11" s="91">
+        <v>1</v>
+      </c>
+      <c r="F11" s="91">
+        <v>1</v>
+      </c>
+      <c r="G11" s="91">
+        <v>1</v>
+      </c>
+      <c r="H11" s="91">
+        <v>1</v>
+      </c>
+      <c r="I11" s="91">
+        <v>1</v>
+      </c>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91">
+        <v>1</v>
+      </c>
+      <c r="O11" s="91"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="90" t="str">
         <f>IF(Antibiogram!A13=0,A11,Antibiogram!A13)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="91" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="str">
+      <c r="D12" s="91"/>
+      <c r="E12" s="91">
+        <v>1</v>
+      </c>
+      <c r="F12" s="91">
+        <v>1</v>
+      </c>
+      <c r="G12" s="91">
+        <v>1</v>
+      </c>
+      <c r="H12" s="91">
+        <v>1</v>
+      </c>
+      <c r="I12" s="91">
+        <v>1</v>
+      </c>
+      <c r="J12" s="91">
+        <v>1</v>
+      </c>
+      <c r="K12" s="91">
+        <v>1</v>
+      </c>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91">
+        <v>1</v>
+      </c>
+      <c r="N12" s="91">
+        <v>1</v>
+      </c>
+      <c r="O12" s="91"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="90" t="str">
         <f>IF(Antibiogram!A14=0,A12,Antibiogram!A14)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="str">
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91">
+        <v>1</v>
+      </c>
+      <c r="F13" s="91">
+        <v>1</v>
+      </c>
+      <c r="G13" s="91">
+        <v>1</v>
+      </c>
+      <c r="H13" s="91">
+        <v>1</v>
+      </c>
+      <c r="I13" s="91">
+        <v>1</v>
+      </c>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91">
+        <v>1</v>
+      </c>
+      <c r="L13" s="91">
+        <v>1</v>
+      </c>
+      <c r="M13" s="91">
+        <v>1</v>
+      </c>
+      <c r="N13" s="91">
+        <v>1</v>
+      </c>
+      <c r="O13" s="91"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="90" t="str">
         <f>IF(Antibiogram!A15=0,A13,Antibiogram!A15)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="str">
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91">
+        <v>1</v>
+      </c>
+      <c r="F14" s="91">
+        <v>1</v>
+      </c>
+      <c r="G14" s="91">
+        <v>1</v>
+      </c>
+      <c r="H14" s="91">
+        <v>1</v>
+      </c>
+      <c r="I14" s="91">
+        <v>1</v>
+      </c>
+      <c r="J14" s="91">
+        <v>1</v>
+      </c>
+      <c r="K14" s="91">
+        <v>1</v>
+      </c>
+      <c r="L14" s="91">
+        <v>1</v>
+      </c>
+      <c r="M14" s="91">
+        <v>1</v>
+      </c>
+      <c r="N14" s="91">
+        <v>1</v>
+      </c>
+      <c r="O14" s="91"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="90" t="str">
         <f>IF(Antibiogram!A16=0,A14,Antibiogram!A16)</f>
         <v>Monobactams</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="str">
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91">
+        <v>1</v>
+      </c>
+      <c r="H15" s="91">
+        <v>1</v>
+      </c>
+      <c r="I15" s="91">
+        <v>1</v>
+      </c>
+      <c r="J15" s="91">
+        <v>1</v>
+      </c>
+      <c r="K15" s="91">
+        <v>1</v>
+      </c>
+      <c r="L15" s="91">
+        <v>1</v>
+      </c>
+      <c r="M15" s="91">
+        <v>1</v>
+      </c>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="90" t="str">
         <f>IF(Antibiogram!A17=0,A15,Antibiogram!A17)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="str">
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91">
+        <v>1</v>
+      </c>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91">
+        <v>1</v>
+      </c>
+      <c r="H16" s="91">
+        <v>1</v>
+      </c>
+      <c r="I16" s="91">
+        <v>1</v>
+      </c>
+      <c r="J16" s="91">
+        <v>1</v>
+      </c>
+      <c r="K16" s="91">
+        <v>1</v>
+      </c>
+      <c r="L16" s="91">
+        <v>1</v>
+      </c>
+      <c r="M16" s="91">
+        <v>1</v>
+      </c>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="90" t="str">
         <f>IF(Antibiogram!A18=0,A16,Antibiogram!A18)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="str">
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91">
+        <v>1</v>
+      </c>
+      <c r="F17" s="91">
+        <v>1</v>
+      </c>
+      <c r="G17" s="91">
+        <v>1</v>
+      </c>
+      <c r="H17" s="91">
+        <v>1</v>
+      </c>
+      <c r="I17" s="91">
+        <v>1</v>
+      </c>
+      <c r="J17" s="91">
+        <v>1</v>
+      </c>
+      <c r="K17" s="91">
+        <v>1</v>
+      </c>
+      <c r="L17" s="91">
+        <v>1</v>
+      </c>
+      <c r="M17" s="91">
+        <v>1</v>
+      </c>
+      <c r="N17" s="91"/>
+      <c r="O17" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="90" t="str">
         <f>IF(Antibiogram!A19=0,A17,Antibiogram!A19)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="str">
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91">
+        <v>1</v>
+      </c>
+      <c r="F18" s="91">
+        <v>1</v>
+      </c>
+      <c r="G18" s="91">
+        <v>1</v>
+      </c>
+      <c r="H18" s="91">
+        <v>1</v>
+      </c>
+      <c r="I18" s="91">
+        <v>1</v>
+      </c>
+      <c r="J18" s="91"/>
+      <c r="K18" s="91">
+        <v>1</v>
+      </c>
+      <c r="L18" s="91">
+        <v>1</v>
+      </c>
+      <c r="M18" s="91">
+        <v>1</v>
+      </c>
+      <c r="N18" s="91">
+        <v>1</v>
+      </c>
+      <c r="O18" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="90" t="str">
         <f>IF(Antibiogram!A20=0,A18,Antibiogram!A20)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="str">
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91">
+        <v>1</v>
+      </c>
+      <c r="H19" s="91">
+        <v>1</v>
+      </c>
+      <c r="I19" s="91">
+        <v>1</v>
+      </c>
+      <c r="J19" s="91">
+        <v>1</v>
+      </c>
+      <c r="K19" s="91">
+        <v>1</v>
+      </c>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="90" t="str">
         <f>IF(Antibiogram!A21=0,A19,Antibiogram!A21)</f>
         <v>Lincosamide</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="str">
+      <c r="C20" s="91"/>
+      <c r="D20" s="91">
+        <v>1</v>
+      </c>
+      <c r="E20" s="91">
+        <v>1</v>
+      </c>
+      <c r="F20" s="91">
+        <v>1</v>
+      </c>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91">
+        <v>1</v>
+      </c>
+      <c r="O20" s="91"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="90" t="str">
         <f>IF(Antibiogram!A22=0,A20,Antibiogram!A22)</f>
         <v>Macrolides</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="str">
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91">
+        <v>1</v>
+      </c>
+      <c r="F21" s="91">
+        <v>1</v>
+      </c>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="91">
+        <v>1</v>
+      </c>
+      <c r="N21" s="91"/>
+      <c r="O21" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="90" t="str">
         <f>IF(Antibiogram!A23=0,A21,Antibiogram!A23)</f>
         <v>Tetracyclines</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="str">
+      <c r="C22" s="91"/>
+      <c r="D22" s="91">
+        <v>1</v>
+      </c>
+      <c r="E22" s="91">
+        <v>1</v>
+      </c>
+      <c r="F22" s="91">
+        <v>1</v>
+      </c>
+      <c r="G22" s="91">
+        <v>1</v>
+      </c>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91">
+        <v>1</v>
+      </c>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="90" t="str">
         <f>IF(Antibiogram!A24=0,A22,Antibiogram!A24)</f>
         <v>Glycopeptides</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="str">
+      <c r="C23" s="91"/>
+      <c r="D23" s="91">
+        <v>1</v>
+      </c>
+      <c r="E23" s="91">
+        <v>1</v>
+      </c>
+      <c r="F23" s="91">
+        <v>1</v>
+      </c>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="90" t="str">
         <f>IF(Antibiogram!A25=0,A23,Antibiogram!A25)</f>
         <v>Antimetabolite</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="91" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="str">
+      <c r="D24" s="91">
+        <v>1</v>
+      </c>
+      <c r="E24" s="91">
+        <v>1</v>
+      </c>
+      <c r="F24" s="91">
+        <v>1</v>
+      </c>
+      <c r="G24" s="91">
+        <v>1</v>
+      </c>
+      <c r="H24" s="91">
+        <v>1</v>
+      </c>
+      <c r="I24" s="91">
+        <v>1</v>
+      </c>
+      <c r="J24" s="91"/>
+      <c r="K24" s="91">
+        <v>1</v>
+      </c>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91">
+        <v>1</v>
+      </c>
+      <c r="N24" s="91"/>
+      <c r="O24" s="91"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="90" t="str">
         <f>IF(Antibiogram!A26=0,A24,Antibiogram!A26)</f>
         <v>Nitroimidazoles</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="91"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91">
+        <v>1</v>
+      </c>
+      <c r="O25" s="91"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2219,4 +3130,1504 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38DBB59-9153-4008-AD05-F81C07E1E687}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I42" sqref="I42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
+    <col min="16" max="16" width="42.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="89" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f>'Drug Information'!B2</f>
+        <v>Benzylpenicillin</v>
+      </c>
+      <c r="C3" s="18" t="str">
+        <f>IF('Drug Information'!D2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D3" s="18" t="str">
+        <f>IF('Drug Information'!E2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E3" s="18" t="str">
+        <f>IF('Drug Information'!F2=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F3" s="18" t="str">
+        <f>IF('Drug Information'!G2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G3" s="18" t="str">
+        <f>IF('Drug Information'!H2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H3" s="18" t="str">
+        <f>IF('Drug Information'!I2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I3" s="18" t="str">
+        <f>IF('Drug Information'!J2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J3" s="18" t="str">
+        <f>IF('Drug Information'!K2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K3" s="18" t="str">
+        <f>IF('Drug Information'!L2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L3" s="18" t="str">
+        <f>IF('Drug Information'!M2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M3" s="18" t="str">
+        <f>IF('Drug Information'!N2=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N3" s="18" t="str">
+        <f>IF('Drug Information'!O2=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f>'Drug Information'!B3</f>
+        <v>Naficillin, Oxacillin, Flucloxacillin</v>
+      </c>
+      <c r="C4" s="18" t="str">
+        <f>IF('Drug Information'!D3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D4" s="18" t="str">
+        <f>IF('Drug Information'!E3=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E4" s="18" t="str">
+        <f>IF('Drug Information'!F3=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F4" s="18" t="str">
+        <f>IF('Drug Information'!G3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G4" s="18" t="str">
+        <f>IF('Drug Information'!H3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H4" s="18" t="str">
+        <f>IF('Drug Information'!I3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I4" s="18" t="str">
+        <f>IF('Drug Information'!J3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J4" s="18" t="str">
+        <f>IF('Drug Information'!K3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K4" s="18" t="str">
+        <f>IF('Drug Information'!L3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L4" s="18" t="str">
+        <f>IF('Drug Information'!M3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M4" s="18" t="str">
+        <f>IF('Drug Information'!N3=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N4" s="18" t="str">
+        <f>IF('Drug Information'!O3=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f>'Drug Information'!B4</f>
+        <v>Ampicillin, Amoxicillin</v>
+      </c>
+      <c r="C5" s="18" t="str">
+        <f>IF('Drug Information'!D4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D5" s="18" t="str">
+        <f>IF('Drug Information'!E4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E5" s="18" t="str">
+        <f>IF('Drug Information'!F4=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F5" s="18" t="str">
+        <f>IF('Drug Information'!G4=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G5" s="18" t="str">
+        <f>IF('Drug Information'!H4=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H5" s="18" t="str">
+        <f>IF('Drug Information'!I4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I5" s="18" t="str">
+        <f>IF('Drug Information'!J4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J5" s="18" t="str">
+        <f>IF('Drug Information'!K4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K5" s="18" t="str">
+        <f>IF('Drug Information'!L4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L5" s="18" t="str">
+        <f>IF('Drug Information'!M4=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M5" s="18" t="str">
+        <f>IF('Drug Information'!N4=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N5" s="18" t="str">
+        <f>IF('Drug Information'!O4=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f>'Drug Information'!B5</f>
+        <v>Cefazolin, Cefalexin</v>
+      </c>
+      <c r="C6" s="18" t="str">
+        <f>IF('Drug Information'!D5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D6" s="18" t="str">
+        <f>IF('Drug Information'!E5=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E6" s="18" t="str">
+        <f>IF('Drug Information'!F5=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F6" s="18" t="str">
+        <f>IF('Drug Information'!G5=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G6" s="18" t="str">
+        <f>IF('Drug Information'!H5=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H6" s="18" t="str">
+        <f>IF('Drug Information'!I5=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I6" s="18" t="str">
+        <f>IF('Drug Information'!J5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J6" s="18" t="str">
+        <f>IF('Drug Information'!K5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K6" s="18" t="str">
+        <f>IF('Drug Information'!L5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L6" s="18" t="str">
+        <f>IF('Drug Information'!M5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M6" s="18" t="str">
+        <f>IF('Drug Information'!N5=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N6" s="18" t="str">
+        <f>IF('Drug Information'!O5=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f>'Drug Information'!B6</f>
+        <v>Cephotetan, Cefoxitin</v>
+      </c>
+      <c r="C7" s="18" t="str">
+        <f>IF('Drug Information'!D6=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D7" s="18" t="str">
+        <f>IF('Drug Information'!E6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E7" s="18" t="str">
+        <f>IF('Drug Information'!F6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F7" s="18" t="str">
+        <f>IF('Drug Information'!G6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G7" s="18" t="str">
+        <f>IF('Drug Information'!H6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H7" s="18" t="str">
+        <f>IF('Drug Information'!I6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I7" s="18" t="str">
+        <f>IF('Drug Information'!J6=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J7" s="18" t="str">
+        <f>IF('Drug Information'!K6=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K7" s="18" t="str">
+        <f>IF('Drug Information'!L6=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L7" s="18" t="str">
+        <f>IF('Drug Information'!M6=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M7" s="18" t="str">
+        <f>IF('Drug Information'!N6=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>IF('Drug Information'!O6=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="str">
+        <f>'Drug Information'!B7</f>
+        <v>Ceftriaxone</v>
+      </c>
+      <c r="C8" s="18" t="str">
+        <f>IF('Drug Information'!D7=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D8" s="18" t="str">
+        <f>IF('Drug Information'!E7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E8" s="18" t="str">
+        <f>IF('Drug Information'!F7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F8" s="18" t="str">
+        <f>IF('Drug Information'!G7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G8" s="18" t="str">
+        <f>IF('Drug Information'!H7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H8" s="18" t="str">
+        <f>IF('Drug Information'!I7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I8" s="18" t="str">
+        <f>IF('Drug Information'!J7=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J8" s="18" t="str">
+        <f>IF('Drug Information'!K7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K8" s="18" t="str">
+        <f>IF('Drug Information'!L7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L8" s="18" t="str">
+        <f>IF('Drug Information'!M7=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M8" s="18" t="str">
+        <f>IF('Drug Information'!N7=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N8" s="18" t="str">
+        <f>IF('Drug Information'!O7=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5" t="str">
+        <f>'Drug Information'!B8</f>
+        <v>Ceftazidime</v>
+      </c>
+      <c r="C9" s="18" t="str">
+        <f>IF('Drug Information'!D8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D9" s="18" t="str">
+        <f>IF('Drug Information'!E8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E9" s="18" t="str">
+        <f>IF('Drug Information'!F8=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F9" s="18" t="str">
+        <f>IF('Drug Information'!G8=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G9" s="18" t="str">
+        <f>IF('Drug Information'!H8=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H9" s="18" t="str">
+        <f>IF('Drug Information'!I8=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I9" s="18" t="str">
+        <f>IF('Drug Information'!J8=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J9" s="18" t="str">
+        <f>IF('Drug Information'!K8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K9" s="18" t="str">
+        <f>IF('Drug Information'!L8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L9" s="18" t="str">
+        <f>IF('Drug Information'!M8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M9" s="18" t="str">
+        <f>IF('Drug Information'!N8=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N9" s="18" t="str">
+        <f>IF('Drug Information'!O8=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="str">
+        <f>'Drug Information'!B9</f>
+        <v>Cefepime</v>
+      </c>
+      <c r="C10" s="18" t="str">
+        <f>IF('Drug Information'!D9=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D10" s="18" t="str">
+        <f>IF('Drug Information'!E9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E10" s="18" t="str">
+        <f>IF('Drug Information'!F9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F10" s="18" t="str">
+        <f>IF('Drug Information'!G9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G10" s="18" t="str">
+        <f>IF('Drug Information'!H9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H10" s="18" t="str">
+        <f>IF('Drug Information'!I9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I10" s="18" t="str">
+        <f>IF('Drug Information'!J9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J10" s="18" t="str">
+        <f>IF('Drug Information'!K9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K10" s="18" t="str">
+        <f>IF('Drug Information'!L9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L10" s="18" t="str">
+        <f>IF('Drug Information'!M9=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M10" s="18" t="str">
+        <f>IF('Drug Information'!N9=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N10" s="18" t="str">
+        <f>IF('Drug Information'!O9=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <f>'Drug Information'!B10</f>
+        <v>Amoxicillin-Clavulanic Acid</v>
+      </c>
+      <c r="C11" s="18" t="str">
+        <f>IF('Drug Information'!D10=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D11" s="18" t="str">
+        <f>IF('Drug Information'!E10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E11" s="18" t="str">
+        <f>IF('Drug Information'!F10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F11" s="18" t="str">
+        <f>IF('Drug Information'!G10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G11" s="18" t="str">
+        <f>IF('Drug Information'!H10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H11" s="18" t="str">
+        <f>IF('Drug Information'!I10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I11" s="18" t="str">
+        <f>IF('Drug Information'!J10=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J11" s="18" t="str">
+        <f>IF('Drug Information'!K10=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K11" s="18" t="str">
+        <f>IF('Drug Information'!L10=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L11" s="18" t="str">
+        <f>IF('Drug Information'!M10=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M11" s="18" t="str">
+        <f>IF('Drug Information'!N10=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N11" s="18" t="str">
+        <f>IF('Drug Information'!O10=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="5" t="str">
+        <f>'Drug Information'!B11</f>
+        <v>Ampicillin/Sulbactam</v>
+      </c>
+      <c r="C12" s="18" t="str">
+        <f>IF('Drug Information'!D11=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D12" s="18" t="str">
+        <f>IF('Drug Information'!E11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E12" s="18" t="str">
+        <f>IF('Drug Information'!F11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F12" s="18" t="str">
+        <f>IF('Drug Information'!G11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>IF('Drug Information'!H11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H12" s="18" t="str">
+        <f>IF('Drug Information'!I11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I12" s="18" t="str">
+        <f>IF('Drug Information'!J11=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J12" s="18" t="str">
+        <f>IF('Drug Information'!K11=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K12" s="18" t="str">
+        <f>IF('Drug Information'!L11=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L12" s="18" t="str">
+        <f>IF('Drug Information'!M11=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M12" s="18" t="str">
+        <f>IF('Drug Information'!N11=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N12" s="18" t="str">
+        <f>IF('Drug Information'!O11=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="5" t="str">
+        <f>'Drug Information'!B12</f>
+        <v>Piperacillin-Tazobactam</v>
+      </c>
+      <c r="C13" s="18" t="str">
+        <f>IF('Drug Information'!D12=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D13" s="18" t="str">
+        <f>IF('Drug Information'!E12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E13" s="18" t="str">
+        <f>IF('Drug Information'!F12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F13" s="18" t="str">
+        <f>IF('Drug Information'!G12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G13" s="18" t="str">
+        <f>IF('Drug Information'!H12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H13" s="18" t="str">
+        <f>IF('Drug Information'!I12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I13" s="18" t="str">
+        <f>IF('Drug Information'!J12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J13" s="18" t="str">
+        <f>IF('Drug Information'!K12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K13" s="18" t="str">
+        <f>IF('Drug Information'!L12=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L13" s="18" t="str">
+        <f>IF('Drug Information'!M12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M13" s="18" t="str">
+        <f>IF('Drug Information'!N12=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N13" s="18" t="str">
+        <f>IF('Drug Information'!O12=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="5" t="str">
+        <f>'Drug Information'!B13</f>
+        <v>Ertapenem</v>
+      </c>
+      <c r="C14" s="18" t="str">
+        <f>IF('Drug Information'!D13=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D14" s="18" t="str">
+        <f>IF('Drug Information'!E13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E14" s="18" t="str">
+        <f>IF('Drug Information'!F13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F14" s="18" t="str">
+        <f>IF('Drug Information'!G13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G14" s="18" t="str">
+        <f>IF('Drug Information'!H13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H14" s="18" t="str">
+        <f>IF('Drug Information'!I13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I14" s="18" t="str">
+        <f>IF('Drug Information'!J13=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J14" s="18" t="str">
+        <f>IF('Drug Information'!K13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K14" s="18" t="str">
+        <f>IF('Drug Information'!L13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L14" s="18" t="str">
+        <f>IF('Drug Information'!M13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M14" s="18" t="str">
+        <f>IF('Drug Information'!N13=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N14" s="18" t="str">
+        <f>IF('Drug Information'!O13=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="5" t="str">
+        <f>'Drug Information'!B14</f>
+        <v>Imipenem, Meropenem</v>
+      </c>
+      <c r="C15" s="18" t="str">
+        <f>IF('Drug Information'!D14=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D15" s="18" t="str">
+        <f>IF('Drug Information'!E14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E15" s="18" t="str">
+        <f>IF('Drug Information'!F14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F15" s="18" t="str">
+        <f>IF('Drug Information'!G14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G15" s="18" t="str">
+        <f>IF('Drug Information'!H14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H15" s="18" t="str">
+        <f>IF('Drug Information'!I14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I15" s="18" t="str">
+        <f>IF('Drug Information'!J14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J15" s="18" t="str">
+        <f>IF('Drug Information'!K14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K15" s="18" t="str">
+        <f>IF('Drug Information'!L14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L15" s="18" t="str">
+        <f>IF('Drug Information'!M14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M15" s="18" t="str">
+        <f>IF('Drug Information'!N14=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N15" s="18" t="str">
+        <f>IF('Drug Information'!O14=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f>'Drug Information'!B15</f>
+        <v>Aztreonam</v>
+      </c>
+      <c r="C16" s="18" t="str">
+        <f>IF('Drug Information'!D15=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D16" s="18" t="str">
+        <f>IF('Drug Information'!E15=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E16" s="18" t="str">
+        <f>IF('Drug Information'!F15=1,".","")</f>
+        <v/>
+      </c>
+      <c r="F16" s="18" t="str">
+        <f>IF('Drug Information'!G15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G16" s="18" t="str">
+        <f>IF('Drug Information'!H15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H16" s="18" t="str">
+        <f>IF('Drug Information'!I15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I16" s="18" t="str">
+        <f>IF('Drug Information'!J15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J16" s="18" t="str">
+        <f>IF('Drug Information'!K15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K16" s="18" t="str">
+        <f>IF('Drug Information'!L15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L16" s="18" t="str">
+        <f>IF('Drug Information'!M15=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M16" s="18" t="str">
+        <f>IF('Drug Information'!N15=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N16" s="18" t="str">
+        <f>IF('Drug Information'!O15=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f>'Drug Information'!B16</f>
+        <v>Ciprofloxacin</v>
+      </c>
+      <c r="C17" s="18" t="str">
+        <f>IF('Drug Information'!D16=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D17" s="18" t="str">
+        <f>IF('Drug Information'!E16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E17" s="18" t="str">
+        <f>IF('Drug Information'!F16=1,".","")</f>
+        <v/>
+      </c>
+      <c r="F17" s="18" t="str">
+        <f>IF('Drug Information'!G16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G17" s="18" t="str">
+        <f>IF('Drug Information'!H16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H17" s="18" t="str">
+        <f>IF('Drug Information'!I16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I17" s="18" t="str">
+        <f>IF('Drug Information'!J16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J17" s="18" t="str">
+        <f>IF('Drug Information'!K16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K17" s="18" t="str">
+        <f>IF('Drug Information'!L16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L17" s="18" t="str">
+        <f>IF('Drug Information'!M16=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M17" s="18" t="str">
+        <f>IF('Drug Information'!N16=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N17" s="18" t="str">
+        <f>IF('Drug Information'!O16=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5" t="str">
+        <f>'Drug Information'!B17</f>
+        <v>Levofloxacin</v>
+      </c>
+      <c r="C18" s="18" t="str">
+        <f>IF('Drug Information'!D17=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D18" s="18" t="str">
+        <f>IF('Drug Information'!E17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E18" s="18" t="str">
+        <f>IF('Drug Information'!F17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F18" s="18" t="str">
+        <f>IF('Drug Information'!G17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G18" s="18" t="str">
+        <f>IF('Drug Information'!H17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H18" s="18" t="str">
+        <f>IF('Drug Information'!I17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I18" s="18" t="str">
+        <f>IF('Drug Information'!J17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J18" s="18" t="str">
+        <f>IF('Drug Information'!K17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K18" s="18" t="str">
+        <f>IF('Drug Information'!L17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L18" s="18" t="str">
+        <f>IF('Drug Information'!M17=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M18" s="18" t="str">
+        <f>IF('Drug Information'!N17=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N18" s="18" t="str">
+        <f>IF('Drug Information'!O17=1,".","")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="5" t="str">
+        <f>'Drug Information'!B18</f>
+        <v>Moxifloxacin</v>
+      </c>
+      <c r="C19" s="18" t="str">
+        <f>IF('Drug Information'!D18=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D19" s="18" t="str">
+        <f>IF('Drug Information'!E18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E19" s="18" t="str">
+        <f>IF('Drug Information'!F18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F19" s="18" t="str">
+        <f>IF('Drug Information'!G18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G19" s="18" t="str">
+        <f>IF('Drug Information'!H18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H19" s="18" t="str">
+        <f>IF('Drug Information'!I18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I19" s="18" t="str">
+        <f>IF('Drug Information'!J18=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J19" s="18" t="str">
+        <f>IF('Drug Information'!K18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K19" s="18" t="str">
+        <f>IF('Drug Information'!L18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="L19" s="18" t="str">
+        <f>IF('Drug Information'!M18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M19" s="18" t="str">
+        <f>IF('Drug Information'!N18=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N19" s="18" t="str">
+        <f>IF('Drug Information'!O18=1,".","")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f>'Drug Information'!B19</f>
+        <v>Gentamicin, Tobramycin, Amikacin</v>
+      </c>
+      <c r="C20" s="18" t="str">
+        <f>IF('Drug Information'!D19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D20" s="18" t="str">
+        <f>IF('Drug Information'!E19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E20" s="18" t="str">
+        <f>IF('Drug Information'!F19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="F20" s="18" t="str">
+        <f>IF('Drug Information'!G19=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G20" s="18" t="str">
+        <f>IF('Drug Information'!H19=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H20" s="18" t="str">
+        <f>IF('Drug Information'!I19=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I20" s="18" t="str">
+        <f>IF('Drug Information'!J19=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="J20" s="18" t="str">
+        <f>IF('Drug Information'!K19=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K20" s="18" t="str">
+        <f>IF('Drug Information'!L19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L20" s="18" t="str">
+        <f>IF('Drug Information'!M19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M20" s="18" t="str">
+        <f>IF('Drug Information'!N19=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N20" s="18" t="str">
+        <f>IF('Drug Information'!O19=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f>'Drug Information'!B20</f>
+        <v>Clindamycin</v>
+      </c>
+      <c r="C21" s="18" t="str">
+        <f>IF('Drug Information'!D20=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="D21" s="18" t="str">
+        <f>IF('Drug Information'!E20=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E21" s="18" t="str">
+        <f>IF('Drug Information'!F20=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F21" s="18" t="str">
+        <f>IF('Drug Information'!G20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G21" s="18" t="str">
+        <f>IF('Drug Information'!H20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H21" s="18" t="str">
+        <f>IF('Drug Information'!I20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I21" s="18" t="str">
+        <f>IF('Drug Information'!J20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J21" s="18" t="str">
+        <f>IF('Drug Information'!K20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K21" s="18" t="str">
+        <f>IF('Drug Information'!L20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L21" s="18" t="str">
+        <f>IF('Drug Information'!M20=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M21" s="18" t="str">
+        <f>IF('Drug Information'!N20=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N21" s="18" t="str">
+        <f>IF('Drug Information'!O20=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f>'Drug Information'!B21</f>
+        <v>Azithromycin</v>
+      </c>
+      <c r="C22" s="18" t="str">
+        <f>IF('Drug Information'!D21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D22" s="18" t="str">
+        <f>IF('Drug Information'!E21=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E22" s="18" t="str">
+        <f>IF('Drug Information'!F21=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F22" s="18" t="str">
+        <f>IF('Drug Information'!G21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G22" s="18" t="str">
+        <f>IF('Drug Information'!H21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H22" s="18" t="str">
+        <f>IF('Drug Information'!I21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I22" s="18" t="str">
+        <f>IF('Drug Information'!J21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J22" s="18" t="str">
+        <f>IF('Drug Information'!K21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K22" s="18" t="str">
+        <f>IF('Drug Information'!L21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L22" s="18" t="str">
+        <f>IF('Drug Information'!M21=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M22" s="18" t="str">
+        <f>IF('Drug Information'!N21=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N22" s="18" t="str">
+        <f>IF('Drug Information'!O21=1,".","")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f>'Drug Information'!B22</f>
+        <v>Doxycycline</v>
+      </c>
+      <c r="C23" s="18" t="str">
+        <f>IF('Drug Information'!D22=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="D23" s="18" t="str">
+        <f>IF('Drug Information'!E22=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E23" s="18" t="str">
+        <f>IF('Drug Information'!F22=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F23" s="18" t="str">
+        <f>IF('Drug Information'!G22=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G23" s="18" t="str">
+        <f>IF('Drug Information'!H22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H23" s="18" t="str">
+        <f>IF('Drug Information'!I22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I23" s="18" t="str">
+        <f>IF('Drug Information'!J22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J23" s="18" t="str">
+        <f>IF('Drug Information'!K22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K23" s="18" t="str">
+        <f>IF('Drug Information'!L22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L23" s="18" t="str">
+        <f>IF('Drug Information'!M22=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M23" s="18" t="str">
+        <f>IF('Drug Information'!N22=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N23" s="18" t="str">
+        <f>IF('Drug Information'!O22=1,".","")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f>'Drug Information'!B23</f>
+        <v>Vancomycin</v>
+      </c>
+      <c r="C24" s="18" t="str">
+        <f>IF('Drug Information'!D23=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="D24" s="18" t="str">
+        <f>IF('Drug Information'!E23=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E24" s="18" t="str">
+        <f>IF('Drug Information'!F23=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F24" s="18" t="str">
+        <f>IF('Drug Information'!G23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G24" s="18" t="str">
+        <f>IF('Drug Information'!H23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H24" s="18" t="str">
+        <f>IF('Drug Information'!I23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I24" s="18" t="str">
+        <f>IF('Drug Information'!J23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J24" s="18" t="str">
+        <f>IF('Drug Information'!K23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K24" s="18" t="str">
+        <f>IF('Drug Information'!L23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L24" s="18" t="str">
+        <f>IF('Drug Information'!M23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M24" s="18" t="str">
+        <f>IF('Drug Information'!N23=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N24" s="18" t="str">
+        <f>IF('Drug Information'!O23=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>'Drug Information'!B24</f>
+        <v>TMP/SMX</v>
+      </c>
+      <c r="C25" s="18" t="str">
+        <f>IF('Drug Information'!D24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="D25" s="18" t="str">
+        <f>IF('Drug Information'!E24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="E25" s="18" t="str">
+        <f>IF('Drug Information'!F24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="F25" s="18" t="str">
+        <f>IF('Drug Information'!G24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="G25" s="18" t="str">
+        <f>IF('Drug Information'!H24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="H25" s="18" t="str">
+        <f>IF('Drug Information'!I24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="I25" s="18" t="str">
+        <f>IF('Drug Information'!J24=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J25" s="18" t="str">
+        <f>IF('Drug Information'!K24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="K25" s="18" t="str">
+        <f>IF('Drug Information'!L24=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L25" s="18" t="str">
+        <f>IF('Drug Information'!M24=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="M25" s="18" t="str">
+        <f>IF('Drug Information'!N24=1,".","")</f>
+        <v/>
+      </c>
+      <c r="N25" s="18" t="str">
+        <f>IF('Drug Information'!O24=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f>'Drug Information'!B25</f>
+        <v>Metronidazole</v>
+      </c>
+      <c r="C26" s="18" t="str">
+        <f>IF('Drug Information'!D25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="D26" s="18" t="str">
+        <f>IF('Drug Information'!E25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="E26" s="18" t="str">
+        <f>IF('Drug Information'!F25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="F26" s="18" t="str">
+        <f>IF('Drug Information'!G25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="G26" s="18" t="str">
+        <f>IF('Drug Information'!H25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="H26" s="18" t="str">
+        <f>IF('Drug Information'!I25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="I26" s="18" t="str">
+        <f>IF('Drug Information'!J25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="J26" s="18" t="str">
+        <f>IF('Drug Information'!K25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="K26" s="18" t="str">
+        <f>IF('Drug Information'!L25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="L26" s="18" t="str">
+        <f>IF('Drug Information'!M25=1,".","")</f>
+        <v/>
+      </c>
+      <c r="M26" s="18" t="str">
+        <f>IF('Drug Information'!N25=1,".","")</f>
+        <v>.</v>
+      </c>
+      <c r="N26" s="18" t="str">
+        <f>IF('Drug Information'!O25=1,".","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A27:N27"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:M2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:N26">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add conditional formatting to test table
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F054E16-CE1E-455A-A5E0-C2C4CE8BBEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A557AA2-F0E6-46F3-8625-66561D320B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Example Brand</t>
-  </si>
-  <si>
-    <t>Example Drug</t>
   </si>
   <si>
     <t>Augmentin</t>
@@ -453,7 +450,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -601,13 +598,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -881,6 +893,179 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -888,24 +1073,60 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="0.39994506668294322"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1258,26 +1479,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:O25" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:O25" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:O25" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
   <tableColumns count="15">
-    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{42E0601C-2822-4BA1-84B0-34013D392289}" name="Drug Class" dataDxfId="21">
       <calculatedColumnFormula>IF(Antibiogram!A3=0,A1,Antibiogram!A3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Example Drug" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Example Brand" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1554,7 +1775,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G33" sqref="G33"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1825,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="81" t="s">
         <v>1</v>
@@ -2226,7 +2447,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2251,10 +2472,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="91" t="s">
-        <v>53</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>52</v>
@@ -2326,7 +2547,7 @@
         <v>Anti-staphylococcal penicillins</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="91"/>
       <c r="D3" s="91"/>
@@ -2352,7 +2573,7 @@
         <v>Aminopenicillins</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="91"/>
       <c r="D4" s="91"/>
@@ -2558,10 +2779,10 @@
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B10" s="91" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="91"/>
       <c r="E10" s="91">
@@ -2594,10 +2815,10 @@
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B11" s="91" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="91" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="91"/>
       <c r="E11" s="91">
@@ -2630,10 +2851,10 @@
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B12" s="91" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="91"/>
       <c r="E12" s="91">
@@ -2912,7 +3133,7 @@
         <v>Aminoglycosides</v>
       </c>
       <c r="B19" s="91" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="91"/>
       <c r="D19" s="91"/>
@@ -2944,7 +3165,7 @@
         <v>Lincosamide</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="91"/>
       <c r="D20" s="91">
@@ -3069,7 +3290,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="91">
         <v>1</v>
@@ -3138,17 +3359,17 @@
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I42" sqref="I42"/>
+      <selection pane="topRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="127" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" style="2" bestFit="1" customWidth="1"/>
@@ -3169,1446 +3390,1590 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="12" t="s">
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="10" t="s">
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="7" t="s">
+      <c r="L1" s="99"/>
+      <c r="M1" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="101" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="102" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="82" t="s">
+      <c r="C2" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="I2" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="86" t="s">
+      <c r="J2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="87" t="s">
+      <c r="K2" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="88" t="s">
+      <c r="L2" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="89" t="s">
+      <c r="M2" s="100"/>
+      <c r="N2" s="106" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="str">
+      <c r="B3" s="125" t="str">
         <f>'Drug Information'!B2</f>
         <v>Benzylpenicillin</v>
       </c>
-      <c r="C3" s="18" t="str">
-        <f>IF('Drug Information'!D2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D3" s="18" t="str">
-        <f>IF('Drug Information'!E2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E3" s="18" t="str">
-        <f>IF('Drug Information'!F2=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F3" s="18" t="str">
-        <f>IF('Drug Information'!G2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G3" s="18" t="str">
-        <f>IF('Drug Information'!H2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H3" s="18" t="str">
-        <f>IF('Drug Information'!I2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I3" s="18" t="str">
-        <f>IF('Drug Information'!J2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J3" s="18" t="str">
-        <f>IF('Drug Information'!K2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K3" s="18" t="str">
-        <f>IF('Drug Information'!L2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L3" s="18" t="str">
-        <f>IF('Drug Information'!M2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M3" s="18" t="str">
-        <f>IF('Drug Information'!N2=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N3" s="18" t="str">
-        <f>IF('Drug Information'!O2=1,".","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="107" t="str">
+        <f>IF('Drug Information'!D2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D3" s="107" t="str">
+        <f>IF('Drug Information'!E2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E3" s="107" t="str">
+        <f>IF('Drug Information'!F2=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F3" s="107" t="str">
+        <f>IF('Drug Information'!G2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G3" s="107" t="str">
+        <f>IF('Drug Information'!H2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H3" s="107" t="str">
+        <f>IF('Drug Information'!I2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I3" s="107" t="str">
+        <f>IF('Drug Information'!J2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J3" s="107" t="str">
+        <f>IF('Drug Information'!K2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K3" s="107" t="str">
+        <f>IF('Drug Information'!L2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L3" s="107" t="str">
+        <f>IF('Drug Information'!M2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M3" s="107" t="str">
+        <f>IF('Drug Information'!N2=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N3" s="107" t="str">
+        <f>IF('Drug Information'!O2=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="125" t="str">
         <f>'Drug Information'!B3</f>
         <v>Naficillin, Oxacillin, Flucloxacillin</v>
       </c>
-      <c r="C4" s="18" t="str">
-        <f>IF('Drug Information'!D3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D4" s="18" t="str">
-        <f>IF('Drug Information'!E3=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E4" s="18" t="str">
-        <f>IF('Drug Information'!F3=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F4" s="18" t="str">
-        <f>IF('Drug Information'!G3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G4" s="18" t="str">
-        <f>IF('Drug Information'!H3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H4" s="18" t="str">
-        <f>IF('Drug Information'!I3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I4" s="18" t="str">
-        <f>IF('Drug Information'!J3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J4" s="18" t="str">
-        <f>IF('Drug Information'!K3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K4" s="18" t="str">
-        <f>IF('Drug Information'!L3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L4" s="18" t="str">
-        <f>IF('Drug Information'!M3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M4" s="18" t="str">
-        <f>IF('Drug Information'!N3=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N4" s="18" t="str">
-        <f>IF('Drug Information'!O3=1,".","")</f>
-        <v/>
+      <c r="C4" s="107" t="str">
+        <f>IF('Drug Information'!D3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D4" s="107" t="str">
+        <f>IF('Drug Information'!E3=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E4" s="107" t="str">
+        <f>IF('Drug Information'!F3=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F4" s="107" t="str">
+        <f>IF('Drug Information'!G3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G4" s="107" t="str">
+        <f>IF('Drug Information'!H3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H4" s="107" t="str">
+        <f>IF('Drug Information'!I3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I4" s="107" t="str">
+        <f>IF('Drug Information'!J3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J4" s="107" t="str">
+        <f>IF('Drug Information'!K3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K4" s="107" t="str">
+        <f>IF('Drug Information'!L3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L4" s="107" t="str">
+        <f>IF('Drug Information'!M3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M4" s="107" t="str">
+        <f>IF('Drug Information'!N3=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N4" s="107" t="str">
+        <f>IF('Drug Information'!O3=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="5" t="str">
+      <c r="B5" s="125" t="str">
         <f>'Drug Information'!B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
-      <c r="C5" s="18" t="str">
-        <f>IF('Drug Information'!D4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D5" s="18" t="str">
-        <f>IF('Drug Information'!E4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E5" s="18" t="str">
-        <f>IF('Drug Information'!F4=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F5" s="18" t="str">
-        <f>IF('Drug Information'!G4=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G5" s="18" t="str">
-        <f>IF('Drug Information'!H4=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H5" s="18" t="str">
-        <f>IF('Drug Information'!I4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I5" s="18" t="str">
-        <f>IF('Drug Information'!J4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J5" s="18" t="str">
-        <f>IF('Drug Information'!K4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K5" s="18" t="str">
-        <f>IF('Drug Information'!L4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L5" s="18" t="str">
-        <f>IF('Drug Information'!M4=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M5" s="18" t="str">
-        <f>IF('Drug Information'!N4=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N5" s="18" t="str">
-        <f>IF('Drug Information'!O4=1,".","")</f>
-        <v/>
+      <c r="C5" s="107" t="str">
+        <f>IF('Drug Information'!D4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D5" s="107" t="str">
+        <f>IF('Drug Information'!E4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E5" s="107" t="str">
+        <f>IF('Drug Information'!F4=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F5" s="107" t="str">
+        <f>IF('Drug Information'!G4=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G5" s="107" t="str">
+        <f>IF('Drug Information'!H4=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H5" s="107" t="str">
+        <f>IF('Drug Information'!I4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I5" s="107" t="str">
+        <f>IF('Drug Information'!J4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J5" s="107" t="str">
+        <f>IF('Drug Information'!K4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K5" s="107" t="str">
+        <f>IF('Drug Information'!L4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L5" s="107" t="str">
+        <f>IF('Drug Information'!M4=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M5" s="107" t="str">
+        <f>IF('Drug Information'!N4=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N5" s="107" t="str">
+        <f>IF('Drug Information'!O4=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="129" t="str">
         <f>'Drug Information'!B5</f>
         <v>Cefazolin, Cefalexin</v>
       </c>
-      <c r="C6" s="18" t="str">
-        <f>IF('Drug Information'!D5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D6" s="18" t="str">
-        <f>IF('Drug Information'!E5=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E6" s="18" t="str">
-        <f>IF('Drug Information'!F5=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F6" s="18" t="str">
-        <f>IF('Drug Information'!G5=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G6" s="18" t="str">
-        <f>IF('Drug Information'!H5=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H6" s="18" t="str">
-        <f>IF('Drug Information'!I5=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I6" s="18" t="str">
-        <f>IF('Drug Information'!J5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J6" s="18" t="str">
-        <f>IF('Drug Information'!K5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K6" s="18" t="str">
-        <f>IF('Drug Information'!L5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L6" s="18" t="str">
-        <f>IF('Drug Information'!M5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M6" s="18" t="str">
-        <f>IF('Drug Information'!N5=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N6" s="18" t="str">
-        <f>IF('Drug Information'!O5=1,".","")</f>
-        <v/>
+      <c r="C6" s="108" t="str">
+        <f>IF('Drug Information'!D5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D6" s="108" t="str">
+        <f>IF('Drug Information'!E5=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E6" s="108" t="str">
+        <f>IF('Drug Information'!F5=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F6" s="108" t="str">
+        <f>IF('Drug Information'!G5=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G6" s="108" t="str">
+        <f>IF('Drug Information'!H5=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H6" s="108" t="str">
+        <f>IF('Drug Information'!I5=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I6" s="108" t="str">
+        <f>IF('Drug Information'!J5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J6" s="108" t="str">
+        <f>IF('Drug Information'!K5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K6" s="108" t="str">
+        <f>IF('Drug Information'!L5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L6" s="108" t="str">
+        <f>IF('Drug Information'!M5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M6" s="108" t="str">
+        <f>IF('Drug Information'!N5=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N6" s="108" t="str">
+        <f>IF('Drug Information'!O5=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="129" t="str">
         <f>'Drug Information'!B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="C7" s="18" t="str">
-        <f>IF('Drug Information'!D6=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D7" s="18" t="str">
-        <f>IF('Drug Information'!E6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E7" s="18" t="str">
-        <f>IF('Drug Information'!F6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F7" s="18" t="str">
-        <f>IF('Drug Information'!G6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G7" s="18" t="str">
-        <f>IF('Drug Information'!H6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H7" s="18" t="str">
-        <f>IF('Drug Information'!I6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I7" s="18" t="str">
-        <f>IF('Drug Information'!J6=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J7" s="18" t="str">
-        <f>IF('Drug Information'!K6=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K7" s="18" t="str">
-        <f>IF('Drug Information'!L6=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L7" s="18" t="str">
-        <f>IF('Drug Information'!M6=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M7" s="18" t="str">
-        <f>IF('Drug Information'!N6=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N7" s="18" t="str">
-        <f>IF('Drug Information'!O6=1,".","")</f>
-        <v/>
+      <c r="C7" s="108" t="str">
+        <f>IF('Drug Information'!D6=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D7" s="108" t="str">
+        <f>IF('Drug Information'!E6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E7" s="108" t="str">
+        <f>IF('Drug Information'!F6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F7" s="108" t="str">
+        <f>IF('Drug Information'!G6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G7" s="108" t="str">
+        <f>IF('Drug Information'!H6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H7" s="108" t="str">
+        <f>IF('Drug Information'!I6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I7" s="108" t="str">
+        <f>IF('Drug Information'!J6=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J7" s="108" t="str">
+        <f>IF('Drug Information'!K6=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K7" s="108" t="str">
+        <f>IF('Drug Information'!L6=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L7" s="108" t="str">
+        <f>IF('Drug Information'!M6=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M7" s="108" t="str">
+        <f>IF('Drug Information'!N6=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N7" s="108" t="str">
+        <f>IF('Drug Information'!O6=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="129" t="str">
         <f>'Drug Information'!B7</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="C8" s="18" t="str">
-        <f>IF('Drug Information'!D7=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D8" s="18" t="str">
-        <f>IF('Drug Information'!E7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E8" s="18" t="str">
-        <f>IF('Drug Information'!F7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F8" s="18" t="str">
-        <f>IF('Drug Information'!G7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G8" s="18" t="str">
-        <f>IF('Drug Information'!H7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H8" s="18" t="str">
-        <f>IF('Drug Information'!I7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I8" s="18" t="str">
-        <f>IF('Drug Information'!J7=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J8" s="18" t="str">
-        <f>IF('Drug Information'!K7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K8" s="18" t="str">
-        <f>IF('Drug Information'!L7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L8" s="18" t="str">
-        <f>IF('Drug Information'!M7=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M8" s="18" t="str">
-        <f>IF('Drug Information'!N7=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N8" s="18" t="str">
-        <f>IF('Drug Information'!O7=1,".","")</f>
-        <v/>
+      <c r="C8" s="108" t="str">
+        <f>IF('Drug Information'!D7=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D8" s="108" t="str">
+        <f>IF('Drug Information'!E7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E8" s="108" t="str">
+        <f>IF('Drug Information'!F7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F8" s="108" t="str">
+        <f>IF('Drug Information'!G7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G8" s="108" t="str">
+        <f>IF('Drug Information'!H7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H8" s="108" t="str">
+        <f>IF('Drug Information'!I7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I8" s="108" t="str">
+        <f>IF('Drug Information'!J7=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J8" s="108" t="str">
+        <f>IF('Drug Information'!K7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K8" s="108" t="str">
+        <f>IF('Drug Information'!L7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L8" s="108" t="str">
+        <f>IF('Drug Information'!M7=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M8" s="108" t="str">
+        <f>IF('Drug Information'!N7=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N8" s="108" t="str">
+        <f>IF('Drug Information'!O7=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="str">
+      <c r="A9" s="130"/>
+      <c r="B9" s="129" t="str">
         <f>'Drug Information'!B8</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="C9" s="18" t="str">
-        <f>IF('Drug Information'!D8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D9" s="18" t="str">
-        <f>IF('Drug Information'!E8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E9" s="18" t="str">
-        <f>IF('Drug Information'!F8=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F9" s="18" t="str">
-        <f>IF('Drug Information'!G8=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G9" s="18" t="str">
-        <f>IF('Drug Information'!H8=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H9" s="18" t="str">
-        <f>IF('Drug Information'!I8=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I9" s="18" t="str">
-        <f>IF('Drug Information'!J8=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J9" s="18" t="str">
-        <f>IF('Drug Information'!K8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K9" s="18" t="str">
-        <f>IF('Drug Information'!L8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L9" s="18" t="str">
-        <f>IF('Drug Information'!M8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M9" s="18" t="str">
-        <f>IF('Drug Information'!N8=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N9" s="18" t="str">
-        <f>IF('Drug Information'!O8=1,".","")</f>
-        <v/>
+      <c r="C9" s="108" t="str">
+        <f>IF('Drug Information'!D8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D9" s="108" t="str">
+        <f>IF('Drug Information'!E8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E9" s="108" t="str">
+        <f>IF('Drug Information'!F8=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F9" s="108" t="str">
+        <f>IF('Drug Information'!G8=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G9" s="108" t="str">
+        <f>IF('Drug Information'!H8=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H9" s="108" t="str">
+        <f>IF('Drug Information'!I8=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I9" s="108" t="str">
+        <f>IF('Drug Information'!J8=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J9" s="108" t="str">
+        <f>IF('Drug Information'!K8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K9" s="108" t="str">
+        <f>IF('Drug Information'!L8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L9" s="108" t="str">
+        <f>IF('Drug Information'!M8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M9" s="108" t="str">
+        <f>IF('Drug Information'!N8=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N9" s="108" t="str">
+        <f>IF('Drug Information'!O8=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="128" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="129" t="str">
         <f>'Drug Information'!B9</f>
         <v>Cefepime</v>
       </c>
-      <c r="C10" s="18" t="str">
-        <f>IF('Drug Information'!D9=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D10" s="18" t="str">
-        <f>IF('Drug Information'!E9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E10" s="18" t="str">
-        <f>IF('Drug Information'!F9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F10" s="18" t="str">
-        <f>IF('Drug Information'!G9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G10" s="18" t="str">
-        <f>IF('Drug Information'!H9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H10" s="18" t="str">
-        <f>IF('Drug Information'!I9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I10" s="18" t="str">
-        <f>IF('Drug Information'!J9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J10" s="18" t="str">
-        <f>IF('Drug Information'!K9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K10" s="18" t="str">
-        <f>IF('Drug Information'!L9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L10" s="18" t="str">
-        <f>IF('Drug Information'!M9=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M10" s="18" t="str">
-        <f>IF('Drug Information'!N9=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N10" s="18" t="str">
-        <f>IF('Drug Information'!O9=1,".","")</f>
-        <v/>
+      <c r="C10" s="108" t="str">
+        <f>IF('Drug Information'!D9=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D10" s="108" t="str">
+        <f>IF('Drug Information'!E9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E10" s="108" t="str">
+        <f>IF('Drug Information'!F9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F10" s="108" t="str">
+        <f>IF('Drug Information'!G9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G10" s="108" t="str">
+        <f>IF('Drug Information'!H9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H10" s="108" t="str">
+        <f>IF('Drug Information'!I9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I10" s="108" t="str">
+        <f>IF('Drug Information'!J9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J10" s="108" t="str">
+        <f>IF('Drug Information'!K9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K10" s="108" t="str">
+        <f>IF('Drug Information'!L9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L10" s="108" t="str">
+        <f>IF('Drug Information'!M9=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M10" s="108" t="str">
+        <f>IF('Drug Information'!N9=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N10" s="108" t="str">
+        <f>IF('Drug Information'!O9=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="132" t="str">
         <f>'Drug Information'!B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="C11" s="18" t="str">
-        <f>IF('Drug Information'!D10=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D11" s="18" t="str">
-        <f>IF('Drug Information'!E10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E11" s="18" t="str">
-        <f>IF('Drug Information'!F10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F11" s="18" t="str">
-        <f>IF('Drug Information'!G10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G11" s="18" t="str">
-        <f>IF('Drug Information'!H10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H11" s="18" t="str">
-        <f>IF('Drug Information'!I10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I11" s="18" t="str">
-        <f>IF('Drug Information'!J10=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J11" s="18" t="str">
-        <f>IF('Drug Information'!K10=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K11" s="18" t="str">
-        <f>IF('Drug Information'!L10=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L11" s="18" t="str">
-        <f>IF('Drug Information'!M10=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M11" s="18" t="str">
-        <f>IF('Drug Information'!N10=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N11" s="18" t="str">
-        <f>IF('Drug Information'!O10=1,".","")</f>
-        <v/>
+      <c r="C11" s="109" t="str">
+        <f>IF('Drug Information'!D10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D11" s="109" t="str">
+        <f>IF('Drug Information'!E10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E11" s="109" t="str">
+        <f>IF('Drug Information'!F10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F11" s="109" t="str">
+        <f>IF('Drug Information'!G10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G11" s="109" t="str">
+        <f>IF('Drug Information'!H10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H11" s="109" t="str">
+        <f>IF('Drug Information'!I10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I11" s="109" t="str">
+        <f>IF('Drug Information'!J10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J11" s="109" t="str">
+        <f>IF('Drug Information'!K10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K11" s="109" t="str">
+        <f>IF('Drug Information'!L10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L11" s="109" t="str">
+        <f>IF('Drug Information'!M10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M11" s="109" t="str">
+        <f>IF('Drug Information'!N10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N11" s="109" t="str">
+        <f>IF('Drug Information'!O10=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="str">
+      <c r="A12" s="131"/>
+      <c r="B12" s="132" t="str">
         <f>'Drug Information'!B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="C12" s="18" t="str">
-        <f>IF('Drug Information'!D11=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D12" s="18" t="str">
-        <f>IF('Drug Information'!E11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E12" s="18" t="str">
-        <f>IF('Drug Information'!F11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F12" s="18" t="str">
-        <f>IF('Drug Information'!G11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G12" s="18" t="str">
-        <f>IF('Drug Information'!H11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H12" s="18" t="str">
-        <f>IF('Drug Information'!I11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I12" s="18" t="str">
-        <f>IF('Drug Information'!J11=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J12" s="18" t="str">
-        <f>IF('Drug Information'!K11=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K12" s="18" t="str">
-        <f>IF('Drug Information'!L11=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L12" s="18" t="str">
-        <f>IF('Drug Information'!M11=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M12" s="18" t="str">
-        <f>IF('Drug Information'!N11=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N12" s="18" t="str">
-        <f>IF('Drug Information'!O11=1,".","")</f>
-        <v/>
+      <c r="C12" s="109" t="str">
+        <f>IF('Drug Information'!D11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D12" s="109" t="str">
+        <f>IF('Drug Information'!E11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E12" s="109" t="str">
+        <f>IF('Drug Information'!F11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F12" s="109" t="str">
+        <f>IF('Drug Information'!G11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G12" s="109" t="str">
+        <f>IF('Drug Information'!H11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H12" s="109" t="str">
+        <f>IF('Drug Information'!I11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I12" s="109" t="str">
+        <f>IF('Drug Information'!J11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J12" s="109" t="str">
+        <f>IF('Drug Information'!K11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K12" s="109" t="str">
+        <f>IF('Drug Information'!L11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L12" s="109" t="str">
+        <f>IF('Drug Information'!M11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M12" s="109" t="str">
+        <f>IF('Drug Information'!N11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N12" s="109" t="str">
+        <f>IF('Drug Information'!O11=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5" t="str">
+      <c r="A13" s="131"/>
+      <c r="B13" s="132" t="str">
         <f>'Drug Information'!B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="C13" s="18" t="str">
-        <f>IF('Drug Information'!D12=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D13" s="18" t="str">
-        <f>IF('Drug Information'!E12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E13" s="18" t="str">
-        <f>IF('Drug Information'!F12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F13" s="18" t="str">
-        <f>IF('Drug Information'!G12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G13" s="18" t="str">
-        <f>IF('Drug Information'!H12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H13" s="18" t="str">
-        <f>IF('Drug Information'!I12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I13" s="18" t="str">
-        <f>IF('Drug Information'!J12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J13" s="18" t="str">
-        <f>IF('Drug Information'!K12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K13" s="18" t="str">
-        <f>IF('Drug Information'!L12=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L13" s="18" t="str">
-        <f>IF('Drug Information'!M12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M13" s="18" t="str">
-        <f>IF('Drug Information'!N12=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N13" s="18" t="str">
-        <f>IF('Drug Information'!O12=1,".","")</f>
-        <v/>
+      <c r="C13" s="109" t="str">
+        <f>IF('Drug Information'!D12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D13" s="109" t="str">
+        <f>IF('Drug Information'!E12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E13" s="109" t="str">
+        <f>IF('Drug Information'!F12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F13" s="109" t="str">
+        <f>IF('Drug Information'!G12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G13" s="109" t="str">
+        <f>IF('Drug Information'!H12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H13" s="109" t="str">
+        <f>IF('Drug Information'!I12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I13" s="109" t="str">
+        <f>IF('Drug Information'!J12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J13" s="109" t="str">
+        <f>IF('Drug Information'!K12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K13" s="109" t="str">
+        <f>IF('Drug Information'!L12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L13" s="109" t="str">
+        <f>IF('Drug Information'!M12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M13" s="109" t="str">
+        <f>IF('Drug Information'!N12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N13" s="109" t="str">
+        <f>IF('Drug Information'!O12=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="133" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B14" s="134" t="str">
         <f>'Drug Information'!B13</f>
         <v>Ertapenem</v>
       </c>
-      <c r="C14" s="18" t="str">
-        <f>IF('Drug Information'!D13=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D14" s="18" t="str">
-        <f>IF('Drug Information'!E13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E14" s="18" t="str">
-        <f>IF('Drug Information'!F13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F14" s="18" t="str">
-        <f>IF('Drug Information'!G13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G14" s="18" t="str">
-        <f>IF('Drug Information'!H13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H14" s="18" t="str">
-        <f>IF('Drug Information'!I13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I14" s="18" t="str">
-        <f>IF('Drug Information'!J13=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J14" s="18" t="str">
-        <f>IF('Drug Information'!K13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K14" s="18" t="str">
-        <f>IF('Drug Information'!L13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L14" s="18" t="str">
-        <f>IF('Drug Information'!M13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M14" s="18" t="str">
-        <f>IF('Drug Information'!N13=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N14" s="18" t="str">
-        <f>IF('Drug Information'!O13=1,".","")</f>
-        <v/>
+      <c r="C14" s="110" t="str">
+        <f>IF('Drug Information'!D13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D14" s="110" t="str">
+        <f>IF('Drug Information'!E13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E14" s="110" t="str">
+        <f>IF('Drug Information'!F13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F14" s="110" t="str">
+        <f>IF('Drug Information'!G13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G14" s="110" t="str">
+        <f>IF('Drug Information'!H13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H14" s="110" t="str">
+        <f>IF('Drug Information'!I13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I14" s="110" t="str">
+        <f>IF('Drug Information'!J13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J14" s="110" t="str">
+        <f>IF('Drug Information'!K13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K14" s="110" t="str">
+        <f>IF('Drug Information'!L13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L14" s="110" t="str">
+        <f>IF('Drug Information'!M13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M14" s="110" t="str">
+        <f>IF('Drug Information'!N13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N14" s="110" t="str">
+        <f>IF('Drug Information'!O13=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5" t="str">
+      <c r="A15" s="133"/>
+      <c r="B15" s="134" t="str">
         <f>'Drug Information'!B14</f>
         <v>Imipenem, Meropenem</v>
       </c>
-      <c r="C15" s="18" t="str">
-        <f>IF('Drug Information'!D14=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D15" s="18" t="str">
-        <f>IF('Drug Information'!E14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E15" s="18" t="str">
-        <f>IF('Drug Information'!F14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F15" s="18" t="str">
-        <f>IF('Drug Information'!G14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G15" s="18" t="str">
-        <f>IF('Drug Information'!H14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H15" s="18" t="str">
-        <f>IF('Drug Information'!I14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I15" s="18" t="str">
-        <f>IF('Drug Information'!J14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J15" s="18" t="str">
-        <f>IF('Drug Information'!K14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K15" s="18" t="str">
-        <f>IF('Drug Information'!L14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L15" s="18" t="str">
-        <f>IF('Drug Information'!M14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M15" s="18" t="str">
-        <f>IF('Drug Information'!N14=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N15" s="18" t="str">
-        <f>IF('Drug Information'!O14=1,".","")</f>
-        <v/>
+      <c r="C15" s="110" t="str">
+        <f>IF('Drug Information'!D14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D15" s="110" t="str">
+        <f>IF('Drug Information'!E14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E15" s="110" t="str">
+        <f>IF('Drug Information'!F14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F15" s="110" t="str">
+        <f>IF('Drug Information'!G14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G15" s="110" t="str">
+        <f>IF('Drug Information'!H14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H15" s="110" t="str">
+        <f>IF('Drug Information'!I14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I15" s="110" t="str">
+        <f>IF('Drug Information'!J14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J15" s="110" t="str">
+        <f>IF('Drug Information'!K14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K15" s="110" t="str">
+        <f>IF('Drug Information'!L14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L15" s="110" t="str">
+        <f>IF('Drug Information'!M14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M15" s="110" t="str">
+        <f>IF('Drug Information'!N14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N15" s="110" t="str">
+        <f>IF('Drug Information'!O14=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B16" s="136" t="str">
         <f>'Drug Information'!B15</f>
         <v>Aztreonam</v>
       </c>
-      <c r="C16" s="18" t="str">
-        <f>IF('Drug Information'!D15=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D16" s="18" t="str">
-        <f>IF('Drug Information'!E15=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E16" s="18" t="str">
-        <f>IF('Drug Information'!F15=1,".","")</f>
-        <v/>
-      </c>
-      <c r="F16" s="18" t="str">
-        <f>IF('Drug Information'!G15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G16" s="18" t="str">
-        <f>IF('Drug Information'!H15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H16" s="18" t="str">
-        <f>IF('Drug Information'!I15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I16" s="18" t="str">
-        <f>IF('Drug Information'!J15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J16" s="18" t="str">
-        <f>IF('Drug Information'!K15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K16" s="18" t="str">
-        <f>IF('Drug Information'!L15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L16" s="18" t="str">
-        <f>IF('Drug Information'!M15=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M16" s="18" t="str">
-        <f>IF('Drug Information'!N15=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N16" s="18" t="str">
-        <f>IF('Drug Information'!O15=1,".","")</f>
-        <v/>
+      <c r="C16" s="111" t="str">
+        <f>IF('Drug Information'!D15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D16" s="111" t="str">
+        <f>IF('Drug Information'!E15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E16" s="111" t="str">
+        <f>IF('Drug Information'!F15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="F16" s="111" t="str">
+        <f>IF('Drug Information'!G15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G16" s="111" t="str">
+        <f>IF('Drug Information'!H15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H16" s="111" t="str">
+        <f>IF('Drug Information'!I15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I16" s="111" t="str">
+        <f>IF('Drug Information'!J15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J16" s="111" t="str">
+        <f>IF('Drug Information'!K15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K16" s="111" t="str">
+        <f>IF('Drug Information'!L15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L16" s="111" t="str">
+        <f>IF('Drug Information'!M15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M16" s="111" t="str">
+        <f>IF('Drug Information'!N15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N16" s="111" t="str">
+        <f>IF('Drug Information'!O15=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="138" t="str">
         <f>'Drug Information'!B16</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="C17" s="18" t="str">
-        <f>IF('Drug Information'!D16=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D17" s="18" t="str">
-        <f>IF('Drug Information'!E16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E17" s="18" t="str">
-        <f>IF('Drug Information'!F16=1,".","")</f>
-        <v/>
-      </c>
-      <c r="F17" s="18" t="str">
-        <f>IF('Drug Information'!G16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G17" s="18" t="str">
-        <f>IF('Drug Information'!H16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H17" s="18" t="str">
-        <f>IF('Drug Information'!I16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I17" s="18" t="str">
-        <f>IF('Drug Information'!J16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J17" s="18" t="str">
-        <f>IF('Drug Information'!K16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K17" s="18" t="str">
-        <f>IF('Drug Information'!L16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L17" s="18" t="str">
-        <f>IF('Drug Information'!M16=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M17" s="18" t="str">
-        <f>IF('Drug Information'!N16=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N17" s="18" t="str">
-        <f>IF('Drug Information'!O16=1,".","")</f>
-        <v/>
+      <c r="C17" s="112" t="str">
+        <f>IF('Drug Information'!D16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D17" s="112" t="str">
+        <f>IF('Drug Information'!E16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E17" s="112" t="str">
+        <f>IF('Drug Information'!F16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="F17" s="112" t="str">
+        <f>IF('Drug Information'!G16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G17" s="112" t="str">
+        <f>IF('Drug Information'!H16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H17" s="112" t="str">
+        <f>IF('Drug Information'!I16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I17" s="112" t="str">
+        <f>IF('Drug Information'!J16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J17" s="112" t="str">
+        <f>IF('Drug Information'!K16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K17" s="112" t="str">
+        <f>IF('Drug Information'!L16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L17" s="112" t="str">
+        <f>IF('Drug Information'!M16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M17" s="112" t="str">
+        <f>IF('Drug Information'!N16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N17" s="112" t="str">
+        <f>IF('Drug Information'!O16=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5" t="str">
+      <c r="A18" s="137"/>
+      <c r="B18" s="138" t="str">
         <f>'Drug Information'!B17</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="C18" s="18" t="str">
-        <f>IF('Drug Information'!D17=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D18" s="18" t="str">
-        <f>IF('Drug Information'!E17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E18" s="18" t="str">
-        <f>IF('Drug Information'!F17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F18" s="18" t="str">
-        <f>IF('Drug Information'!G17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G18" s="18" t="str">
-        <f>IF('Drug Information'!H17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H18" s="18" t="str">
-        <f>IF('Drug Information'!I17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I18" s="18" t="str">
-        <f>IF('Drug Information'!J17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J18" s="18" t="str">
-        <f>IF('Drug Information'!K17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K18" s="18" t="str">
-        <f>IF('Drug Information'!L17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L18" s="18" t="str">
-        <f>IF('Drug Information'!M17=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M18" s="18" t="str">
-        <f>IF('Drug Information'!N17=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N18" s="18" t="str">
-        <f>IF('Drug Information'!O17=1,".","")</f>
-        <v>.</v>
+      <c r="C18" s="112" t="str">
+        <f>IF('Drug Information'!D17=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D18" s="112" t="str">
+        <f>IF('Drug Information'!E17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E18" s="112" t="str">
+        <f>IF('Drug Information'!F17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F18" s="112" t="str">
+        <f>IF('Drug Information'!G17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G18" s="112" t="str">
+        <f>IF('Drug Information'!H17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H18" s="112" t="str">
+        <f>IF('Drug Information'!I17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I18" s="112" t="str">
+        <f>IF('Drug Information'!J17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J18" s="112" t="str">
+        <f>IF('Drug Information'!K17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K18" s="112" t="str">
+        <f>IF('Drug Information'!L17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L18" s="112" t="str">
+        <f>IF('Drug Information'!M17=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M18" s="112" t="str">
+        <f>IF('Drug Information'!N17=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N18" s="112" t="str">
+        <f>IF('Drug Information'!O17=1,"",".")</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5" t="str">
+      <c r="A19" s="137"/>
+      <c r="B19" s="138" t="str">
         <f>'Drug Information'!B18</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="C19" s="18" t="str">
-        <f>IF('Drug Information'!D18=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D19" s="18" t="str">
-        <f>IF('Drug Information'!E18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E19" s="18" t="str">
-        <f>IF('Drug Information'!F18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F19" s="18" t="str">
-        <f>IF('Drug Information'!G18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G19" s="18" t="str">
-        <f>IF('Drug Information'!H18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H19" s="18" t="str">
-        <f>IF('Drug Information'!I18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I19" s="18" t="str">
-        <f>IF('Drug Information'!J18=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J19" s="18" t="str">
-        <f>IF('Drug Information'!K18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K19" s="18" t="str">
-        <f>IF('Drug Information'!L18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="L19" s="18" t="str">
-        <f>IF('Drug Information'!M18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M19" s="18" t="str">
-        <f>IF('Drug Information'!N18=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N19" s="18" t="str">
-        <f>IF('Drug Information'!O18=1,".","")</f>
-        <v>.</v>
+      <c r="C19" s="113" t="str">
+        <f>IF('Drug Information'!D18=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D19" s="113" t="str">
+        <f>IF('Drug Information'!E18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E19" s="113" t="str">
+        <f>IF('Drug Information'!F18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F19" s="113" t="str">
+        <f>IF('Drug Information'!G18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G19" s="113" t="str">
+        <f>IF('Drug Information'!H18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H19" s="113" t="str">
+        <f>IF('Drug Information'!I18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I19" s="113" t="str">
+        <f>IF('Drug Information'!J18=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J19" s="113" t="str">
+        <f>IF('Drug Information'!K18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K19" s="113" t="str">
+        <f>IF('Drug Information'!L18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L19" s="113" t="str">
+        <f>IF('Drug Information'!M18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M19" s="113" t="str">
+        <f>IF('Drug Information'!N18=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N19" s="113" t="str">
+        <f>IF('Drug Information'!O18=1,"",".")</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="139" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="5" t="str">
+      <c r="B20" s="140" t="str">
         <f>'Drug Information'!B19</f>
         <v>Gentamicin, Tobramycin, Amikacin</v>
       </c>
-      <c r="C20" s="18" t="str">
-        <f>IF('Drug Information'!D19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D20" s="18" t="str">
-        <f>IF('Drug Information'!E19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E20" s="18" t="str">
-        <f>IF('Drug Information'!F19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="F20" s="18" t="str">
-        <f>IF('Drug Information'!G19=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G20" s="18" t="str">
-        <f>IF('Drug Information'!H19=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H20" s="18" t="str">
-        <f>IF('Drug Information'!I19=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I20" s="18" t="str">
-        <f>IF('Drug Information'!J19=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="J20" s="18" t="str">
-        <f>IF('Drug Information'!K19=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K20" s="18" t="str">
-        <f>IF('Drug Information'!L19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L20" s="18" t="str">
-        <f>IF('Drug Information'!M19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M20" s="18" t="str">
-        <f>IF('Drug Information'!N19=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N20" s="18" t="str">
-        <f>IF('Drug Information'!O19=1,".","")</f>
-        <v/>
+      <c r="C20" s="114" t="str">
+        <f>IF('Drug Information'!D19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D20" s="114" t="str">
+        <f>IF('Drug Information'!E19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E20" s="114" t="str">
+        <f>IF('Drug Information'!F19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="F20" s="114" t="str">
+        <f>IF('Drug Information'!G19=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G20" s="114" t="str">
+        <f>IF('Drug Information'!H19=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H20" s="114" t="str">
+        <f>IF('Drug Information'!I19=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I20" s="114" t="str">
+        <f>IF('Drug Information'!J19=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J20" s="114" t="str">
+        <f>IF('Drug Information'!K19=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K20" s="114" t="str">
+        <f>IF('Drug Information'!L19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L20" s="114" t="str">
+        <f>IF('Drug Information'!M19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M20" s="114" t="str">
+        <f>IF('Drug Information'!N19=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N20" s="114" t="str">
+        <f>IF('Drug Information'!O19=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5" t="str">
+      <c r="B21" s="142" t="str">
         <f>'Drug Information'!B20</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="18" t="str">
-        <f>IF('Drug Information'!D20=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="D21" s="18" t="str">
-        <f>IF('Drug Information'!E20=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E21" s="18" t="str">
-        <f>IF('Drug Information'!F20=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F21" s="18" t="str">
-        <f>IF('Drug Information'!G20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G21" s="18" t="str">
-        <f>IF('Drug Information'!H20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H21" s="18" t="str">
-        <f>IF('Drug Information'!I20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I21" s="18" t="str">
-        <f>IF('Drug Information'!J20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J21" s="18" t="str">
-        <f>IF('Drug Information'!K20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K21" s="18" t="str">
-        <f>IF('Drug Information'!L20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L21" s="18" t="str">
-        <f>IF('Drug Information'!M20=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M21" s="18" t="str">
-        <f>IF('Drug Information'!N20=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N21" s="18" t="str">
-        <f>IF('Drug Information'!O20=1,".","")</f>
-        <v/>
+      <c r="C21" s="115" t="str">
+        <f>IF('Drug Information'!D20=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="D21" s="115" t="str">
+        <f>IF('Drug Information'!E20=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E21" s="115" t="str">
+        <f>IF('Drug Information'!F20=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F21" s="115" t="str">
+        <f>IF('Drug Information'!G20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G21" s="115" t="str">
+        <f>IF('Drug Information'!H20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H21" s="115" t="str">
+        <f>IF('Drug Information'!I20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I21" s="115" t="str">
+        <f>IF('Drug Information'!J20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J21" s="115" t="str">
+        <f>IF('Drug Information'!K20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K21" s="115" t="str">
+        <f>IF('Drug Information'!L20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L21" s="115" t="str">
+        <f>IF('Drug Information'!M20=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M21" s="115" t="str">
+        <f>IF('Drug Information'!N20=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N21" s="115" t="str">
+        <f>IF('Drug Information'!O20=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="str">
+      <c r="B22" s="144" t="str">
         <f>'Drug Information'!B21</f>
         <v>Azithromycin</v>
       </c>
-      <c r="C22" s="18" t="str">
-        <f>IF('Drug Information'!D21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D22" s="18" t="str">
-        <f>IF('Drug Information'!E21=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E22" s="18" t="str">
-        <f>IF('Drug Information'!F21=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F22" s="18" t="str">
-        <f>IF('Drug Information'!G21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G22" s="18" t="str">
-        <f>IF('Drug Information'!H21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H22" s="18" t="str">
-        <f>IF('Drug Information'!I21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I22" s="18" t="str">
-        <f>IF('Drug Information'!J21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J22" s="18" t="str">
-        <f>IF('Drug Information'!K21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K22" s="18" t="str">
-        <f>IF('Drug Information'!L21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L22" s="18" t="str">
-        <f>IF('Drug Information'!M21=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M22" s="18" t="str">
-        <f>IF('Drug Information'!N21=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N22" s="18" t="str">
-        <f>IF('Drug Information'!O21=1,".","")</f>
-        <v>.</v>
+      <c r="C22" s="116" t="str">
+        <f>IF('Drug Information'!D21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D22" s="116" t="str">
+        <f>IF('Drug Information'!E21=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E22" s="116" t="str">
+        <f>IF('Drug Information'!F21=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F22" s="116" t="str">
+        <f>IF('Drug Information'!G21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G22" s="116" t="str">
+        <f>IF('Drug Information'!H21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H22" s="116" t="str">
+        <f>IF('Drug Information'!I21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I22" s="116" t="str">
+        <f>IF('Drug Information'!J21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J22" s="116" t="str">
+        <f>IF('Drug Information'!K21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K22" s="116" t="str">
+        <f>IF('Drug Information'!L21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L22" s="116" t="str">
+        <f>IF('Drug Information'!M21=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M22" s="116" t="str">
+        <f>IF('Drug Information'!N21=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N22" s="116" t="str">
+        <f>IF('Drug Information'!O21=1,"",".")</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="5" t="str">
+      <c r="B23" s="146" t="str">
         <f>'Drug Information'!B22</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="18" t="str">
-        <f>IF('Drug Information'!D22=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="D23" s="18" t="str">
-        <f>IF('Drug Information'!E22=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E23" s="18" t="str">
-        <f>IF('Drug Information'!F22=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F23" s="18" t="str">
-        <f>IF('Drug Information'!G22=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G23" s="18" t="str">
-        <f>IF('Drug Information'!H22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H23" s="18" t="str">
-        <f>IF('Drug Information'!I22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I23" s="18" t="str">
-        <f>IF('Drug Information'!J22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J23" s="18" t="str">
-        <f>IF('Drug Information'!K22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K23" s="18" t="str">
-        <f>IF('Drug Information'!L22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L23" s="18" t="str">
-        <f>IF('Drug Information'!M22=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M23" s="18" t="str">
-        <f>IF('Drug Information'!N22=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N23" s="18" t="str">
-        <f>IF('Drug Information'!O22=1,".","")</f>
-        <v>.</v>
+      <c r="C23" s="117" t="str">
+        <f>IF('Drug Information'!D22=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="D23" s="117" t="str">
+        <f>IF('Drug Information'!E22=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E23" s="117" t="str">
+        <f>IF('Drug Information'!F22=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F23" s="117" t="str">
+        <f>IF('Drug Information'!G22=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G23" s="117" t="str">
+        <f>IF('Drug Information'!H22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H23" s="117" t="str">
+        <f>IF('Drug Information'!I22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I23" s="117" t="str">
+        <f>IF('Drug Information'!J22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J23" s="117" t="str">
+        <f>IF('Drug Information'!K22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K23" s="117" t="str">
+        <f>IF('Drug Information'!L22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L23" s="117" t="str">
+        <f>IF('Drug Information'!M22=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M23" s="117" t="str">
+        <f>IF('Drug Information'!N22=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N23" s="117" t="str">
+        <f>IF('Drug Information'!O22=1,"",".")</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5" t="str">
+      <c r="B24" s="148" t="str">
         <f>'Drug Information'!B23</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="18" t="str">
-        <f>IF('Drug Information'!D23=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="D24" s="18" t="str">
-        <f>IF('Drug Information'!E23=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E24" s="18" t="str">
-        <f>IF('Drug Information'!F23=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F24" s="18" t="str">
-        <f>IF('Drug Information'!G23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G24" s="18" t="str">
-        <f>IF('Drug Information'!H23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H24" s="18" t="str">
-        <f>IF('Drug Information'!I23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I24" s="18" t="str">
-        <f>IF('Drug Information'!J23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J24" s="18" t="str">
-        <f>IF('Drug Information'!K23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K24" s="18" t="str">
-        <f>IF('Drug Information'!L23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L24" s="18" t="str">
-        <f>IF('Drug Information'!M23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M24" s="18" t="str">
-        <f>IF('Drug Information'!N23=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N24" s="18" t="str">
-        <f>IF('Drug Information'!O23=1,".","")</f>
-        <v/>
+      <c r="C24" s="118" t="str">
+        <f>IF('Drug Information'!D23=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="D24" s="118" t="str">
+        <f>IF('Drug Information'!E23=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E24" s="118" t="str">
+        <f>IF('Drug Information'!F23=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F24" s="118" t="str">
+        <f>IF('Drug Information'!G23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G24" s="118" t="str">
+        <f>IF('Drug Information'!H23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H24" s="118" t="str">
+        <f>IF('Drug Information'!I23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I24" s="118" t="str">
+        <f>IF('Drug Information'!J23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J24" s="118" t="str">
+        <f>IF('Drug Information'!K23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K24" s="118" t="str">
+        <f>IF('Drug Information'!L23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L24" s="118" t="str">
+        <f>IF('Drug Information'!M23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M24" s="118" t="str">
+        <f>IF('Drug Information'!N23=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N24" s="118" t="str">
+        <f>IF('Drug Information'!O23=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="5" t="str">
+      <c r="B25" s="150" t="str">
         <f>'Drug Information'!B24</f>
         <v>TMP/SMX</v>
       </c>
-      <c r="C25" s="18" t="str">
-        <f>IF('Drug Information'!D24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="D25" s="18" t="str">
-        <f>IF('Drug Information'!E24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="E25" s="18" t="str">
-        <f>IF('Drug Information'!F24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="F25" s="18" t="str">
-        <f>IF('Drug Information'!G24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="G25" s="18" t="str">
-        <f>IF('Drug Information'!H24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="H25" s="18" t="str">
-        <f>IF('Drug Information'!I24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="I25" s="18" t="str">
-        <f>IF('Drug Information'!J24=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J25" s="18" t="str">
-        <f>IF('Drug Information'!K24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="K25" s="18" t="str">
-        <f>IF('Drug Information'!L24=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L25" s="18" t="str">
-        <f>IF('Drug Information'!M24=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="M25" s="18" t="str">
-        <f>IF('Drug Information'!N24=1,".","")</f>
-        <v/>
-      </c>
-      <c r="N25" s="18" t="str">
-        <f>IF('Drug Information'!O24=1,".","")</f>
-        <v/>
+      <c r="C25" s="119" t="str">
+        <f>IF('Drug Information'!D24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="D25" s="119" t="str">
+        <f>IF('Drug Information'!E24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E25" s="119" t="str">
+        <f>IF('Drug Information'!F24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F25" s="119" t="str">
+        <f>IF('Drug Information'!G24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G25" s="119" t="str">
+        <f>IF('Drug Information'!H24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H25" s="119" t="str">
+        <f>IF('Drug Information'!I24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I25" s="119" t="str">
+        <f>IF('Drug Information'!J24=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J25" s="119" t="str">
+        <f>IF('Drug Information'!K24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K25" s="119" t="str">
+        <f>IF('Drug Information'!L24=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L25" s="119" t="str">
+        <f>IF('Drug Information'!M24=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M25" s="119" t="str">
+        <f>IF('Drug Information'!N24=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N25" s="119" t="str">
+        <f>IF('Drug Information'!O24=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5" t="str">
+      <c r="B26" s="152" t="str">
         <f>'Drug Information'!B25</f>
         <v>Metronidazole</v>
       </c>
-      <c r="C26" s="18" t="str">
-        <f>IF('Drug Information'!D25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="D26" s="18" t="str">
-        <f>IF('Drug Information'!E25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="E26" s="18" t="str">
-        <f>IF('Drug Information'!F25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="F26" s="18" t="str">
-        <f>IF('Drug Information'!G25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="G26" s="18" t="str">
-        <f>IF('Drug Information'!H25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="H26" s="18" t="str">
-        <f>IF('Drug Information'!I25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="I26" s="18" t="str">
-        <f>IF('Drug Information'!J25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="J26" s="18" t="str">
-        <f>IF('Drug Information'!K25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="K26" s="18" t="str">
-        <f>IF('Drug Information'!L25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="L26" s="18" t="str">
-        <f>IF('Drug Information'!M25=1,".","")</f>
-        <v/>
-      </c>
-      <c r="M26" s="18" t="str">
-        <f>IF('Drug Information'!N25=1,".","")</f>
-        <v>.</v>
-      </c>
-      <c r="N26" s="18" t="str">
-        <f>IF('Drug Information'!O25=1,".","")</f>
-        <v/>
+      <c r="C26" s="120" t="str">
+        <f>IF('Drug Information'!D25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D26" s="120" t="str">
+        <f>IF('Drug Information'!E25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E26" s="120" t="str">
+        <f>IF('Drug Information'!F25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="F26" s="120" t="str">
+        <f>IF('Drug Information'!G25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="G26" s="120" t="str">
+        <f>IF('Drug Information'!H25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="H26" s="120" t="str">
+        <f>IF('Drug Information'!I25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="I26" s="120" t="str">
+        <f>IF('Drug Information'!J25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J26" s="120" t="str">
+        <f>IF('Drug Information'!K25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K26" s="120" t="str">
+        <f>IF('Drug Information'!L25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L26" s="120" t="str">
+        <f>IF('Drug Information'!M25=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M26" s="120" t="str">
+        <f>IF('Drug Information'!N25=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N26" s="120" t="str">
+        <f>IF('Drug Information'!O25=1,"",".")</f>
+        <v>.</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="121"/>
+      <c r="G27" s="121"/>
+      <c r="H27" s="121"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="121"/>
+      <c r="K27" s="121"/>
+      <c r="L27" s="121"/>
+      <c r="M27" s="121"/>
+      <c r="N27" s="121"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="94"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="95"/>
+      <c r="N28" s="95"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="94"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="95"/>
+      <c r="N29" s="95"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="94"/>
+      <c r="B30" s="126"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="95"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="95"/>
+      <c r="N30" s="95"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="94"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
+      <c r="G31" s="95"/>
+      <c r="H31" s="95"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="95"/>
+      <c r="M31" s="95"/>
+      <c r="N31" s="95"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="94"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="95"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="95"/>
+      <c r="L32" s="95"/>
+      <c r="M32" s="95"/>
+      <c r="N32" s="95"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="94"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="95"/>
+      <c r="J33" s="95"/>
+      <c r="K33" s="95"/>
+      <c r="L33" s="95"/>
+      <c r="M33" s="95"/>
+      <c r="N33" s="95"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="94"/>
+      <c r="B34" s="126"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="95"/>
+      <c r="K34" s="95"/>
+      <c r="L34" s="95"/>
+      <c r="M34" s="95"/>
+      <c r="N34" s="95"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="94"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="95"/>
+      <c r="H35" s="95"/>
+      <c r="I35" s="95"/>
+      <c r="J35" s="95"/>
+      <c r="K35" s="95"/>
+      <c r="L35" s="95"/>
+      <c r="M35" s="95"/>
+      <c r="N35" s="95"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="94"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="95"/>
+      <c r="I36" s="95"/>
+      <c r="J36" s="95"/>
+      <c r="K36" s="95"/>
+      <c r="L36" s="95"/>
+      <c r="M36" s="95"/>
+      <c r="N36" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4623,7 +4988,12 @@
     <mergeCell ref="M1:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N26">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Resize rows to fit A4 better
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A557AA2-F0E6-46F3-8625-66561D320B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2032CD-0D13-4B46-8E88-2608664F7D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +330,13 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -450,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -613,13 +620,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -898,9 +931,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,9 +946,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,61 +958,9 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1062,10 +1037,64 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1113,12 +1142,6 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1129,6 +1152,12 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1775,7 +1804,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:M26"/>
+      <selection pane="topRight" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3361,15 +3390,15 @@
   </sheetPr>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I36" sqref="I36"/>
+      <selection pane="topRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="127" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="107" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" style="2" bestFit="1" customWidth="1"/>
@@ -3389,1451 +3418,1451 @@
     <col min="19" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="96"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="97" t="s">
+    <row r="1" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="133" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="133" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98" t="s">
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99" t="s">
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="99"/>
-      <c r="M1" s="100" t="s">
+      <c r="L1" s="98"/>
+      <c r="M1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="101" t="s">
+      <c r="N1" s="100" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="124" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="103" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="103" t="s">
+    <row r="2" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="134"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="K2" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="100"/>
-      <c r="N2" s="106" t="s">
+      <c r="M2" s="99"/>
+      <c r="N2" s="104" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+    <row r="3" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="125" t="str">
+      <c r="B3" s="135" t="str">
         <f>'Drug Information'!B2</f>
         <v>Benzylpenicillin</v>
       </c>
-      <c r="C3" s="107" t="str">
+      <c r="C3" s="137" t="str">
         <f>IF('Drug Information'!D2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D3" s="107" t="str">
+      <c r="D3" s="137" t="str">
         <f>IF('Drug Information'!E2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E3" s="107" t="str">
+      <c r="E3" s="137" t="str">
         <f>IF('Drug Information'!F2=1,"",".")</f>
         <v/>
       </c>
-      <c r="F3" s="107" t="str">
+      <c r="F3" s="137" t="str">
         <f>IF('Drug Information'!G2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G3" s="107" t="str">
+      <c r="G3" s="137" t="str">
         <f>IF('Drug Information'!H2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H3" s="107" t="str">
+      <c r="H3" s="137" t="str">
         <f>IF('Drug Information'!I2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I3" s="107" t="str">
+      <c r="I3" s="137" t="str">
         <f>IF('Drug Information'!J2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J3" s="107" t="str">
+      <c r="J3" s="137" t="str">
         <f>IF('Drug Information'!K2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K3" s="107" t="str">
+      <c r="K3" s="137" t="str">
         <f>IF('Drug Information'!L2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L3" s="107" t="str">
+      <c r="L3" s="137" t="str">
         <f>IF('Drug Information'!M2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M3" s="107" t="str">
+      <c r="M3" s="137" t="str">
         <f>IF('Drug Information'!N2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N3" s="107" t="str">
+      <c r="N3" s="137" t="str">
         <f>IF('Drug Information'!O2=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+    <row r="4" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="125" t="str">
+      <c r="B4" s="135" t="str">
         <f>'Drug Information'!B3</f>
         <v>Naficillin, Oxacillin, Flucloxacillin</v>
       </c>
-      <c r="C4" s="107" t="str">
+      <c r="C4" s="137" t="str">
         <f>IF('Drug Information'!D3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D4" s="107" t="str">
+      <c r="D4" s="137" t="str">
         <f>IF('Drug Information'!E3=1,"",".")</f>
         <v/>
       </c>
-      <c r="E4" s="107" t="str">
+      <c r="E4" s="137" t="str">
         <f>IF('Drug Information'!F3=1,"",".")</f>
         <v/>
       </c>
-      <c r="F4" s="107" t="str">
+      <c r="F4" s="137" t="str">
         <f>IF('Drug Information'!G3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G4" s="107" t="str">
+      <c r="G4" s="137" t="str">
         <f>IF('Drug Information'!H3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H4" s="107" t="str">
+      <c r="H4" s="137" t="str">
         <f>IF('Drug Information'!I3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I4" s="107" t="str">
+      <c r="I4" s="137" t="str">
         <f>IF('Drug Information'!J3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J4" s="107" t="str">
+      <c r="J4" s="137" t="str">
         <f>IF('Drug Information'!K3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K4" s="107" t="str">
+      <c r="K4" s="137" t="str">
         <f>IF('Drug Information'!L3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L4" s="107" t="str">
+      <c r="L4" s="137" t="str">
         <f>IF('Drug Information'!M3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M4" s="107" t="str">
+      <c r="M4" s="137" t="str">
         <f>IF('Drug Information'!N3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N4" s="107" t="str">
+      <c r="N4" s="137" t="str">
         <f>IF('Drug Information'!O3=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
+    <row r="5" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="125" t="str">
+      <c r="B5" s="135" t="str">
         <f>'Drug Information'!B4</f>
         <v>Ampicillin, Amoxicillin</v>
       </c>
-      <c r="C5" s="107" t="str">
+      <c r="C5" s="137" t="str">
         <f>IF('Drug Information'!D4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D5" s="107" t="str">
+      <c r="D5" s="137" t="str">
         <f>IF('Drug Information'!E4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E5" s="107" t="str">
+      <c r="E5" s="137" t="str">
         <f>IF('Drug Information'!F4=1,"",".")</f>
         <v/>
       </c>
-      <c r="F5" s="107" t="str">
+      <c r="F5" s="137" t="str">
         <f>IF('Drug Information'!G4=1,"",".")</f>
         <v/>
       </c>
-      <c r="G5" s="107" t="str">
+      <c r="G5" s="137" t="str">
         <f>IF('Drug Information'!H4=1,"",".")</f>
         <v/>
       </c>
-      <c r="H5" s="107" t="str">
+      <c r="H5" s="137" t="str">
         <f>IF('Drug Information'!I4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I5" s="107" t="str">
+      <c r="I5" s="137" t="str">
         <f>IF('Drug Information'!J4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J5" s="107" t="str">
+      <c r="J5" s="137" t="str">
         <f>IF('Drug Information'!K4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K5" s="107" t="str">
+      <c r="K5" s="137" t="str">
         <f>IF('Drug Information'!L4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L5" s="107" t="str">
+      <c r="L5" s="137" t="str">
         <f>IF('Drug Information'!M4=1,"",".")</f>
         <v/>
       </c>
-      <c r="M5" s="107" t="str">
+      <c r="M5" s="137" t="str">
         <f>IF('Drug Information'!N4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N5" s="107" t="str">
+      <c r="N5" s="137" t="str">
         <f>IF('Drug Information'!O4=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+    <row r="6" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="129" t="str">
+      <c r="B6" s="109" t="str">
         <f>'Drug Information'!B5</f>
         <v>Cefazolin, Cefalexin</v>
       </c>
-      <c r="C6" s="108" t="str">
+      <c r="C6" s="138" t="str">
         <f>IF('Drug Information'!D5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D6" s="108" t="str">
+      <c r="D6" s="138" t="str">
         <f>IF('Drug Information'!E5=1,"",".")</f>
         <v/>
       </c>
-      <c r="E6" s="108" t="str">
+      <c r="E6" s="138" t="str">
         <f>IF('Drug Information'!F5=1,"",".")</f>
         <v/>
       </c>
-      <c r="F6" s="108" t="str">
+      <c r="F6" s="138" t="str">
         <f>IF('Drug Information'!G5=1,"",".")</f>
         <v/>
       </c>
-      <c r="G6" s="108" t="str">
+      <c r="G6" s="138" t="str">
         <f>IF('Drug Information'!H5=1,"",".")</f>
         <v/>
       </c>
-      <c r="H6" s="108" t="str">
+      <c r="H6" s="138" t="str">
         <f>IF('Drug Information'!I5=1,"",".")</f>
         <v/>
       </c>
-      <c r="I6" s="108" t="str">
+      <c r="I6" s="138" t="str">
         <f>IF('Drug Information'!J5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J6" s="108" t="str">
+      <c r="J6" s="138" t="str">
         <f>IF('Drug Information'!K5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K6" s="108" t="str">
+      <c r="K6" s="138" t="str">
         <f>IF('Drug Information'!L5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L6" s="108" t="str">
+      <c r="L6" s="138" t="str">
         <f>IF('Drug Information'!M5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M6" s="108" t="str">
+      <c r="M6" s="138" t="str">
         <f>IF('Drug Information'!N5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N6" s="108" t="str">
+      <c r="N6" s="138" t="str">
         <f>IF('Drug Information'!O5=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
+    <row r="7" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="129" t="str">
+      <c r="B7" s="109" t="str">
         <f>'Drug Information'!B6</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="C7" s="108" t="str">
+      <c r="C7" s="138" t="str">
         <f>IF('Drug Information'!D6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D7" s="108" t="str">
+      <c r="D7" s="138" t="str">
         <f>IF('Drug Information'!E6=1,"",".")</f>
         <v/>
       </c>
-      <c r="E7" s="108" t="str">
+      <c r="E7" s="138" t="str">
         <f>IF('Drug Information'!F6=1,"",".")</f>
         <v/>
       </c>
-      <c r="F7" s="108" t="str">
+      <c r="F7" s="138" t="str">
         <f>IF('Drug Information'!G6=1,"",".")</f>
         <v/>
       </c>
-      <c r="G7" s="108" t="str">
+      <c r="G7" s="138" t="str">
         <f>IF('Drug Information'!H6=1,"",".")</f>
         <v/>
       </c>
-      <c r="H7" s="108" t="str">
+      <c r="H7" s="138" t="str">
         <f>IF('Drug Information'!I6=1,"",".")</f>
         <v/>
       </c>
-      <c r="I7" s="108" t="str">
+      <c r="I7" s="138" t="str">
         <f>IF('Drug Information'!J6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J7" s="108" t="str">
+      <c r="J7" s="138" t="str">
         <f>IF('Drug Information'!K6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K7" s="108" t="str">
+      <c r="K7" s="138" t="str">
         <f>IF('Drug Information'!L6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L7" s="108" t="str">
+      <c r="L7" s="138" t="str">
         <f>IF('Drug Information'!M6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M7" s="108" t="str">
+      <c r="M7" s="138" t="str">
         <f>IF('Drug Information'!N6=1,"",".")</f>
         <v/>
       </c>
-      <c r="N7" s="108" t="str">
+      <c r="N7" s="138" t="str">
         <f>IF('Drug Information'!O6=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="130" t="s">
+    <row r="8" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="129" t="str">
+      <c r="B8" s="109" t="str">
         <f>'Drug Information'!B7</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="C8" s="108" t="str">
+      <c r="C8" s="138" t="str">
         <f>IF('Drug Information'!D7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D8" s="108" t="str">
+      <c r="D8" s="138" t="str">
         <f>IF('Drug Information'!E7=1,"",".")</f>
         <v/>
       </c>
-      <c r="E8" s="108" t="str">
+      <c r="E8" s="138" t="str">
         <f>IF('Drug Information'!F7=1,"",".")</f>
         <v/>
       </c>
-      <c r="F8" s="108" t="str">
+      <c r="F8" s="138" t="str">
         <f>IF('Drug Information'!G7=1,"",".")</f>
         <v/>
       </c>
-      <c r="G8" s="108" t="str">
+      <c r="G8" s="138" t="str">
         <f>IF('Drug Information'!H7=1,"",".")</f>
         <v/>
       </c>
-      <c r="H8" s="108" t="str">
+      <c r="H8" s="138" t="str">
         <f>IF('Drug Information'!I7=1,"",".")</f>
         <v/>
       </c>
-      <c r="I8" s="108" t="str">
+      <c r="I8" s="138" t="str">
         <f>IF('Drug Information'!J7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J8" s="108" t="str">
+      <c r="J8" s="138" t="str">
         <f>IF('Drug Information'!K7=1,"",".")</f>
         <v/>
       </c>
-      <c r="K8" s="108" t="str">
+      <c r="K8" s="138" t="str">
         <f>IF('Drug Information'!L7=1,"",".")</f>
         <v/>
       </c>
-      <c r="L8" s="108" t="str">
+      <c r="L8" s="138" t="str">
         <f>IF('Drug Information'!M7=1,"",".")</f>
         <v/>
       </c>
-      <c r="M8" s="108" t="str">
+      <c r="M8" s="138" t="str">
         <f>IF('Drug Information'!N7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N8" s="108" t="str">
+      <c r="N8" s="138" t="str">
         <f>IF('Drug Information'!O7=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
-      <c r="B9" s="129" t="str">
+    <row r="9" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="110"/>
+      <c r="B9" s="109" t="str">
         <f>'Drug Information'!B8</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="C9" s="108" t="str">
+      <c r="C9" s="138" t="str">
         <f>IF('Drug Information'!D8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D9" s="108" t="str">
+      <c r="D9" s="138" t="str">
         <f>IF('Drug Information'!E8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E9" s="108" t="str">
+      <c r="E9" s="138" t="str">
         <f>IF('Drug Information'!F8=1,"",".")</f>
         <v/>
       </c>
-      <c r="F9" s="108" t="str">
+      <c r="F9" s="138" t="str">
         <f>IF('Drug Information'!G8=1,"",".")</f>
         <v/>
       </c>
-      <c r="G9" s="108" t="str">
+      <c r="G9" s="138" t="str">
         <f>IF('Drug Information'!H8=1,"",".")</f>
         <v/>
       </c>
-      <c r="H9" s="108" t="str">
+      <c r="H9" s="138" t="str">
         <f>IF('Drug Information'!I8=1,"",".")</f>
         <v/>
       </c>
-      <c r="I9" s="108" t="str">
+      <c r="I9" s="138" t="str">
         <f>IF('Drug Information'!J8=1,"",".")</f>
         <v/>
       </c>
-      <c r="J9" s="108" t="str">
+      <c r="J9" s="138" t="str">
         <f>IF('Drug Information'!K8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K9" s="108" t="str">
+      <c r="K9" s="138" t="str">
         <f>IF('Drug Information'!L8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L9" s="108" t="str">
+      <c r="L9" s="138" t="str">
         <f>IF('Drug Information'!M8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M9" s="108" t="str">
+      <c r="M9" s="138" t="str">
         <f>IF('Drug Information'!N8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N9" s="108" t="str">
+      <c r="N9" s="138" t="str">
         <f>IF('Drug Information'!O8=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="128" t="s">
+    <row r="10" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="129" t="str">
+      <c r="B10" s="109" t="str">
         <f>'Drug Information'!B9</f>
         <v>Cefepime</v>
       </c>
-      <c r="C10" s="108" t="str">
+      <c r="C10" s="138" t="str">
         <f>IF('Drug Information'!D9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D10" s="108" t="str">
+      <c r="D10" s="138" t="str">
         <f>IF('Drug Information'!E9=1,"",".")</f>
         <v/>
       </c>
-      <c r="E10" s="108" t="str">
+      <c r="E10" s="138" t="str">
         <f>IF('Drug Information'!F9=1,"",".")</f>
         <v/>
       </c>
-      <c r="F10" s="108" t="str">
+      <c r="F10" s="138" t="str">
         <f>IF('Drug Information'!G9=1,"",".")</f>
         <v/>
       </c>
-      <c r="G10" s="108" t="str">
+      <c r="G10" s="138" t="str">
         <f>IF('Drug Information'!H9=1,"",".")</f>
         <v/>
       </c>
-      <c r="H10" s="108" t="str">
+      <c r="H10" s="138" t="str">
         <f>IF('Drug Information'!I9=1,"",".")</f>
         <v/>
       </c>
-      <c r="I10" s="108" t="str">
+      <c r="I10" s="138" t="str">
         <f>IF('Drug Information'!J9=1,"",".")</f>
         <v/>
       </c>
-      <c r="J10" s="108" t="str">
+      <c r="J10" s="138" t="str">
         <f>IF('Drug Information'!K9=1,"",".")</f>
         <v/>
       </c>
-      <c r="K10" s="108" t="str">
+      <c r="K10" s="138" t="str">
         <f>IF('Drug Information'!L9=1,"",".")</f>
         <v/>
       </c>
-      <c r="L10" s="108" t="str">
+      <c r="L10" s="138" t="str">
         <f>IF('Drug Information'!M9=1,"",".")</f>
         <v/>
       </c>
-      <c r="M10" s="108" t="str">
+      <c r="M10" s="138" t="str">
         <f>IF('Drug Information'!N9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N10" s="108" t="str">
+      <c r="N10" s="138" t="str">
         <f>IF('Drug Information'!O9=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="131" t="s">
+    <row r="11" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="132" t="str">
+      <c r="B11" s="112" t="str">
         <f>'Drug Information'!B10</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="C11" s="109" t="str">
+      <c r="C11" s="139" t="str">
         <f>IF('Drug Information'!D10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D11" s="109" t="str">
+      <c r="D11" s="139" t="str">
         <f>IF('Drug Information'!E10=1,"",".")</f>
         <v/>
       </c>
-      <c r="E11" s="109" t="str">
+      <c r="E11" s="139" t="str">
         <f>IF('Drug Information'!F10=1,"",".")</f>
         <v/>
       </c>
-      <c r="F11" s="109" t="str">
+      <c r="F11" s="139" t="str">
         <f>IF('Drug Information'!G10=1,"",".")</f>
         <v/>
       </c>
-      <c r="G11" s="109" t="str">
+      <c r="G11" s="139" t="str">
         <f>IF('Drug Information'!H10=1,"",".")</f>
         <v/>
       </c>
-      <c r="H11" s="109" t="str">
+      <c r="H11" s="139" t="str">
         <f>IF('Drug Information'!I10=1,"",".")</f>
         <v/>
       </c>
-      <c r="I11" s="109" t="str">
+      <c r="I11" s="139" t="str">
         <f>IF('Drug Information'!J10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J11" s="109" t="str">
+      <c r="J11" s="139" t="str">
         <f>IF('Drug Information'!K10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K11" s="109" t="str">
+      <c r="K11" s="139" t="str">
         <f>IF('Drug Information'!L10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L11" s="109" t="str">
+      <c r="L11" s="139" t="str">
         <f>IF('Drug Information'!M10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M11" s="109" t="str">
+      <c r="M11" s="139" t="str">
         <f>IF('Drug Information'!N10=1,"",".")</f>
         <v/>
       </c>
-      <c r="N11" s="109" t="str">
+      <c r="N11" s="139" t="str">
         <f>IF('Drug Information'!O10=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="131"/>
-      <c r="B12" s="132" t="str">
+    <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="111"/>
+      <c r="B12" s="112" t="str">
         <f>'Drug Information'!B11</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="C12" s="109" t="str">
+      <c r="C12" s="139" t="str">
         <f>IF('Drug Information'!D11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D12" s="109" t="str">
+      <c r="D12" s="139" t="str">
         <f>IF('Drug Information'!E11=1,"",".")</f>
         <v/>
       </c>
-      <c r="E12" s="109" t="str">
+      <c r="E12" s="139" t="str">
         <f>IF('Drug Information'!F11=1,"",".")</f>
         <v/>
       </c>
-      <c r="F12" s="109" t="str">
+      <c r="F12" s="139" t="str">
         <f>IF('Drug Information'!G11=1,"",".")</f>
         <v/>
       </c>
-      <c r="G12" s="109" t="str">
+      <c r="G12" s="139" t="str">
         <f>IF('Drug Information'!H11=1,"",".")</f>
         <v/>
       </c>
-      <c r="H12" s="109" t="str">
+      <c r="H12" s="139" t="str">
         <f>IF('Drug Information'!I11=1,"",".")</f>
         <v/>
       </c>
-      <c r="I12" s="109" t="str">
+      <c r="I12" s="139" t="str">
         <f>IF('Drug Information'!J11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J12" s="109" t="str">
+      <c r="J12" s="139" t="str">
         <f>IF('Drug Information'!K11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K12" s="109" t="str">
+      <c r="K12" s="139" t="str">
         <f>IF('Drug Information'!L11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L12" s="109" t="str">
+      <c r="L12" s="139" t="str">
         <f>IF('Drug Information'!M11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M12" s="109" t="str">
+      <c r="M12" s="139" t="str">
         <f>IF('Drug Information'!N11=1,"",".")</f>
         <v/>
       </c>
-      <c r="N12" s="109" t="str">
+      <c r="N12" s="139" t="str">
         <f>IF('Drug Information'!O11=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
-      <c r="B13" s="132" t="str">
+    <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="111"/>
+      <c r="B13" s="112" t="str">
         <f>'Drug Information'!B12</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="C13" s="109" t="str">
+      <c r="C13" s="139" t="str">
         <f>IF('Drug Information'!D12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D13" s="109" t="str">
+      <c r="D13" s="139" t="str">
         <f>IF('Drug Information'!E12=1,"",".")</f>
         <v/>
       </c>
-      <c r="E13" s="109" t="str">
+      <c r="E13" s="139" t="str">
         <f>IF('Drug Information'!F12=1,"",".")</f>
         <v/>
       </c>
-      <c r="F13" s="109" t="str">
+      <c r="F13" s="139" t="str">
         <f>IF('Drug Information'!G12=1,"",".")</f>
         <v/>
       </c>
-      <c r="G13" s="109" t="str">
+      <c r="G13" s="139" t="str">
         <f>IF('Drug Information'!H12=1,"",".")</f>
         <v/>
       </c>
-      <c r="H13" s="109" t="str">
+      <c r="H13" s="139" t="str">
         <f>IF('Drug Information'!I12=1,"",".")</f>
         <v/>
       </c>
-      <c r="I13" s="109" t="str">
+      <c r="I13" s="139" t="str">
         <f>IF('Drug Information'!J12=1,"",".")</f>
         <v/>
       </c>
-      <c r="J13" s="109" t="str">
+      <c r="J13" s="139" t="str">
         <f>IF('Drug Information'!K12=1,"",".")</f>
         <v/>
       </c>
-      <c r="K13" s="109" t="str">
+      <c r="K13" s="139" t="str">
         <f>IF('Drug Information'!L12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L13" s="109" t="str">
+      <c r="L13" s="139" t="str">
         <f>IF('Drug Information'!M12=1,"",".")</f>
         <v/>
       </c>
-      <c r="M13" s="109" t="str">
+      <c r="M13" s="139" t="str">
         <f>IF('Drug Information'!N12=1,"",".")</f>
         <v/>
       </c>
-      <c r="N13" s="109" t="str">
+      <c r="N13" s="139" t="str">
         <f>IF('Drug Information'!O12=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="133" t="s">
+    <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="134" t="str">
+      <c r="B14" s="114" t="str">
         <f>'Drug Information'!B13</f>
         <v>Ertapenem</v>
       </c>
-      <c r="C14" s="110" t="str">
+      <c r="C14" s="140" t="str">
         <f>IF('Drug Information'!D13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D14" s="110" t="str">
+      <c r="D14" s="140" t="str">
         <f>IF('Drug Information'!E13=1,"",".")</f>
         <v/>
       </c>
-      <c r="E14" s="110" t="str">
+      <c r="E14" s="140" t="str">
         <f>IF('Drug Information'!F13=1,"",".")</f>
         <v/>
       </c>
-      <c r="F14" s="110" t="str">
+      <c r="F14" s="140" t="str">
         <f>IF('Drug Information'!G13=1,"",".")</f>
         <v/>
       </c>
-      <c r="G14" s="110" t="str">
+      <c r="G14" s="140" t="str">
         <f>IF('Drug Information'!H13=1,"",".")</f>
         <v/>
       </c>
-      <c r="H14" s="110" t="str">
+      <c r="H14" s="140" t="str">
         <f>IF('Drug Information'!I13=1,"",".")</f>
         <v/>
       </c>
-      <c r="I14" s="110" t="str">
+      <c r="I14" s="140" t="str">
         <f>IF('Drug Information'!J13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J14" s="110" t="str">
+      <c r="J14" s="140" t="str">
         <f>IF('Drug Information'!K13=1,"",".")</f>
         <v/>
       </c>
-      <c r="K14" s="110" t="str">
+      <c r="K14" s="140" t="str">
         <f>IF('Drug Information'!L13=1,"",".")</f>
         <v/>
       </c>
-      <c r="L14" s="110" t="str">
+      <c r="L14" s="140" t="str">
         <f>IF('Drug Information'!M13=1,"",".")</f>
         <v/>
       </c>
-      <c r="M14" s="110" t="str">
+      <c r="M14" s="140" t="str">
         <f>IF('Drug Information'!N13=1,"",".")</f>
         <v/>
       </c>
-      <c r="N14" s="110" t="str">
+      <c r="N14" s="140" t="str">
         <f>IF('Drug Information'!O13=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="134" t="str">
+    <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="113"/>
+      <c r="B15" s="114" t="str">
         <f>'Drug Information'!B14</f>
         <v>Imipenem, Meropenem</v>
       </c>
-      <c r="C15" s="110" t="str">
+      <c r="C15" s="140" t="str">
         <f>IF('Drug Information'!D14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D15" s="110" t="str">
+      <c r="D15" s="140" t="str">
         <f>IF('Drug Information'!E14=1,"",".")</f>
         <v/>
       </c>
-      <c r="E15" s="110" t="str">
+      <c r="E15" s="140" t="str">
         <f>IF('Drug Information'!F14=1,"",".")</f>
         <v/>
       </c>
-      <c r="F15" s="110" t="str">
+      <c r="F15" s="140" t="str">
         <f>IF('Drug Information'!G14=1,"",".")</f>
         <v/>
       </c>
-      <c r="G15" s="110" t="str">
+      <c r="G15" s="140" t="str">
         <f>IF('Drug Information'!H14=1,"",".")</f>
         <v/>
       </c>
-      <c r="H15" s="110" t="str">
+      <c r="H15" s="140" t="str">
         <f>IF('Drug Information'!I14=1,"",".")</f>
         <v/>
       </c>
-      <c r="I15" s="110" t="str">
+      <c r="I15" s="140" t="str">
         <f>IF('Drug Information'!J14=1,"",".")</f>
         <v/>
       </c>
-      <c r="J15" s="110" t="str">
+      <c r="J15" s="140" t="str">
         <f>IF('Drug Information'!K14=1,"",".")</f>
         <v/>
       </c>
-      <c r="K15" s="110" t="str">
+      <c r="K15" s="140" t="str">
         <f>IF('Drug Information'!L14=1,"",".")</f>
         <v/>
       </c>
-      <c r="L15" s="110" t="str">
+      <c r="L15" s="140" t="str">
         <f>IF('Drug Information'!M14=1,"",".")</f>
         <v/>
       </c>
-      <c r="M15" s="110" t="str">
+      <c r="M15" s="140" t="str">
         <f>IF('Drug Information'!N14=1,"",".")</f>
         <v/>
       </c>
-      <c r="N15" s="110" t="str">
+      <c r="N15" s="140" t="str">
         <f>IF('Drug Information'!O14=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="135" t="s">
+    <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="136" t="str">
+      <c r="B16" s="116" t="str">
         <f>'Drug Information'!B15</f>
         <v>Aztreonam</v>
       </c>
-      <c r="C16" s="111" t="str">
+      <c r="C16" s="141" t="str">
         <f>IF('Drug Information'!D15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D16" s="111" t="str">
+      <c r="D16" s="141" t="str">
         <f>IF('Drug Information'!E15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E16" s="111" t="str">
+      <c r="E16" s="141" t="str">
         <f>IF('Drug Information'!F15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F16" s="111" t="str">
+      <c r="F16" s="141" t="str">
         <f>IF('Drug Information'!G15=1,"",".")</f>
         <v/>
       </c>
-      <c r="G16" s="111" t="str">
+      <c r="G16" s="141" t="str">
         <f>IF('Drug Information'!H15=1,"",".")</f>
         <v/>
       </c>
-      <c r="H16" s="111" t="str">
+      <c r="H16" s="141" t="str">
         <f>IF('Drug Information'!I15=1,"",".")</f>
         <v/>
       </c>
-      <c r="I16" s="111" t="str">
+      <c r="I16" s="141" t="str">
         <f>IF('Drug Information'!J15=1,"",".")</f>
         <v/>
       </c>
-      <c r="J16" s="111" t="str">
+      <c r="J16" s="141" t="str">
         <f>IF('Drug Information'!K15=1,"",".")</f>
         <v/>
       </c>
-      <c r="K16" s="111" t="str">
+      <c r="K16" s="141" t="str">
         <f>IF('Drug Information'!L15=1,"",".")</f>
         <v/>
       </c>
-      <c r="L16" s="111" t="str">
+      <c r="L16" s="141" t="str">
         <f>IF('Drug Information'!M15=1,"",".")</f>
         <v/>
       </c>
-      <c r="M16" s="111" t="str">
+      <c r="M16" s="141" t="str">
         <f>IF('Drug Information'!N15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N16" s="111" t="str">
+      <c r="N16" s="141" t="str">
         <f>IF('Drug Information'!O15=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="137" t="s">
+    <row r="17" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="138" t="str">
+      <c r="B17" s="118" t="str">
         <f>'Drug Information'!B16</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="C17" s="112" t="str">
+      <c r="C17" s="142" t="str">
         <f>IF('Drug Information'!D16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D17" s="112" t="str">
+      <c r="D17" s="142" t="str">
         <f>IF('Drug Information'!E16=1,"",".")</f>
         <v/>
       </c>
-      <c r="E17" s="112" t="str">
+      <c r="E17" s="142" t="str">
         <f>IF('Drug Information'!F16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F17" s="112" t="str">
+      <c r="F17" s="142" t="str">
         <f>IF('Drug Information'!G16=1,"",".")</f>
         <v/>
       </c>
-      <c r="G17" s="112" t="str">
+      <c r="G17" s="142" t="str">
         <f>IF('Drug Information'!H16=1,"",".")</f>
         <v/>
       </c>
-      <c r="H17" s="112" t="str">
+      <c r="H17" s="142" t="str">
         <f>IF('Drug Information'!I16=1,"",".")</f>
         <v/>
       </c>
-      <c r="I17" s="112" t="str">
+      <c r="I17" s="142" t="str">
         <f>IF('Drug Information'!J16=1,"",".")</f>
         <v/>
       </c>
-      <c r="J17" s="112" t="str">
+      <c r="J17" s="142" t="str">
         <f>IF('Drug Information'!K16=1,"",".")</f>
         <v/>
       </c>
-      <c r="K17" s="112" t="str">
+      <c r="K17" s="142" t="str">
         <f>IF('Drug Information'!L16=1,"",".")</f>
         <v/>
       </c>
-      <c r="L17" s="112" t="str">
+      <c r="L17" s="142" t="str">
         <f>IF('Drug Information'!M16=1,"",".")</f>
         <v/>
       </c>
-      <c r="M17" s="112" t="str">
+      <c r="M17" s="142" t="str">
         <f>IF('Drug Information'!N16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N17" s="112" t="str">
+      <c r="N17" s="142" t="str">
         <f>IF('Drug Information'!O16=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138" t="str">
+    <row r="18" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="117"/>
+      <c r="B18" s="118" t="str">
         <f>'Drug Information'!B17</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="C18" s="112" t="str">
+      <c r="C18" s="142" t="str">
         <f>IF('Drug Information'!D17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D18" s="112" t="str">
+      <c r="D18" s="142" t="str">
         <f>IF('Drug Information'!E17=1,"",".")</f>
         <v/>
       </c>
-      <c r="E18" s="112" t="str">
+      <c r="E18" s="142" t="str">
         <f>IF('Drug Information'!F17=1,"",".")</f>
         <v/>
       </c>
-      <c r="F18" s="112" t="str">
+      <c r="F18" s="142" t="str">
         <f>IF('Drug Information'!G17=1,"",".")</f>
         <v/>
       </c>
-      <c r="G18" s="112" t="str">
+      <c r="G18" s="142" t="str">
         <f>IF('Drug Information'!H17=1,"",".")</f>
         <v/>
       </c>
-      <c r="H18" s="112" t="str">
+      <c r="H18" s="142" t="str">
         <f>IF('Drug Information'!I17=1,"",".")</f>
         <v/>
       </c>
-      <c r="I18" s="112" t="str">
+      <c r="I18" s="142" t="str">
         <f>IF('Drug Information'!J17=1,"",".")</f>
         <v/>
       </c>
-      <c r="J18" s="112" t="str">
+      <c r="J18" s="142" t="str">
         <f>IF('Drug Information'!K17=1,"",".")</f>
         <v/>
       </c>
-      <c r="K18" s="112" t="str">
+      <c r="K18" s="142" t="str">
         <f>IF('Drug Information'!L17=1,"",".")</f>
         <v/>
       </c>
-      <c r="L18" s="112" t="str">
+      <c r="L18" s="142" t="str">
         <f>IF('Drug Information'!M17=1,"",".")</f>
         <v/>
       </c>
-      <c r="M18" s="112" t="str">
+      <c r="M18" s="142" t="str">
         <f>IF('Drug Information'!N17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N18" s="112" t="str">
+      <c r="N18" s="142" t="str">
         <f>IF('Drug Information'!O17=1,"",".")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138" t="str">
+    <row r="19" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="117"/>
+      <c r="B19" s="118" t="str">
         <f>'Drug Information'!B18</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="C19" s="113" t="str">
+      <c r="C19" s="143" t="str">
         <f>IF('Drug Information'!D18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D19" s="113" t="str">
+      <c r="D19" s="143" t="str">
         <f>IF('Drug Information'!E18=1,"",".")</f>
         <v/>
       </c>
-      <c r="E19" s="113" t="str">
+      <c r="E19" s="143" t="str">
         <f>IF('Drug Information'!F18=1,"",".")</f>
         <v/>
       </c>
-      <c r="F19" s="113" t="str">
+      <c r="F19" s="143" t="str">
         <f>IF('Drug Information'!G18=1,"",".")</f>
         <v/>
       </c>
-      <c r="G19" s="113" t="str">
+      <c r="G19" s="143" t="str">
         <f>IF('Drug Information'!H18=1,"",".")</f>
         <v/>
       </c>
-      <c r="H19" s="113" t="str">
+      <c r="H19" s="143" t="str">
         <f>IF('Drug Information'!I18=1,"",".")</f>
         <v/>
       </c>
-      <c r="I19" s="113" t="str">
+      <c r="I19" s="143" t="str">
         <f>IF('Drug Information'!J18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J19" s="113" t="str">
+      <c r="J19" s="143" t="str">
         <f>IF('Drug Information'!K18=1,"",".")</f>
         <v/>
       </c>
-      <c r="K19" s="113" t="str">
+      <c r="K19" s="143" t="str">
         <f>IF('Drug Information'!L18=1,"",".")</f>
         <v/>
       </c>
-      <c r="L19" s="113" t="str">
+      <c r="L19" s="143" t="str">
         <f>IF('Drug Information'!M18=1,"",".")</f>
         <v/>
       </c>
-      <c r="M19" s="113" t="str">
+      <c r="M19" s="143" t="str">
         <f>IF('Drug Information'!N18=1,"",".")</f>
         <v/>
       </c>
-      <c r="N19" s="113" t="str">
+      <c r="N19" s="143" t="str">
         <f>IF('Drug Information'!O18=1,"",".")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="139" t="s">
+    <row r="20" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="140" t="str">
+      <c r="B20" s="120" t="str">
         <f>'Drug Information'!B19</f>
         <v>Gentamicin, Tobramycin, Amikacin</v>
       </c>
-      <c r="C20" s="114" t="str">
+      <c r="C20" s="144" t="str">
         <f>IF('Drug Information'!D19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D20" s="114" t="str">
+      <c r="D20" s="144" t="str">
         <f>IF('Drug Information'!E19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E20" s="114" t="str">
+      <c r="E20" s="144" t="str">
         <f>IF('Drug Information'!F19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F20" s="114" t="str">
+      <c r="F20" s="144" t="str">
         <f>IF('Drug Information'!G19=1,"",".")</f>
         <v/>
       </c>
-      <c r="G20" s="114" t="str">
+      <c r="G20" s="144" t="str">
         <f>IF('Drug Information'!H19=1,"",".")</f>
         <v/>
       </c>
-      <c r="H20" s="114" t="str">
+      <c r="H20" s="144" t="str">
         <f>IF('Drug Information'!I19=1,"",".")</f>
         <v/>
       </c>
-      <c r="I20" s="114" t="str">
+      <c r="I20" s="144" t="str">
         <f>IF('Drug Information'!J19=1,"",".")</f>
         <v/>
       </c>
-      <c r="J20" s="114" t="str">
+      <c r="J20" s="144" t="str">
         <f>IF('Drug Information'!K19=1,"",".")</f>
         <v/>
       </c>
-      <c r="K20" s="114" t="str">
+      <c r="K20" s="144" t="str">
         <f>IF('Drug Information'!L19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L20" s="114" t="str">
+      <c r="L20" s="144" t="str">
         <f>IF('Drug Information'!M19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M20" s="114" t="str">
+      <c r="M20" s="144" t="str">
         <f>IF('Drug Information'!N19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N20" s="114" t="str">
+      <c r="N20" s="144" t="str">
         <f>IF('Drug Information'!O19=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="141" t="s">
+    <row r="21" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="142" t="str">
+      <c r="B21" s="122" t="str">
         <f>'Drug Information'!B20</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="115" t="str">
+      <c r="C21" s="145" t="str">
         <f>IF('Drug Information'!D20=1,"",".")</f>
         <v/>
       </c>
-      <c r="D21" s="115" t="str">
+      <c r="D21" s="145" t="str">
         <f>IF('Drug Information'!E20=1,"",".")</f>
         <v/>
       </c>
-      <c r="E21" s="115" t="str">
+      <c r="E21" s="145" t="str">
         <f>IF('Drug Information'!F20=1,"",".")</f>
         <v/>
       </c>
-      <c r="F21" s="115" t="str">
+      <c r="F21" s="145" t="str">
         <f>IF('Drug Information'!G20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G21" s="115" t="str">
+      <c r="G21" s="145" t="str">
         <f>IF('Drug Information'!H20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H21" s="115" t="str">
+      <c r="H21" s="145" t="str">
         <f>IF('Drug Information'!I20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I21" s="115" t="str">
+      <c r="I21" s="145" t="str">
         <f>IF('Drug Information'!J20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J21" s="115" t="str">
+      <c r="J21" s="145" t="str">
         <f>IF('Drug Information'!K20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K21" s="115" t="str">
+      <c r="K21" s="145" t="str">
         <f>IF('Drug Information'!L20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L21" s="115" t="str">
+      <c r="L21" s="145" t="str">
         <f>IF('Drug Information'!M20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M21" s="115" t="str">
+      <c r="M21" s="145" t="str">
         <f>IF('Drug Information'!N20=1,"",".")</f>
         <v/>
       </c>
-      <c r="N21" s="115" t="str">
+      <c r="N21" s="145" t="str">
         <f>IF('Drug Information'!O20=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="143" t="s">
+    <row r="22" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="144" t="str">
+      <c r="B22" s="124" t="str">
         <f>'Drug Information'!B21</f>
         <v>Azithromycin</v>
       </c>
-      <c r="C22" s="116" t="str">
+      <c r="C22" s="146" t="str">
         <f>IF('Drug Information'!D21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D22" s="116" t="str">
+      <c r="D22" s="146" t="str">
         <f>IF('Drug Information'!E21=1,"",".")</f>
         <v/>
       </c>
-      <c r="E22" s="116" t="str">
+      <c r="E22" s="146" t="str">
         <f>IF('Drug Information'!F21=1,"",".")</f>
         <v/>
       </c>
-      <c r="F22" s="116" t="str">
+      <c r="F22" s="146" t="str">
         <f>IF('Drug Information'!G21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G22" s="116" t="str">
+      <c r="G22" s="146" t="str">
         <f>IF('Drug Information'!H21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H22" s="116" t="str">
+      <c r="H22" s="146" t="str">
         <f>IF('Drug Information'!I21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I22" s="116" t="str">
+      <c r="I22" s="146" t="str">
         <f>IF('Drug Information'!J21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J22" s="116" t="str">
+      <c r="J22" s="146" t="str">
         <f>IF('Drug Information'!K21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K22" s="116" t="str">
+      <c r="K22" s="146" t="str">
         <f>IF('Drug Information'!L21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L22" s="116" t="str">
+      <c r="L22" s="146" t="str">
         <f>IF('Drug Information'!M21=1,"",".")</f>
         <v/>
       </c>
-      <c r="M22" s="116" t="str">
+      <c r="M22" s="146" t="str">
         <f>IF('Drug Information'!N21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N22" s="116" t="str">
+      <c r="N22" s="146" t="str">
         <f>IF('Drug Information'!O21=1,"",".")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="145" t="s">
+    <row r="23" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="146" t="str">
+      <c r="B23" s="126" t="str">
         <f>'Drug Information'!B22</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="117" t="str">
+      <c r="C23" s="147" t="str">
         <f>IF('Drug Information'!D22=1,"",".")</f>
         <v/>
       </c>
-      <c r="D23" s="117" t="str">
+      <c r="D23" s="147" t="str">
         <f>IF('Drug Information'!E22=1,"",".")</f>
         <v/>
       </c>
-      <c r="E23" s="117" t="str">
+      <c r="E23" s="147" t="str">
         <f>IF('Drug Information'!F22=1,"",".")</f>
         <v/>
       </c>
-      <c r="F23" s="117" t="str">
+      <c r="F23" s="147" t="str">
         <f>IF('Drug Information'!G22=1,"",".")</f>
         <v/>
       </c>
-      <c r="G23" s="117" t="str">
+      <c r="G23" s="147" t="str">
         <f>IF('Drug Information'!H22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H23" s="117" t="str">
+      <c r="H23" s="147" t="str">
         <f>IF('Drug Information'!I22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I23" s="117" t="str">
+      <c r="I23" s="147" t="str">
         <f>IF('Drug Information'!J22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J23" s="117" t="str">
+      <c r="J23" s="147" t="str">
         <f>IF('Drug Information'!K22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K23" s="117" t="str">
+      <c r="K23" s="147" t="str">
         <f>IF('Drug Information'!L22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L23" s="117" t="str">
+      <c r="L23" s="147" t="str">
         <f>IF('Drug Information'!M22=1,"",".")</f>
         <v/>
       </c>
-      <c r="M23" s="117" t="str">
+      <c r="M23" s="147" t="str">
         <f>IF('Drug Information'!N22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N23" s="117" t="str">
+      <c r="N23" s="147" t="str">
         <f>IF('Drug Information'!O22=1,"",".")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="147" t="s">
+    <row r="24" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="148" t="str">
+      <c r="B24" s="128" t="str">
         <f>'Drug Information'!B23</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="118" t="str">
+      <c r="C24" s="148" t="str">
         <f>IF('Drug Information'!D23=1,"",".")</f>
         <v/>
       </c>
-      <c r="D24" s="118" t="str">
+      <c r="D24" s="148" t="str">
         <f>IF('Drug Information'!E23=1,"",".")</f>
         <v/>
       </c>
-      <c r="E24" s="118" t="str">
+      <c r="E24" s="148" t="str">
         <f>IF('Drug Information'!F23=1,"",".")</f>
         <v/>
       </c>
-      <c r="F24" s="118" t="str">
+      <c r="F24" s="148" t="str">
         <f>IF('Drug Information'!G23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G24" s="118" t="str">
+      <c r="G24" s="148" t="str">
         <f>IF('Drug Information'!H23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H24" s="118" t="str">
+      <c r="H24" s="148" t="str">
         <f>IF('Drug Information'!I23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I24" s="118" t="str">
+      <c r="I24" s="148" t="str">
         <f>IF('Drug Information'!J23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J24" s="118" t="str">
+      <c r="J24" s="148" t="str">
         <f>IF('Drug Information'!K23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K24" s="118" t="str">
+      <c r="K24" s="148" t="str">
         <f>IF('Drug Information'!L23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L24" s="118" t="str">
+      <c r="L24" s="148" t="str">
         <f>IF('Drug Information'!M23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M24" s="118" t="str">
+      <c r="M24" s="148" t="str">
         <f>IF('Drug Information'!N23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N24" s="118" t="str">
+      <c r="N24" s="148" t="str">
         <f>IF('Drug Information'!O23=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
+    <row r="25" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="150" t="str">
+      <c r="B25" s="130" t="str">
         <f>'Drug Information'!B24</f>
         <v>TMP/SMX</v>
       </c>
-      <c r="C25" s="119" t="str">
+      <c r="C25" s="149" t="str">
         <f>IF('Drug Information'!D24=1,"",".")</f>
         <v/>
       </c>
-      <c r="D25" s="119" t="str">
+      <c r="D25" s="149" t="str">
         <f>IF('Drug Information'!E24=1,"",".")</f>
         <v/>
       </c>
-      <c r="E25" s="119" t="str">
+      <c r="E25" s="149" t="str">
         <f>IF('Drug Information'!F24=1,"",".")</f>
         <v/>
       </c>
-      <c r="F25" s="119" t="str">
+      <c r="F25" s="149" t="str">
         <f>IF('Drug Information'!G24=1,"",".")</f>
         <v/>
       </c>
-      <c r="G25" s="119" t="str">
+      <c r="G25" s="149" t="str">
         <f>IF('Drug Information'!H24=1,"",".")</f>
         <v/>
       </c>
-      <c r="H25" s="119" t="str">
+      <c r="H25" s="149" t="str">
         <f>IF('Drug Information'!I24=1,"",".")</f>
         <v/>
       </c>
-      <c r="I25" s="119" t="str">
+      <c r="I25" s="149" t="str">
         <f>IF('Drug Information'!J24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J25" s="119" t="str">
+      <c r="J25" s="149" t="str">
         <f>IF('Drug Information'!K24=1,"",".")</f>
         <v/>
       </c>
-      <c r="K25" s="119" t="str">
+      <c r="K25" s="149" t="str">
         <f>IF('Drug Information'!L24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L25" s="119" t="str">
+      <c r="L25" s="149" t="str">
         <f>IF('Drug Information'!M24=1,"",".")</f>
         <v/>
       </c>
-      <c r="M25" s="119" t="str">
+      <c r="M25" s="149" t="str">
         <f>IF('Drug Information'!N24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N25" s="119" t="str">
+      <c r="N25" s="149" t="str">
         <f>IF('Drug Information'!O24=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="151" t="s">
+    <row r="26" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="152" t="str">
+      <c r="B26" s="131" t="str">
         <f>'Drug Information'!B25</f>
         <v>Metronidazole</v>
       </c>
-      <c r="C26" s="120" t="str">
+      <c r="C26" s="150" t="str">
         <f>IF('Drug Information'!D25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D26" s="120" t="str">
+      <c r="D26" s="150" t="str">
         <f>IF('Drug Information'!E25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E26" s="120" t="str">
+      <c r="E26" s="150" t="str">
         <f>IF('Drug Information'!F25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F26" s="120" t="str">
+      <c r="F26" s="150" t="str">
         <f>IF('Drug Information'!G25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G26" s="120" t="str">
+      <c r="G26" s="150" t="str">
         <f>IF('Drug Information'!H25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H26" s="120" t="str">
+      <c r="H26" s="150" t="str">
         <f>IF('Drug Information'!I25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I26" s="120" t="str">
+      <c r="I26" s="150" t="str">
         <f>IF('Drug Information'!J25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J26" s="120" t="str">
+      <c r="J26" s="150" t="str">
         <f>IF('Drug Information'!K25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K26" s="120" t="str">
+      <c r="K26" s="150" t="str">
         <f>IF('Drug Information'!L25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L26" s="120" t="str">
+      <c r="L26" s="150" t="str">
         <f>IF('Drug Information'!M25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M26" s="120" t="str">
+      <c r="M26" s="150" t="str">
         <f>IF('Drug Information'!N25=1,"",".")</f>
         <v/>
       </c>
-      <c r="N26" s="120" t="str">
+      <c r="N26" s="150" t="str">
         <f>IF('Drug Information'!O25=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="121" t="s">
+    <row r="27" spans="1:14" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="121"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="121"/>
-      <c r="K27" s="121"/>
-      <c r="L27" s="121"/>
-      <c r="M27" s="121"/>
-      <c r="N27" s="121"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="132"/>
+      <c r="G27" s="132"/>
+      <c r="H27" s="132"/>
+      <c r="I27" s="132"/>
+      <c r="J27" s="132"/>
+      <c r="K27" s="132"/>
+      <c r="L27" s="132"/>
+      <c r="M27" s="132"/>
+      <c r="N27" s="132"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="94"/>
-      <c r="B28" s="126"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="95"/>
       <c r="D28" s="95"/>
       <c r="E28" s="95"/>
@@ -4849,7 +4878,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
-      <c r="B29" s="126"/>
+      <c r="B29" s="106"/>
       <c r="C29" s="95"/>
       <c r="D29" s="95"/>
       <c r="E29" s="95"/>
@@ -4865,7 +4894,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
-      <c r="B30" s="126"/>
+      <c r="B30" s="106"/>
       <c r="C30" s="95"/>
       <c r="D30" s="95"/>
       <c r="E30" s="95"/>
@@ -4881,7 +4910,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
-      <c r="B31" s="126"/>
+      <c r="B31" s="106"/>
       <c r="C31" s="95"/>
       <c r="D31" s="95"/>
       <c r="E31" s="95"/>
@@ -4897,7 +4926,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
-      <c r="B32" s="126"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="95"/>
       <c r="D32" s="95"/>
       <c r="E32" s="95"/>
@@ -4913,7 +4942,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
-      <c r="B33" s="126"/>
+      <c r="B33" s="106"/>
       <c r="C33" s="95"/>
       <c r="D33" s="95"/>
       <c r="E33" s="95"/>
@@ -4929,7 +4958,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="94"/>
-      <c r="B34" s="126"/>
+      <c r="B34" s="106"/>
       <c r="C34" s="95"/>
       <c r="D34" s="95"/>
       <c r="E34" s="95"/>
@@ -4945,7 +4974,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="94"/>
-      <c r="B35" s="126"/>
+      <c r="B35" s="106"/>
       <c r="C35" s="95"/>
       <c r="D35" s="95"/>
       <c r="E35" s="95"/>
@@ -4961,7 +4990,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="94"/>
-      <c r="B36" s="126"/>
+      <c r="B36" s="106"/>
       <c r="C36" s="95"/>
       <c r="D36" s="95"/>
       <c r="E36" s="95"/>
@@ -4976,7 +5005,9 @@
       <c r="N36" s="95"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A27:N27"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A17:A19"/>
@@ -4988,7 +5019,7 @@
     <mergeCell ref="M1:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N26">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Darker grey for the cephalosporins
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8576EF-2403-4A8F-B61B-9956DECF3D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C08D4C7-82A4-4B70-B834-AD2D6C440A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +480,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,9 +812,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -848,9 +851,6 @@
     <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1106,15 +1106,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1131,6 +1122,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1793,7 +1799,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1894,7 @@
       <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="134" t="str">
+      <c r="A3" s="132" t="str">
         <f>IF(Antibiogram!A4=0,A2,Antibiogram!A4)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
@@ -1914,7 +1920,7 @@
       <c r="O3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="str">
+      <c r="A4" s="132" t="str">
         <f>IF(Antibiogram!A5=0,A3,Antibiogram!A5)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
@@ -1966,7 +1972,7 @@
       <c r="O5" s="32"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="134" t="str">
+      <c r="A6" s="132" t="str">
         <f>IF(Antibiogram!A7=0,A5,Antibiogram!A7)</f>
         <v>Aminopenicillins</v>
       </c>
@@ -2025,15 +2031,17 @@
       <c r="N7" s="32"/>
       <c r="O7" s="32"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="str">
-        <f>IF(Antibiogram!A9=0,A7,Antibiogram!A9)</f>
+        <f>IF(Antibiogram!A12=0,A7,Antibiogram!A12)</f>
         <v>1st-gen cephalosporin</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="32"/>
+        <v>53</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>50</v>
+      </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32">
         <v>1</v>
@@ -2054,18 +2062,22 @@
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
+      <c r="N8" s="32">
+        <v>1</v>
+      </c>
       <c r="O8" s="32"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="134" t="str">
-        <f>IF(Antibiogram!A10=0,A8,Antibiogram!A10)</f>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="str">
+        <f>IF(Antibiogram!A13=0,A8,Antibiogram!A13)</f>
         <v>1st-gen cephalosporin</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="32"/>
+        <v>54</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>51</v>
+      </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32">
         <v>1</v>
@@ -2086,18 +2098,22 @@
       <c r="K9" s="32"/>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="N9" s="32">
+        <v>1</v>
+      </c>
       <c r="O9" s="32"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="134" t="str">
-        <f>IF(Antibiogram!A11=0,A9,Antibiogram!A11)</f>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="str">
+        <f>IF(Antibiogram!A14=0,A9,Antibiogram!A14)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="32"/>
+        <v>55</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>52</v>
+      </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32">
         <v>1</v>
@@ -2114,10 +2130,16 @@
       <c r="I10" s="32">
         <v>1</v>
       </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
+      <c r="J10" s="32">
+        <v>1</v>
+      </c>
+      <c r="K10" s="32">
+        <v>1</v>
+      </c>
       <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
       <c r="N10" s="32">
         <v>1</v>
       </c>
@@ -2125,11 +2147,11 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="str">
-        <f>IF(Antibiogram!A12=0,A10,Antibiogram!A12)</f>
+        <f>IF(Antibiogram!A15=0,A10,Antibiogram!A15)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -2152,18 +2174,16 @@
       <c r="K11" s="32"/>
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
-      <c r="N11" s="32">
-        <v>1</v>
-      </c>
+      <c r="N11" s="32"/>
       <c r="O11" s="32"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="str">
-        <f>IF(Antibiogram!A13=0,A11,Antibiogram!A13)</f>
+      <c r="A12" s="132" t="str">
+        <f>IF(Antibiogram!A16=0,A11,Antibiogram!A16)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -2183,29 +2203,25 @@
         <v>1</v>
       </c>
       <c r="J12" s="32"/>
-      <c r="K12" s="32">
-        <v>1</v>
-      </c>
-      <c r="L12" s="32">
-        <v>1</v>
-      </c>
-      <c r="M12" s="32">
-        <v>1</v>
-      </c>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="str">
-        <f>IF(Antibiogram!A14=0,A12,Antibiogram!A14)</f>
+      <c r="A13" s="132" t="str">
+        <f>IF(Antibiogram!A17=0,A12,Antibiogram!A17)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
+      <c r="E13" s="32">
+        <v>1</v>
+      </c>
       <c r="F13" s="32">
         <v>1</v>
       </c>
@@ -2218,22 +2234,22 @@
       <c r="I13" s="32">
         <v>1</v>
       </c>
-      <c r="J13" s="32">
-        <v>1</v>
-      </c>
+      <c r="J13" s="32"/>
       <c r="K13" s="32"/>
       <c r="L13" s="32"/>
       <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="N13" s="32">
+        <v>1</v>
+      </c>
       <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="str">
-        <f>IF(Antibiogram!A15=0,A13,Antibiogram!A15)</f>
+        <f>IF(Antibiogram!A18=0,A13,Antibiogram!A18)</f>
         <v>4th-gen cephalosporin</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -2252,32 +2268,24 @@
       <c r="I14" s="32">
         <v>1</v>
       </c>
-      <c r="J14" s="32">
-        <v>1</v>
-      </c>
-      <c r="K14" s="32">
-        <v>1</v>
-      </c>
-      <c r="L14" s="32">
-        <v>1</v>
-      </c>
-      <c r="M14" s="32">
-        <v>1</v>
-      </c>
-      <c r="N14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32">
+        <v>1</v>
+      </c>
       <c r="O14" s="32"/>
     </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="str">
-        <f>IF(Antibiogram!A16=0,A14,Antibiogram!A16)</f>
+        <f>IF(Antibiogram!A9=0,A14,Antibiogram!A9)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>50</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C15" s="32"/>
       <c r="D15" s="32"/>
       <c r="E15" s="32">
         <v>1</v>
@@ -2295,29 +2303,29 @@
         <v>1</v>
       </c>
       <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32">
-        <v>1</v>
-      </c>
+      <c r="K15" s="32">
+        <v>1</v>
+      </c>
+      <c r="L15" s="32">
+        <v>1</v>
+      </c>
+      <c r="M15" s="32">
+        <v>1</v>
+      </c>
+      <c r="N15" s="32"/>
       <c r="O15" s="32"/>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="str">
-        <f>IF(Antibiogram!A17=0,A15,Antibiogram!A17)</f>
+        <f>IF(Antibiogram!A10=0,A15,Antibiogram!A10)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>51</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C16" s="32"/>
       <c r="D16" s="32"/>
-      <c r="E16" s="32">
-        <v>1</v>
-      </c>
+      <c r="E16" s="32"/>
       <c r="F16" s="32">
         <v>1</v>
       </c>
@@ -2330,26 +2338,24 @@
       <c r="I16" s="32">
         <v>1</v>
       </c>
-      <c r="J16" s="32"/>
+      <c r="J16" s="32">
+        <v>1</v>
+      </c>
       <c r="K16" s="32"/>
       <c r="L16" s="32"/>
       <c r="M16" s="32"/>
-      <c r="N16" s="32">
-        <v>1</v>
-      </c>
+      <c r="N16" s="32"/>
       <c r="O16" s="32"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="str">
-        <f>IF(Antibiogram!A18=0,A16,Antibiogram!A18)</f>
+        <f>IF(Antibiogram!A11=0,A16,Antibiogram!A11)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>52</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C17" s="32"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32">
         <v>1</v>
@@ -2372,13 +2378,13 @@
       <c r="K17" s="32">
         <v>1</v>
       </c>
-      <c r="L17" s="32"/>
+      <c r="L17" s="32">
+        <v>1</v>
+      </c>
       <c r="M17" s="32">
         <v>1</v>
       </c>
-      <c r="N17" s="32">
-        <v>1</v>
-      </c>
+      <c r="N17" s="32"/>
       <c r="O17" s="32"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2422,7 +2428,7 @@
       <c r="O18" s="32"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="134" t="str">
+      <c r="A19" s="132" t="str">
         <f>IF(Antibiogram!A20=0,A18,Antibiogram!A20)</f>
         <v>Carbapenems</v>
       </c>
@@ -2664,7 +2670,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="134" t="str">
+      <c r="A25" s="132" t="str">
         <f>IF(Antibiogram!A26=0,A24,Antibiogram!A26)</f>
         <v>Aminoglycosides</v>
       </c>
@@ -2696,7 +2702,7 @@
       <c r="O25" s="32"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="134" t="str">
+      <c r="A26" s="132" t="str">
         <f>IF(Antibiogram!A27=0,A25,Antibiogram!A27)</f>
         <v>Aminoglycosides</v>
       </c>
@@ -2963,7 +2969,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D30" sqref="D30"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2990,29 +2996,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="131" t="s">
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="132" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="132"/>
-      <c r="M1" s="133" t="s">
+      <c r="L1" s="130"/>
+      <c r="M1" s="131" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="35" t="s">
@@ -3020,8 +3026,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
-      <c r="B2" s="128"/>
+      <c r="A2" s="134"/>
+      <c r="B2" s="126"/>
       <c r="C2" s="36" t="s">
         <v>1</v>
       </c>
@@ -3052,1824 +3058,1815 @@
       <c r="L2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="133"/>
+      <c r="M2" s="131"/>
       <c r="N2" s="39" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="53" t="str">
+      <c r="B3" s="52" t="str">
         <f>'Drug Information'!$B2</f>
         <v>Benzylpenicillin</v>
       </c>
-      <c r="C3" s="54" t="str">
+      <c r="C3" s="53" t="str">
         <f>IF('Drug Information'!D2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D3" s="54" t="str">
+      <c r="D3" s="53" t="str">
         <f>IF('Drug Information'!E2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E3" s="54" t="str">
+      <c r="E3" s="53" t="str">
         <f>IF('Drug Information'!F2=1,"",".")</f>
         <v/>
       </c>
-      <c r="F3" s="54" t="str">
+      <c r="F3" s="53" t="str">
         <f>IF('Drug Information'!G2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G3" s="54" t="str">
+      <c r="G3" s="53" t="str">
         <f>IF('Drug Information'!H2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H3" s="54" t="str">
+      <c r="H3" s="53" t="str">
         <f>IF('Drug Information'!I2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I3" s="54" t="str">
+      <c r="I3" s="53" t="str">
         <f>IF('Drug Information'!J2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J3" s="54" t="str">
+      <c r="J3" s="53" t="str">
         <f>IF('Drug Information'!K2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K3" s="54" t="str">
+      <c r="K3" s="53" t="str">
         <f>IF('Drug Information'!L2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L3" s="54" t="str">
+      <c r="L3" s="53" t="str">
         <f>IF('Drug Information'!M2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M3" s="54" t="str">
+      <c r="M3" s="53" t="str">
         <f>IF('Drug Information'!N2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N3" s="54" t="str">
+      <c r="N3" s="53" t="str">
         <f>IF('Drug Information'!O2=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="53" t="str">
+      <c r="B4" s="52" t="str">
         <f>'Drug Information'!$B3</f>
         <v>Naficillin</v>
       </c>
-      <c r="C4" s="54" t="str">
+      <c r="C4" s="53" t="str">
         <f>IF('Drug Information'!D3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D4" s="54" t="str">
+      <c r="D4" s="53" t="str">
         <f>IF('Drug Information'!E3=1,"",".")</f>
         <v/>
       </c>
-      <c r="E4" s="54" t="str">
+      <c r="E4" s="53" t="str">
         <f>IF('Drug Information'!F3=1,"",".")</f>
         <v/>
       </c>
-      <c r="F4" s="54" t="str">
+      <c r="F4" s="53" t="str">
         <f>IF('Drug Information'!G3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G4" s="54" t="str">
+      <c r="G4" s="53" t="str">
         <f>IF('Drug Information'!H3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H4" s="54" t="str">
+      <c r="H4" s="53" t="str">
         <f>IF('Drug Information'!I3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I4" s="54" t="str">
+      <c r="I4" s="53" t="str">
         <f>IF('Drug Information'!J3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J4" s="54" t="str">
+      <c r="J4" s="53" t="str">
         <f>IF('Drug Information'!K3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K4" s="54" t="str">
+      <c r="K4" s="53" t="str">
         <f>IF('Drug Information'!L3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L4" s="54" t="str">
+      <c r="L4" s="53" t="str">
         <f>IF('Drug Information'!M3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M4" s="54" t="str">
+      <c r="M4" s="53" t="str">
         <f>IF('Drug Information'!N3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N4" s="54" t="str">
+      <c r="N4" s="53" t="str">
         <f>IF('Drug Information'!O3=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="53" t="str">
+      <c r="A5" s="137"/>
+      <c r="B5" s="52" t="str">
         <f>'Drug Information'!$B4</f>
         <v>Oxacillin</v>
       </c>
-      <c r="C5" s="54" t="str">
+      <c r="C5" s="53" t="str">
         <f>IF('Drug Information'!D4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D5" s="54" t="str">
+      <c r="D5" s="53" t="str">
         <f>IF('Drug Information'!E4=1,"",".")</f>
         <v/>
       </c>
-      <c r="E5" s="54" t="str">
+      <c r="E5" s="53" t="str">
         <f>IF('Drug Information'!F4=1,"",".")</f>
         <v/>
       </c>
-      <c r="F5" s="54" t="str">
+      <c r="F5" s="53" t="str">
         <f>IF('Drug Information'!G4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G5" s="54" t="str">
+      <c r="G5" s="53" t="str">
         <f>IF('Drug Information'!H4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H5" s="54" t="str">
+      <c r="H5" s="53" t="str">
         <f>IF('Drug Information'!I4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I5" s="54" t="str">
+      <c r="I5" s="53" t="str">
         <f>IF('Drug Information'!J4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J5" s="54" t="str">
+      <c r="J5" s="53" t="str">
         <f>IF('Drug Information'!K4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K5" s="54" t="str">
+      <c r="K5" s="53" t="str">
         <f>IF('Drug Information'!L4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L5" s="54" t="str">
+      <c r="L5" s="53" t="str">
         <f>IF('Drug Information'!M4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M5" s="54" t="str">
+      <c r="M5" s="53" t="str">
         <f>IF('Drug Information'!N4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N5" s="54" t="str">
+      <c r="N5" s="53" t="str">
         <f>IF('Drug Information'!O4=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140"/>
-      <c r="B6" s="53" t="str">
+      <c r="A6" s="138"/>
+      <c r="B6" s="52" t="str">
         <f>'Drug Information'!$B5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="C6" s="54" t="str">
+      <c r="C6" s="53" t="str">
         <f>IF('Drug Information'!D5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D6" s="54" t="str">
+      <c r="D6" s="53" t="str">
         <f>IF('Drug Information'!E5=1,"",".")</f>
         <v/>
       </c>
-      <c r="E6" s="54" t="str">
+      <c r="E6" s="53" t="str">
         <f>IF('Drug Information'!F5=1,"",".")</f>
         <v/>
       </c>
-      <c r="F6" s="54" t="str">
+      <c r="F6" s="53" t="str">
         <f>IF('Drug Information'!G5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G6" s="54" t="str">
+      <c r="G6" s="53" t="str">
         <f>IF('Drug Information'!H5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H6" s="54" t="str">
+      <c r="H6" s="53" t="str">
         <f>IF('Drug Information'!I5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I6" s="54" t="str">
+      <c r="I6" s="53" t="str">
         <f>IF('Drug Information'!J5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J6" s="54" t="str">
+      <c r="J6" s="53" t="str">
         <f>IF('Drug Information'!K5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K6" s="54" t="str">
+      <c r="K6" s="53" t="str">
         <f>IF('Drug Information'!L5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L6" s="54" t="str">
+      <c r="L6" s="53" t="str">
         <f>IF('Drug Information'!M5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M6" s="54" t="str">
+      <c r="M6" s="53" t="str">
         <f>IF('Drug Information'!N5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N6" s="54" t="str">
+      <c r="N6" s="53" t="str">
         <f>IF('Drug Information'!O5=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="53" t="str">
+      <c r="B7" s="52" t="str">
         <f>'Drug Information'!$B6</f>
         <v>Ampicillin</v>
       </c>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="53" t="str">
         <f>IF('Drug Information'!D6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D7" s="54" t="str">
+      <c r="D7" s="53" t="str">
         <f>IF('Drug Information'!E6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E7" s="54" t="str">
+      <c r="E7" s="53" t="str">
         <f>IF('Drug Information'!F6=1,"",".")</f>
         <v/>
       </c>
-      <c r="F7" s="54" t="str">
+      <c r="F7" s="53" t="str">
         <f>IF('Drug Information'!G6=1,"",".")</f>
         <v/>
       </c>
-      <c r="G7" s="54" t="str">
+      <c r="G7" s="53" t="str">
         <f>IF('Drug Information'!H6=1,"",".")</f>
         <v/>
       </c>
-      <c r="H7" s="54" t="str">
+      <c r="H7" s="53" t="str">
         <f>IF('Drug Information'!I6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I7" s="54" t="str">
+      <c r="I7" s="53" t="str">
         <f>IF('Drug Information'!J6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J7" s="54" t="str">
+      <c r="J7" s="53" t="str">
         <f>IF('Drug Information'!K6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K7" s="54" t="str">
+      <c r="K7" s="53" t="str">
         <f>IF('Drug Information'!L6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L7" s="54" t="str">
+      <c r="L7" s="53" t="str">
         <f>IF('Drug Information'!M6=1,"",".")</f>
         <v/>
       </c>
-      <c r="M7" s="54" t="str">
+      <c r="M7" s="53" t="str">
         <f>IF('Drug Information'!N6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N7" s="54" t="str">
+      <c r="N7" s="53" t="str">
         <f>IF('Drug Information'!O6=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="53" t="str">
+      <c r="A8" s="138"/>
+      <c r="B8" s="52" t="str">
         <f>'Drug Information'!$B7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="C8" s="54" t="str">
+      <c r="C8" s="53" t="str">
         <f>IF('Drug Information'!D7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D8" s="54" t="str">
+      <c r="D8" s="53" t="str">
         <f>IF('Drug Information'!E7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E8" s="54" t="str">
+      <c r="E8" s="53" t="str">
         <f>IF('Drug Information'!F7=1,"",".")</f>
         <v/>
       </c>
-      <c r="F8" s="54" t="str">
+      <c r="F8" s="53" t="str">
         <f>IF('Drug Information'!G7=1,"",".")</f>
         <v/>
       </c>
-      <c r="G8" s="54" t="str">
+      <c r="G8" s="53" t="str">
         <f>IF('Drug Information'!H7=1,"",".")</f>
         <v/>
       </c>
-      <c r="H8" s="54" t="str">
+      <c r="H8" s="53" t="str">
         <f>IF('Drug Information'!I7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I8" s="54" t="str">
+      <c r="I8" s="53" t="str">
         <f>IF('Drug Information'!J7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J8" s="54" t="str">
+      <c r="J8" s="53" t="str">
         <f>IF('Drug Information'!K7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K8" s="54" t="str">
+      <c r="K8" s="53" t="str">
         <f>IF('Drug Information'!L7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L8" s="54" t="str">
+      <c r="L8" s="53" t="str">
         <f>IF('Drug Information'!M7=1,"",".")</f>
         <v/>
       </c>
-      <c r="M8" s="54" t="str">
+      <c r="M8" s="53" t="str">
         <f>IF('Drug Information'!N7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N8" s="54" t="str">
+      <c r="N8" s="53" t="str">
         <f>IF('Drug Information'!O7=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="141" t="s">
-        <v>30</v>
+      <c r="A9" s="139" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="41" t="str">
         <f>'Drug Information'!$B8</f>
-        <v>Cefazolin</v>
-      </c>
-      <c r="C9" s="55" t="str">
+        <v>Amoxicillin-Clavulanic Acid</v>
+      </c>
+      <c r="C9" s="54" t="str">
         <f>IF('Drug Information'!D8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D9" s="55" t="str">
+      <c r="D9" s="54" t="str">
         <f>IF('Drug Information'!E8=1,"",".")</f>
         <v/>
       </c>
-      <c r="E9" s="55" t="str">
+      <c r="E9" s="54" t="str">
         <f>IF('Drug Information'!F8=1,"",".")</f>
         <v/>
       </c>
-      <c r="F9" s="55" t="str">
+      <c r="F9" s="54" t="str">
         <f>IF('Drug Information'!G8=1,"",".")</f>
         <v/>
       </c>
-      <c r="G9" s="55" t="str">
+      <c r="G9" s="54" t="str">
         <f>IF('Drug Information'!H8=1,"",".")</f>
         <v/>
       </c>
-      <c r="H9" s="55" t="str">
+      <c r="H9" s="54" t="str">
         <f>IF('Drug Information'!I8=1,"",".")</f>
         <v/>
       </c>
-      <c r="I9" s="55" t="str">
+      <c r="I9" s="54" t="str">
         <f>IF('Drug Information'!J8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J9" s="55" t="str">
+      <c r="J9" s="54" t="str">
         <f>IF('Drug Information'!K8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K9" s="55" t="str">
+      <c r="K9" s="54" t="str">
         <f>IF('Drug Information'!L8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L9" s="55" t="str">
+      <c r="L9" s="54" t="str">
         <f>IF('Drug Information'!M8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M9" s="55" t="str">
+      <c r="M9" s="54" t="str">
         <f>IF('Drug Information'!N8=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="N9" s="55" t="str">
-        <f>IF('Drug Information'!O8=1,"",".")</f>
-        <v>.</v>
-      </c>
+        <v/>
+      </c>
+      <c r="N9" s="54"/>
     </row>
     <row r="10" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="142"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="41" t="str">
         <f>'Drug Information'!$B9</f>
-        <v>Cefalexin</v>
-      </c>
-      <c r="C10" s="55" t="str">
+        <v>Ampicillin/Sulbactam</v>
+      </c>
+      <c r="C10" s="54" t="str">
         <f>IF('Drug Information'!D9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D10" s="55" t="str">
+      <c r="D10" s="54" t="str">
         <f>IF('Drug Information'!E9=1,"",".")</f>
         <v/>
       </c>
-      <c r="E10" s="55" t="str">
+      <c r="E10" s="54" t="str">
         <f>IF('Drug Information'!F9=1,"",".")</f>
         <v/>
       </c>
-      <c r="F10" s="55" t="str">
+      <c r="F10" s="54" t="str">
         <f>IF('Drug Information'!G9=1,"",".")</f>
         <v/>
       </c>
-      <c r="G10" s="55" t="str">
+      <c r="G10" s="54" t="str">
         <f>IF('Drug Information'!H9=1,"",".")</f>
         <v/>
       </c>
-      <c r="H10" s="55" t="str">
+      <c r="H10" s="54" t="str">
         <f>IF('Drug Information'!I9=1,"",".")</f>
         <v/>
       </c>
-      <c r="I10" s="55" t="str">
+      <c r="I10" s="54" t="str">
         <f>IF('Drug Information'!J9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J10" s="55" t="str">
+      <c r="J10" s="54" t="str">
         <f>IF('Drug Information'!K9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K10" s="55" t="str">
+      <c r="K10" s="54" t="str">
         <f>IF('Drug Information'!L9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L10" s="55" t="str">
+      <c r="L10" s="54" t="str">
         <f>IF('Drug Information'!M9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M10" s="55" t="str">
+      <c r="M10" s="54" t="str">
         <f>IF('Drug Information'!N9=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="N10" s="55" t="str">
-        <f>IF('Drug Information'!O9=1,"",".")</f>
-        <v>.</v>
-      </c>
+        <v/>
+      </c>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="141" t="s">
-        <v>31</v>
-      </c>
+      <c r="A11" s="139"/>
       <c r="B11" s="41" t="str">
         <f>'Drug Information'!$B10</f>
+        <v>Piperacillin-Tazobactam</v>
+      </c>
+      <c r="C11" s="54" t="str">
+        <f>IF('Drug Information'!D10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D11" s="54" t="str">
+        <f>IF('Drug Information'!E10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E11" s="54" t="str">
+        <f>IF('Drug Information'!F10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F11" s="54" t="str">
+        <f>IF('Drug Information'!G10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G11" s="54" t="str">
+        <f>IF('Drug Information'!H10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H11" s="54" t="str">
+        <f>IF('Drug Information'!I10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I11" s="54" t="str">
+        <f>IF('Drug Information'!J10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J11" s="54" t="str">
+        <f>IF('Drug Information'!K10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K11" s="54" t="str">
+        <f>IF('Drug Information'!L10=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L11" s="54" t="str">
+        <f>IF('Drug Information'!M10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M11" s="54" t="str">
+        <f>IF('Drug Information'!N10=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="145" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="146" t="str">
+        <f>'Drug Information'!$B11</f>
+        <v>Cefazolin</v>
+      </c>
+      <c r="C12" s="147" t="str">
+        <f>IF('Drug Information'!D11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D12" s="147" t="str">
+        <f>IF('Drug Information'!E11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E12" s="147" t="str">
+        <f>IF('Drug Information'!F11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F12" s="147" t="str">
+        <f>IF('Drug Information'!G11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G12" s="147" t="str">
+        <f>IF('Drug Information'!H11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H12" s="147" t="str">
+        <f>IF('Drug Information'!I11=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I12" s="147" t="str">
+        <f>IF('Drug Information'!J11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J12" s="147" t="str">
+        <f>IF('Drug Information'!K11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K12" s="147" t="str">
+        <f>IF('Drug Information'!L11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L12" s="147" t="str">
+        <f>IF('Drug Information'!M11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M12" s="147" t="str">
+        <f>IF('Drug Information'!N11=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N12" s="147" t="str">
+        <f>IF('Drug Information'!O11=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="148"/>
+      <c r="B13" s="146" t="str">
+        <f>'Drug Information'!$B12</f>
+        <v>Cefalexin</v>
+      </c>
+      <c r="C13" s="147" t="str">
+        <f>IF('Drug Information'!D12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D13" s="147" t="str">
+        <f>IF('Drug Information'!E12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E13" s="147" t="str">
+        <f>IF('Drug Information'!F12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F13" s="147" t="str">
+        <f>IF('Drug Information'!G12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G13" s="147" t="str">
+        <f>IF('Drug Information'!H12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H13" s="147" t="str">
+        <f>IF('Drug Information'!I12=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I13" s="147" t="str">
+        <f>IF('Drug Information'!J12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J13" s="147" t="str">
+        <f>IF('Drug Information'!K12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K13" s="147" t="str">
+        <f>IF('Drug Information'!L12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L13" s="147" t="str">
+        <f>IF('Drug Information'!M12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M13" s="147" t="str">
+        <f>IF('Drug Information'!N12=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N13" s="147" t="str">
+        <f>IF('Drug Information'!O12=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="145" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="146" t="str">
+        <f>'Drug Information'!$B13</f>
         <v>Cephotetan</v>
       </c>
-      <c r="C11" s="55" t="str">
-        <f>IF('Drug Information'!D10=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D11" s="55" t="str">
-        <f>IF('Drug Information'!E10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E11" s="55" t="str">
-        <f>IF('Drug Information'!F10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F11" s="55" t="str">
-        <f>IF('Drug Information'!G10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G11" s="55" t="str">
-        <f>IF('Drug Information'!H10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H11" s="55" t="str">
-        <f>IF('Drug Information'!I10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I11" s="55" t="str">
-        <f>IF('Drug Information'!J10=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="J11" s="55" t="str">
-        <f>IF('Drug Information'!K10=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="K11" s="55" t="str">
-        <f>IF('Drug Information'!L10=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L11" s="55" t="str">
-        <f>IF('Drug Information'!M10=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="M11" s="55" t="str">
-        <f>IF('Drug Information'!N10=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="N11" s="55" t="str">
-        <f>IF('Drug Information'!O10=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="142"/>
-      <c r="B12" s="41" t="str">
-        <f>'Drug Information'!$B11</f>
+      <c r="C14" s="147" t="str">
+        <f>IF('Drug Information'!D13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D14" s="147" t="str">
+        <f>IF('Drug Information'!E13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E14" s="147" t="str">
+        <f>IF('Drug Information'!F13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F14" s="147" t="str">
+        <f>IF('Drug Information'!G13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G14" s="147" t="str">
+        <f>IF('Drug Information'!H13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H14" s="147" t="str">
+        <f>IF('Drug Information'!I13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I14" s="147" t="str">
+        <f>IF('Drug Information'!J13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J14" s="147" t="str">
+        <f>IF('Drug Information'!K13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K14" s="147" t="str">
+        <f>IF('Drug Information'!L13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L14" s="147" t="str">
+        <f>IF('Drug Information'!M13=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M14" s="147" t="str">
+        <f>IF('Drug Information'!N13=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N14" s="147" t="str">
+        <f>IF('Drug Information'!O13=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="148"/>
+      <c r="B15" s="146" t="str">
+        <f>'Drug Information'!$B14</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="C12" s="55" t="str">
-        <f>IF('Drug Information'!D11=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D12" s="55" t="str">
-        <f>IF('Drug Information'!E11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E12" s="55" t="str">
-        <f>IF('Drug Information'!F11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F12" s="55" t="str">
-        <f>IF('Drug Information'!G11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G12" s="55" t="str">
-        <f>IF('Drug Information'!H11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H12" s="55" t="str">
-        <f>IF('Drug Information'!I11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I12" s="55" t="str">
-        <f>IF('Drug Information'!J11=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="J12" s="55" t="str">
-        <f>IF('Drug Information'!K11=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="K12" s="55" t="str">
-        <f>IF('Drug Information'!L11=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L12" s="55" t="str">
-        <f>IF('Drug Information'!M11=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="M12" s="55" t="str">
-        <f>IF('Drug Information'!N11=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="N12" s="55" t="str">
-        <f>IF('Drug Information'!O11=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="143" t="s">
+      <c r="C15" s="147" t="str">
+        <f>IF('Drug Information'!D14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D15" s="147" t="str">
+        <f>IF('Drug Information'!E14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E15" s="147" t="str">
+        <f>IF('Drug Information'!F14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F15" s="147" t="str">
+        <f>IF('Drug Information'!G14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G15" s="147" t="str">
+        <f>IF('Drug Information'!H14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H15" s="147" t="str">
+        <f>IF('Drug Information'!I14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I15" s="147" t="str">
+        <f>IF('Drug Information'!J14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J15" s="147" t="str">
+        <f>IF('Drug Information'!K14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K15" s="147" t="str">
+        <f>IF('Drug Information'!L14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L15" s="147" t="str">
+        <f>IF('Drug Information'!M14=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M15" s="147" t="str">
+        <f>IF('Drug Information'!N14=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="N15" s="147" t="str">
+        <f>IF('Drug Information'!O14=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="41" t="str">
-        <f>'Drug Information'!$B12</f>
+      <c r="B16" s="146" t="str">
+        <f>'Drug Information'!$B15</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="C13" s="55" t="str">
-        <f>IF('Drug Information'!D12=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D13" s="55" t="str">
-        <f>IF('Drug Information'!E12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E13" s="55" t="str">
-        <f>IF('Drug Information'!F12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F13" s="55" t="str">
-        <f>IF('Drug Information'!G12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G13" s="55" t="str">
-        <f>IF('Drug Information'!H12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H13" s="55" t="str">
-        <f>IF('Drug Information'!I12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I13" s="55" t="str">
-        <f>IF('Drug Information'!J12=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="J13" s="55" t="str">
-        <f>IF('Drug Information'!K12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="K13" s="55" t="str">
-        <f>IF('Drug Information'!L12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="L13" s="55" t="str">
-        <f>IF('Drug Information'!M12=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="M13" s="55" t="str">
-        <f>IF('Drug Information'!N12=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="N13" s="55" t="str">
-        <f>IF('Drug Information'!O12=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="41" t="str">
-        <f>'Drug Information'!$B13</f>
+      <c r="C16" s="147" t="str">
+        <f>IF('Drug Information'!D15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D16" s="147" t="str">
+        <f>IF('Drug Information'!E15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="E16" s="147" t="str">
+        <f>IF('Drug Information'!F15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F16" s="147" t="str">
+        <f>IF('Drug Information'!G15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G16" s="147" t="str">
+        <f>IF('Drug Information'!H15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H16" s="147" t="str">
+        <f>IF('Drug Information'!I15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I16" s="147" t="str">
+        <f>IF('Drug Information'!J15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="J16" s="147" t="str">
+        <f>IF('Drug Information'!K15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="K16" s="147" t="str">
+        <f>IF('Drug Information'!L15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="L16" s="147" t="str">
+        <f>IF('Drug Information'!M15=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="M16" s="147" t="str">
+        <f>IF('Drug Information'!N15=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N16" s="147" t="str">
+        <f>IF('Drug Information'!O15=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="149"/>
+      <c r="B17" s="146" t="str">
+        <f>'Drug Information'!$B16</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="C14" s="55" t="str">
-        <f>IF('Drug Information'!D13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D14" s="55" t="str">
-        <f>IF('Drug Information'!E13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="E14" s="55" t="str">
-        <f>IF('Drug Information'!F13=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F14" s="55" t="str">
-        <f>IF('Drug Information'!G13=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G14" s="55" t="str">
-        <f>IF('Drug Information'!H13=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H14" s="55" t="str">
-        <f>IF('Drug Information'!I13=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I14" s="55" t="str">
-        <f>IF('Drug Information'!J13=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="J14" s="55" t="str">
-        <f>IF('Drug Information'!K13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="K14" s="55" t="str">
-        <f>IF('Drug Information'!L13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L14" s="55" t="str">
-        <f>IF('Drug Information'!M13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="M14" s="55" t="str">
-        <f>IF('Drug Information'!N13=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="N14" s="55" t="str">
-        <f>IF('Drug Information'!O13=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="C17" s="147" t="str">
+        <f>IF('Drug Information'!D16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="D17" s="147" t="str">
+        <f>IF('Drug Information'!E16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="E17" s="147" t="str">
+        <f>IF('Drug Information'!F16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="F17" s="147" t="str">
+        <f>IF('Drug Information'!G16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="G17" s="147" t="str">
+        <f>IF('Drug Information'!H16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="H17" s="147" t="str">
+        <f>IF('Drug Information'!I16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="I17" s="147" t="str">
+        <f>IF('Drug Information'!J16=1,"",".")</f>
+        <v/>
+      </c>
+      <c r="J17" s="147" t="str">
+        <f>IF('Drug Information'!K16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="K17" s="147" t="str">
+        <f>IF('Drug Information'!L16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="L17" s="147" t="str">
+        <f>IF('Drug Information'!M16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="M17" s="147" t="str">
+        <f>IF('Drug Information'!N16=1,"",".")</f>
+        <v>.</v>
+      </c>
+      <c r="N17" s="147" t="str">
+        <f>IF('Drug Information'!O16=1,"",".")</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="41" t="str">
-        <f>'Drug Information'!$B14</f>
+      <c r="B18" s="146" t="str">
+        <f>'Drug Information'!$B17</f>
         <v>Cefepime</v>
       </c>
-      <c r="C15" s="55" t="str">
-        <f>IF('Drug Information'!D14=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D15" s="55" t="str">
-        <f>IF('Drug Information'!E14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E15" s="55" t="str">
-        <f>IF('Drug Information'!F14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F15" s="55" t="str">
-        <f>IF('Drug Information'!G14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G15" s="55" t="str">
-        <f>IF('Drug Information'!H14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H15" s="55" t="str">
-        <f>IF('Drug Information'!I14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I15" s="55" t="str">
-        <f>IF('Drug Information'!J14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="J15" s="55" t="str">
-        <f>IF('Drug Information'!K14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="K15" s="55" t="str">
-        <f>IF('Drug Information'!L14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="L15" s="55" t="str">
-        <f>IF('Drug Information'!M14=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="M15" s="55" t="str">
-        <f>IF('Drug Information'!N14=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="N15" s="55" t="str">
-        <f>IF('Drug Information'!O14=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="144" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="42" t="str">
-        <f>'Drug Information'!$B15</f>
-        <v>Amoxicillin-Clavulanic Acid</v>
-      </c>
-      <c r="C16" s="56" t="str">
-        <f>IF('Drug Information'!D15=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D16" s="56" t="str">
-        <f>IF('Drug Information'!E15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E16" s="56" t="str">
-        <f>IF('Drug Information'!F15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F16" s="56" t="str">
-        <f>IF('Drug Information'!G15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G16" s="56" t="str">
-        <f>IF('Drug Information'!H15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H16" s="56" t="str">
-        <f>IF('Drug Information'!I15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I16" s="56" t="str">
-        <f>IF('Drug Information'!J15=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="J16" s="56" t="str">
-        <f>IF('Drug Information'!K15=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="K16" s="56" t="str">
-        <f>IF('Drug Information'!L15=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L16" s="56" t="str">
-        <f>IF('Drug Information'!M15=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="M16" s="56" t="str">
-        <f>IF('Drug Information'!N15=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="N16" s="56" t="str">
-        <f>IF('Drug Information'!O15=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="144"/>
-      <c r="B17" s="42" t="str">
-        <f>'Drug Information'!$B16</f>
-        <v>Ampicillin/Sulbactam</v>
-      </c>
-      <c r="C17" s="56" t="str">
-        <f>IF('Drug Information'!D16=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="D17" s="56" t="str">
-        <f>IF('Drug Information'!E16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="E17" s="56" t="str">
-        <f>IF('Drug Information'!F16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="F17" s="56" t="str">
-        <f>IF('Drug Information'!G16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="G17" s="56" t="str">
-        <f>IF('Drug Information'!H16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="H17" s="56" t="str">
-        <f>IF('Drug Information'!I16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="I17" s="56" t="str">
-        <f>IF('Drug Information'!J16=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="J17" s="56" t="str">
-        <f>IF('Drug Information'!K16=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="K17" s="56" t="str">
-        <f>IF('Drug Information'!L16=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L17" s="56" t="str">
-        <f>IF('Drug Information'!M16=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="M17" s="56" t="str">
-        <f>IF('Drug Information'!N16=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="N17" s="56" t="str">
-        <f>IF('Drug Information'!O16=1,"",".")</f>
-        <v>.</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
-      <c r="B18" s="42" t="str">
-        <f>'Drug Information'!$B17</f>
-        <v>Piperacillin-Tazobactam</v>
-      </c>
-      <c r="C18" s="56" t="str">
+      <c r="C18" s="147" t="str">
         <f>IF('Drug Information'!D17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D18" s="56" t="str">
+      <c r="D18" s="147" t="str">
         <f>IF('Drug Information'!E17=1,"",".")</f>
         <v/>
       </c>
-      <c r="E18" s="56" t="str">
+      <c r="E18" s="147" t="str">
         <f>IF('Drug Information'!F17=1,"",".")</f>
         <v/>
       </c>
-      <c r="F18" s="56" t="str">
+      <c r="F18" s="147" t="str">
         <f>IF('Drug Information'!G17=1,"",".")</f>
         <v/>
       </c>
-      <c r="G18" s="56" t="str">
+      <c r="G18" s="147" t="str">
         <f>IF('Drug Information'!H17=1,"",".")</f>
         <v/>
       </c>
-      <c r="H18" s="56" t="str">
+      <c r="H18" s="147" t="str">
         <f>IF('Drug Information'!I17=1,"",".")</f>
         <v/>
       </c>
-      <c r="I18" s="56" t="str">
+      <c r="I18" s="147" t="str">
         <f>IF('Drug Information'!J17=1,"",".")</f>
         <v/>
       </c>
-      <c r="J18" s="56" t="str">
+      <c r="J18" s="147" t="str">
         <f>IF('Drug Information'!K17=1,"",".")</f>
         <v/>
       </c>
-      <c r="K18" s="56" t="str">
+      <c r="K18" s="147" t="str">
         <f>IF('Drug Information'!L17=1,"",".")</f>
-        <v>.</v>
-      </c>
-      <c r="L18" s="56" t="str">
+        <v/>
+      </c>
+      <c r="L18" s="147" t="str">
         <f>IF('Drug Information'!M17=1,"",".")</f>
         <v/>
       </c>
-      <c r="M18" s="56" t="str">
+      <c r="M18" s="147" t="str">
         <f>IF('Drug Information'!N17=1,"",".")</f>
-        <v/>
-      </c>
-      <c r="N18" s="56" t="str">
+        <v>.</v>
+      </c>
+      <c r="N18" s="147" t="str">
         <f>IF('Drug Information'!O17=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="145" t="s">
+      <c r="A19" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="43" t="str">
+      <c r="B19" s="42" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Ertapenem</v>
       </c>
-      <c r="C19" s="57" t="str">
+      <c r="C19" s="55" t="str">
         <f>IF('Drug Information'!D18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D19" s="57" t="str">
+      <c r="D19" s="55" t="str">
         <f>IF('Drug Information'!E18=1,"",".")</f>
         <v/>
       </c>
-      <c r="E19" s="57" t="str">
+      <c r="E19" s="55" t="str">
         <f>IF('Drug Information'!F18=1,"",".")</f>
         <v/>
       </c>
-      <c r="F19" s="57" t="str">
+      <c r="F19" s="55" t="str">
         <f>IF('Drug Information'!G18=1,"",".")</f>
         <v/>
       </c>
-      <c r="G19" s="57" t="str">
+      <c r="G19" s="55" t="str">
         <f>IF('Drug Information'!H18=1,"",".")</f>
         <v/>
       </c>
-      <c r="H19" s="57" t="str">
+      <c r="H19" s="55" t="str">
         <f>IF('Drug Information'!I18=1,"",".")</f>
         <v/>
       </c>
-      <c r="I19" s="57" t="str">
+      <c r="I19" s="55" t="str">
         <f>IF('Drug Information'!J18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J19" s="57" t="str">
+      <c r="J19" s="55" t="str">
         <f>IF('Drug Information'!K18=1,"",".")</f>
         <v/>
       </c>
-      <c r="K19" s="57" t="str">
+      <c r="K19" s="55" t="str">
         <f>IF('Drug Information'!L18=1,"",".")</f>
         <v/>
       </c>
-      <c r="L19" s="57" t="str">
+      <c r="L19" s="55" t="str">
         <f>IF('Drug Information'!M18=1,"",".")</f>
         <v/>
       </c>
-      <c r="M19" s="57" t="str">
+      <c r="M19" s="55" t="str">
         <f>IF('Drug Information'!N18=1,"",".")</f>
         <v/>
       </c>
-      <c r="N19" s="57" t="str">
+      <c r="N19" s="55" t="str">
         <f>IF('Drug Information'!O18=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="145"/>
-      <c r="B20" s="43" t="str">
+      <c r="A20" s="140"/>
+      <c r="B20" s="42" t="str">
         <f>'Drug Information'!$B19</f>
         <v>Imipenem</v>
       </c>
-      <c r="C20" s="57" t="str">
+      <c r="C20" s="55" t="str">
         <f>IF('Drug Information'!D19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D20" s="57" t="str">
+      <c r="D20" s="55" t="str">
         <f>IF('Drug Information'!E19=1,"",".")</f>
         <v/>
       </c>
-      <c r="E20" s="57" t="str">
+      <c r="E20" s="55" t="str">
         <f>IF('Drug Information'!F19=1,"",".")</f>
         <v/>
       </c>
-      <c r="F20" s="57" t="str">
+      <c r="F20" s="55" t="str">
         <f>IF('Drug Information'!G19=1,"",".")</f>
         <v/>
       </c>
-      <c r="G20" s="57" t="str">
+      <c r="G20" s="55" t="str">
         <f>IF('Drug Information'!H19=1,"",".")</f>
         <v/>
       </c>
-      <c r="H20" s="57" t="str">
+      <c r="H20" s="55" t="str">
         <f>IF('Drug Information'!I19=1,"",".")</f>
         <v/>
       </c>
-      <c r="I20" s="57" t="str">
+      <c r="I20" s="55" t="str">
         <f>IF('Drug Information'!J19=1,"",".")</f>
         <v/>
       </c>
-      <c r="J20" s="57" t="str">
+      <c r="J20" s="55" t="str">
         <f>IF('Drug Information'!K19=1,"",".")</f>
         <v/>
       </c>
-      <c r="K20" s="57" t="str">
+      <c r="K20" s="55" t="str">
         <f>IF('Drug Information'!L19=1,"",".")</f>
         <v/>
       </c>
-      <c r="L20" s="57" t="str">
+      <c r="L20" s="55" t="str">
         <f>IF('Drug Information'!M19=1,"",".")</f>
         <v/>
       </c>
-      <c r="M20" s="57" t="str">
+      <c r="M20" s="55" t="str">
         <f>IF('Drug Information'!N19=1,"",".")</f>
         <v/>
       </c>
-      <c r="N20" s="57" t="str">
+      <c r="N20" s="55" t="str">
         <f>IF('Drug Information'!O19=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="145"/>
-      <c r="B21" s="43" t="str">
+      <c r="A21" s="140"/>
+      <c r="B21" s="42" t="str">
         <f>'Drug Information'!$B20</f>
         <v>Meropenem</v>
       </c>
-      <c r="C21" s="57" t="str">
+      <c r="C21" s="55" t="str">
         <f>IF('Drug Information'!D20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D21" s="57" t="str">
+      <c r="D21" s="55" t="str">
         <f>IF('Drug Information'!E20=1,"",".")</f>
         <v/>
       </c>
-      <c r="E21" s="57" t="str">
+      <c r="E21" s="55" t="str">
         <f>IF('Drug Information'!F20=1,"",".")</f>
         <v/>
       </c>
-      <c r="F21" s="57" t="str">
+      <c r="F21" s="55" t="str">
         <f>IF('Drug Information'!G20=1,"",".")</f>
         <v/>
       </c>
-      <c r="G21" s="57" t="str">
+      <c r="G21" s="55" t="str">
         <f>IF('Drug Information'!H20=1,"",".")</f>
         <v/>
       </c>
-      <c r="H21" s="57" t="str">
+      <c r="H21" s="55" t="str">
         <f>IF('Drug Information'!I20=1,"",".")</f>
         <v/>
       </c>
-      <c r="I21" s="57" t="str">
+      <c r="I21" s="55" t="str">
         <f>IF('Drug Information'!J20=1,"",".")</f>
         <v/>
       </c>
-      <c r="J21" s="57" t="str">
+      <c r="J21" s="55" t="str">
         <f>IF('Drug Information'!K20=1,"",".")</f>
         <v/>
       </c>
-      <c r="K21" s="57" t="str">
+      <c r="K21" s="55" t="str">
         <f>IF('Drug Information'!L20=1,"",".")</f>
         <v/>
       </c>
-      <c r="L21" s="57" t="str">
+      <c r="L21" s="55" t="str">
         <f>IF('Drug Information'!M20=1,"",".")</f>
         <v/>
       </c>
-      <c r="M21" s="57" t="str">
+      <c r="M21" s="55" t="str">
         <f>IF('Drug Information'!N20=1,"",".")</f>
         <v/>
       </c>
-      <c r="N21" s="57" t="str">
+      <c r="N21" s="55" t="str">
         <f>IF('Drug Information'!O20=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="44" t="str">
+      <c r="B22" s="43" t="str">
         <f>'Drug Information'!$B21</f>
         <v>Aztreonam</v>
       </c>
-      <c r="C22" s="58" t="str">
+      <c r="C22" s="56" t="str">
         <f>IF('Drug Information'!D21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D22" s="58" t="str">
+      <c r="D22" s="56" t="str">
         <f>IF('Drug Information'!E21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E22" s="58" t="str">
+      <c r="E22" s="56" t="str">
         <f>IF('Drug Information'!F21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F22" s="58" t="str">
+      <c r="F22" s="56" t="str">
         <f>IF('Drug Information'!G21=1,"",".")</f>
         <v/>
       </c>
-      <c r="G22" s="58" t="str">
+      <c r="G22" s="56" t="str">
         <f>IF('Drug Information'!H21=1,"",".")</f>
         <v/>
       </c>
-      <c r="H22" s="58" t="str">
+      <c r="H22" s="56" t="str">
         <f>IF('Drug Information'!I21=1,"",".")</f>
         <v/>
       </c>
-      <c r="I22" s="58" t="str">
+      <c r="I22" s="56" t="str">
         <f>IF('Drug Information'!J21=1,"",".")</f>
         <v/>
       </c>
-      <c r="J22" s="58" t="str">
+      <c r="J22" s="56" t="str">
         <f>IF('Drug Information'!K21=1,"",".")</f>
         <v/>
       </c>
-      <c r="K22" s="58" t="str">
+      <c r="K22" s="56" t="str">
         <f>IF('Drug Information'!L21=1,"",".")</f>
         <v/>
       </c>
-      <c r="L22" s="58" t="str">
+      <c r="L22" s="56" t="str">
         <f>IF('Drug Information'!M21=1,"",".")</f>
         <v/>
       </c>
-      <c r="M22" s="58" t="str">
+      <c r="M22" s="56" t="str">
         <f>IF('Drug Information'!N21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N22" s="58" t="str">
+      <c r="N22" s="56" t="str">
         <f>IF('Drug Information'!O21=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="146" t="s">
+      <c r="A23" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="45" t="str">
+      <c r="B23" s="44" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="C23" s="59" t="str">
+      <c r="C23" s="57" t="str">
         <f>IF('Drug Information'!D22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D23" s="59" t="str">
+      <c r="D23" s="57" t="str">
         <f>IF('Drug Information'!E22=1,"",".")</f>
         <v/>
       </c>
-      <c r="E23" s="59" t="str">
+      <c r="E23" s="57" t="str">
         <f>IF('Drug Information'!F22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F23" s="59" t="str">
+      <c r="F23" s="57" t="str">
         <f>IF('Drug Information'!G22=1,"",".")</f>
         <v/>
       </c>
-      <c r="G23" s="59" t="str">
+      <c r="G23" s="57" t="str">
         <f>IF('Drug Information'!H22=1,"",".")</f>
         <v/>
       </c>
-      <c r="H23" s="59" t="str">
+      <c r="H23" s="57" t="str">
         <f>IF('Drug Information'!I22=1,"",".")</f>
         <v/>
       </c>
-      <c r="I23" s="59" t="str">
+      <c r="I23" s="57" t="str">
         <f>IF('Drug Information'!J22=1,"",".")</f>
         <v/>
       </c>
-      <c r="J23" s="59" t="str">
+      <c r="J23" s="57" t="str">
         <f>IF('Drug Information'!K22=1,"",".")</f>
         <v/>
       </c>
-      <c r="K23" s="59" t="str">
+      <c r="K23" s="57" t="str">
         <f>IF('Drug Information'!L22=1,"",".")</f>
         <v/>
       </c>
-      <c r="L23" s="59" t="str">
+      <c r="L23" s="57" t="str">
         <f>IF('Drug Information'!M22=1,"",".")</f>
         <v/>
       </c>
-      <c r="M23" s="59" t="str">
+      <c r="M23" s="57" t="str">
         <f>IF('Drug Information'!N22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N23" s="59" t="str">
+      <c r="N23" s="57" t="str">
         <f>IF('Drug Information'!O22=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="146"/>
-      <c r="B24" s="45" t="str">
+      <c r="A24" s="141"/>
+      <c r="B24" s="44" t="str">
         <f>'Drug Information'!$B23</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="C24" s="59" t="str">
+      <c r="C24" s="57" t="str">
         <f>IF('Drug Information'!D23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D24" s="59" t="str">
+      <c r="D24" s="57" t="str">
         <f>IF('Drug Information'!E23=1,"",".")</f>
         <v/>
       </c>
-      <c r="E24" s="59" t="str">
+      <c r="E24" s="57" t="str">
         <f>IF('Drug Information'!F23=1,"",".")</f>
         <v/>
       </c>
-      <c r="F24" s="59" t="str">
+      <c r="F24" s="57" t="str">
         <f>IF('Drug Information'!G23=1,"",".")</f>
         <v/>
       </c>
-      <c r="G24" s="59" t="str">
+      <c r="G24" s="57" t="str">
         <f>IF('Drug Information'!H23=1,"",".")</f>
         <v/>
       </c>
-      <c r="H24" s="59" t="str">
+      <c r="H24" s="57" t="str">
         <f>IF('Drug Information'!I23=1,"",".")</f>
         <v/>
       </c>
-      <c r="I24" s="59" t="str">
+      <c r="I24" s="57" t="str">
         <f>IF('Drug Information'!J23=1,"",".")</f>
         <v/>
       </c>
-      <c r="J24" s="59" t="str">
+      <c r="J24" s="57" t="str">
         <f>IF('Drug Information'!K23=1,"",".")</f>
         <v/>
       </c>
-      <c r="K24" s="59" t="str">
+      <c r="K24" s="57" t="str">
         <f>IF('Drug Information'!L23=1,"",".")</f>
         <v/>
       </c>
-      <c r="L24" s="59" t="str">
+      <c r="L24" s="57" t="str">
         <f>IF('Drug Information'!M23=1,"",".")</f>
         <v/>
       </c>
-      <c r="M24" s="59" t="str">
+      <c r="M24" s="57" t="str">
         <f>IF('Drug Information'!N23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N24" s="59" t="str">
+      <c r="N24" s="57" t="str">
         <f>IF('Drug Information'!O23=1,"",".")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="146"/>
-      <c r="B25" s="45" t="str">
+      <c r="A25" s="141"/>
+      <c r="B25" s="44" t="str">
         <f>'Drug Information'!$B24</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="C25" s="60" t="str">
+      <c r="C25" s="58" t="str">
         <f>IF('Drug Information'!D24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D25" s="60" t="str">
+      <c r="D25" s="58" t="str">
         <f>IF('Drug Information'!E24=1,"",".")</f>
         <v/>
       </c>
-      <c r="E25" s="60" t="str">
+      <c r="E25" s="58" t="str">
         <f>IF('Drug Information'!F24=1,"",".")</f>
         <v/>
       </c>
-      <c r="F25" s="60" t="str">
+      <c r="F25" s="58" t="str">
         <f>IF('Drug Information'!G24=1,"",".")</f>
         <v/>
       </c>
-      <c r="G25" s="60" t="str">
+      <c r="G25" s="58" t="str">
         <f>IF('Drug Information'!H24=1,"",".")</f>
         <v/>
       </c>
-      <c r="H25" s="60" t="str">
+      <c r="H25" s="58" t="str">
         <f>IF('Drug Information'!I24=1,"",".")</f>
         <v/>
       </c>
-      <c r="I25" s="60" t="str">
+      <c r="I25" s="58" t="str">
         <f>IF('Drug Information'!J24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J25" s="60" t="str">
+      <c r="J25" s="58" t="str">
         <f>IF('Drug Information'!K24=1,"",".")</f>
         <v/>
       </c>
-      <c r="K25" s="60" t="str">
+      <c r="K25" s="58" t="str">
         <f>IF('Drug Information'!L24=1,"",".")</f>
         <v/>
       </c>
-      <c r="L25" s="60" t="str">
+      <c r="L25" s="58" t="str">
         <f>IF('Drug Information'!M24=1,"",".")</f>
         <v/>
       </c>
-      <c r="M25" s="60" t="str">
+      <c r="M25" s="58" t="str">
         <f>IF('Drug Information'!N24=1,"",".")</f>
         <v/>
       </c>
-      <c r="N25" s="60" t="str">
+      <c r="N25" s="58" t="str">
         <f>IF('Drug Information'!O24=1,"",".")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="46" t="str">
+      <c r="B26" s="45" t="str">
         <f>'Drug Information'!$B25</f>
         <v>Gentamicin</v>
       </c>
-      <c r="C26" s="61" t="str">
+      <c r="C26" s="59" t="str">
         <f>IF('Drug Information'!D25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D26" s="61" t="str">
+      <c r="D26" s="59" t="str">
         <f>IF('Drug Information'!E25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E26" s="61" t="str">
+      <c r="E26" s="59" t="str">
         <f>IF('Drug Information'!F25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F26" s="61" t="str">
+      <c r="F26" s="59" t="str">
         <f>IF('Drug Information'!G25=1,"",".")</f>
         <v/>
       </c>
-      <c r="G26" s="61" t="str">
+      <c r="G26" s="59" t="str">
         <f>IF('Drug Information'!H25=1,"",".")</f>
         <v/>
       </c>
-      <c r="H26" s="61" t="str">
+      <c r="H26" s="59" t="str">
         <f>IF('Drug Information'!I25=1,"",".")</f>
         <v/>
       </c>
-      <c r="I26" s="61" t="str">
+      <c r="I26" s="59" t="str">
         <f>IF('Drug Information'!J25=1,"",".")</f>
         <v/>
       </c>
-      <c r="J26" s="61" t="str">
+      <c r="J26" s="59" t="str">
         <f>IF('Drug Information'!K25=1,"",".")</f>
         <v/>
       </c>
-      <c r="K26" s="61" t="str">
+      <c r="K26" s="59" t="str">
         <f>IF('Drug Information'!L25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L26" s="61" t="str">
+      <c r="L26" s="59" t="str">
         <f>IF('Drug Information'!M25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M26" s="61" t="str">
+      <c r="M26" s="59" t="str">
         <f>IF('Drug Information'!N25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N26" s="61" t="str">
+      <c r="N26" s="59" t="str">
         <f>IF('Drug Information'!O25=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="148"/>
-      <c r="B27" s="46" t="str">
+      <c r="A27" s="143"/>
+      <c r="B27" s="45" t="str">
         <f>'Drug Information'!$B26</f>
         <v>Tobramycin</v>
       </c>
-      <c r="C27" s="61" t="str">
+      <c r="C27" s="59" t="str">
         <f>IF('Drug Information'!D26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D27" s="61" t="str">
+      <c r="D27" s="59" t="str">
         <f>IF('Drug Information'!E26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E27" s="61" t="str">
+      <c r="E27" s="59" t="str">
         <f>IF('Drug Information'!F26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F27" s="61" t="str">
+      <c r="F27" s="59" t="str">
         <f>IF('Drug Information'!G26=1,"",".")</f>
         <v/>
       </c>
-      <c r="G27" s="61" t="str">
+      <c r="G27" s="59" t="str">
         <f>IF('Drug Information'!H26=1,"",".")</f>
         <v/>
       </c>
-      <c r="H27" s="61" t="str">
+      <c r="H27" s="59" t="str">
         <f>IF('Drug Information'!I26=1,"",".")</f>
         <v/>
       </c>
-      <c r="I27" s="61" t="str">
+      <c r="I27" s="59" t="str">
         <f>IF('Drug Information'!J26=1,"",".")</f>
         <v/>
       </c>
-      <c r="J27" s="61" t="str">
+      <c r="J27" s="59" t="str">
         <f>IF('Drug Information'!K26=1,"",".")</f>
         <v/>
       </c>
-      <c r="K27" s="61" t="str">
+      <c r="K27" s="59" t="str">
         <f>IF('Drug Information'!L26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L27" s="61" t="str">
+      <c r="L27" s="59" t="str">
         <f>IF('Drug Information'!M26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M27" s="61" t="str">
+      <c r="M27" s="59" t="str">
         <f>IF('Drug Information'!N26=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N27" s="61" t="str">
+      <c r="N27" s="59" t="str">
         <f>IF('Drug Information'!O26=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="149"/>
-      <c r="B28" s="46" t="str">
+      <c r="A28" s="144"/>
+      <c r="B28" s="45" t="str">
         <f>'Drug Information'!$B27</f>
         <v>Amikacin</v>
       </c>
-      <c r="C28" s="61" t="str">
+      <c r="C28" s="59" t="str">
         <f>IF('Drug Information'!D27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D28" s="61" t="str">
+      <c r="D28" s="59" t="str">
         <f>IF('Drug Information'!E27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E28" s="61" t="str">
+      <c r="E28" s="59" t="str">
         <f>IF('Drug Information'!F27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F28" s="61" t="str">
+      <c r="F28" s="59" t="str">
         <f>IF('Drug Information'!G27=1,"",".")</f>
         <v/>
       </c>
-      <c r="G28" s="61" t="str">
+      <c r="G28" s="59" t="str">
         <f>IF('Drug Information'!H27=1,"",".")</f>
         <v/>
       </c>
-      <c r="H28" s="61" t="str">
+      <c r="H28" s="59" t="str">
         <f>IF('Drug Information'!I27=1,"",".")</f>
         <v/>
       </c>
-      <c r="I28" s="61" t="str">
+      <c r="I28" s="59" t="str">
         <f>IF('Drug Information'!J27=1,"",".")</f>
         <v/>
       </c>
-      <c r="J28" s="61" t="str">
+      <c r="J28" s="59" t="str">
         <f>IF('Drug Information'!K27=1,"",".")</f>
         <v/>
       </c>
-      <c r="K28" s="61" t="str">
+      <c r="K28" s="59" t="str">
         <f>IF('Drug Information'!L27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L28" s="61" t="str">
+      <c r="L28" s="59" t="str">
         <f>IF('Drug Information'!M27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M28" s="61" t="str">
+      <c r="M28" s="59" t="str">
         <f>IF('Drug Information'!N27=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N28" s="61" t="str">
+      <c r="N28" s="59" t="str">
         <f>IF('Drug Information'!O27=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="47" t="str">
+      <c r="B29" s="46" t="str">
         <f>'Drug Information'!$B28</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C29" s="62" t="str">
+      <c r="C29" s="60" t="str">
         <f>IF('Drug Information'!D28=1,"",".")</f>
         <v/>
       </c>
-      <c r="D29" s="62" t="str">
+      <c r="D29" s="60" t="str">
         <f>IF('Drug Information'!E28=1,"",".")</f>
         <v/>
       </c>
-      <c r="E29" s="62" t="str">
+      <c r="E29" s="60" t="str">
         <f>IF('Drug Information'!F28=1,"",".")</f>
         <v/>
       </c>
-      <c r="F29" s="62" t="str">
+      <c r="F29" s="60" t="str">
         <f>IF('Drug Information'!G28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G29" s="62" t="str">
+      <c r="G29" s="60" t="str">
         <f>IF('Drug Information'!H28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H29" s="62" t="str">
+      <c r="H29" s="60" t="str">
         <f>IF('Drug Information'!I28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I29" s="62" t="str">
+      <c r="I29" s="60" t="str">
         <f>IF('Drug Information'!J28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J29" s="62" t="str">
+      <c r="J29" s="60" t="str">
         <f>IF('Drug Information'!K28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K29" s="62" t="str">
+      <c r="K29" s="60" t="str">
         <f>IF('Drug Information'!L28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L29" s="62" t="str">
+      <c r="L29" s="60" t="str">
         <f>IF('Drug Information'!M28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M29" s="62" t="str">
+      <c r="M29" s="60" t="str">
         <f>IF('Drug Information'!N28=1,"",".")</f>
         <v/>
       </c>
-      <c r="N29" s="62" t="str">
+      <c r="N29" s="60" t="str">
         <f>IF('Drug Information'!O28=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="48" t="str">
+      <c r="B30" s="47" t="str">
         <f>'Drug Information'!$B29</f>
         <v>Azithromycin</v>
       </c>
-      <c r="C30" s="63" t="str">
+      <c r="C30" s="61" t="str">
         <f>IF('Drug Information'!D29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D30" s="63" t="str">
+      <c r="D30" s="61" t="str">
         <f>IF('Drug Information'!E29=1,"",".")</f>
         <v/>
       </c>
-      <c r="E30" s="63" t="str">
+      <c r="E30" s="61" t="str">
         <f>IF('Drug Information'!F29=1,"",".")</f>
         <v/>
       </c>
-      <c r="F30" s="63" t="str">
+      <c r="F30" s="61" t="str">
         <f>IF('Drug Information'!G29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G30" s="63" t="str">
+      <c r="G30" s="61" t="str">
         <f>IF('Drug Information'!H29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H30" s="63" t="str">
+      <c r="H30" s="61" t="str">
         <f>IF('Drug Information'!I29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I30" s="63" t="str">
+      <c r="I30" s="61" t="str">
         <f>IF('Drug Information'!J29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J30" s="63" t="str">
+      <c r="J30" s="61" t="str">
         <f>IF('Drug Information'!K29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K30" s="63" t="str">
+      <c r="K30" s="61" t="str">
         <f>IF('Drug Information'!L29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L30" s="63" t="str">
+      <c r="L30" s="61" t="str">
         <f>IF('Drug Information'!M29=1,"",".")</f>
         <v/>
       </c>
-      <c r="M30" s="63" t="str">
+      <c r="M30" s="61" t="str">
         <f>IF('Drug Information'!N29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N30" s="63" t="str">
+      <c r="N30" s="61" t="str">
         <f>IF('Drug Information'!O29=1,"",".")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="49" t="str">
+      <c r="B31" s="48" t="str">
         <f>'Drug Information'!$B30</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C31" s="64" t="str">
+      <c r="C31" s="62" t="str">
         <f>IF('Drug Information'!D30=1,"",".")</f>
         <v/>
       </c>
-      <c r="D31" s="64" t="str">
+      <c r="D31" s="62" t="str">
         <f>IF('Drug Information'!E30=1,"",".")</f>
         <v/>
       </c>
-      <c r="E31" s="64" t="str">
+      <c r="E31" s="62" t="str">
         <f>IF('Drug Information'!F30=1,"",".")</f>
         <v/>
       </c>
-      <c r="F31" s="64" t="str">
+      <c r="F31" s="62" t="str">
         <f>IF('Drug Information'!G30=1,"",".")</f>
         <v/>
       </c>
-      <c r="G31" s="64" t="str">
+      <c r="G31" s="62" t="str">
         <f>IF('Drug Information'!H30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H31" s="64" t="str">
+      <c r="H31" s="62" t="str">
         <f>IF('Drug Information'!I30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I31" s="64" t="str">
+      <c r="I31" s="62" t="str">
         <f>IF('Drug Information'!J30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J31" s="64" t="str">
+      <c r="J31" s="62" t="str">
         <f>IF('Drug Information'!K30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K31" s="64" t="str">
+      <c r="K31" s="62" t="str">
         <f>IF('Drug Information'!L30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L31" s="64" t="str">
+      <c r="L31" s="62" t="str">
         <f>IF('Drug Information'!M30=1,"",".")</f>
         <v/>
       </c>
-      <c r="M31" s="64" t="str">
+      <c r="M31" s="62" t="str">
         <f>IF('Drug Information'!N30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N31" s="64" t="str">
+      <c r="N31" s="62" t="str">
         <f>IF('Drug Information'!O30=1,"",".")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="50" t="str">
+      <c r="B32" s="49" t="str">
         <f>'Drug Information'!$B31</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C32" s="65" t="str">
+      <c r="C32" s="63" t="str">
         <f>IF('Drug Information'!D31=1,"",".")</f>
         <v/>
       </c>
-      <c r="D32" s="65" t="str">
+      <c r="D32" s="63" t="str">
         <f>IF('Drug Information'!E31=1,"",".")</f>
         <v/>
       </c>
-      <c r="E32" s="65" t="str">
+      <c r="E32" s="63" t="str">
         <f>IF('Drug Information'!F31=1,"",".")</f>
         <v/>
       </c>
-      <c r="F32" s="65" t="str">
+      <c r="F32" s="63" t="str">
         <f>IF('Drug Information'!G31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G32" s="65" t="str">
+      <c r="G32" s="63" t="str">
         <f>IF('Drug Information'!H31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H32" s="65" t="str">
+      <c r="H32" s="63" t="str">
         <f>IF('Drug Information'!I31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I32" s="65" t="str">
+      <c r="I32" s="63" t="str">
         <f>IF('Drug Information'!J31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J32" s="65" t="str">
+      <c r="J32" s="63" t="str">
         <f>IF('Drug Information'!K31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K32" s="65" t="str">
+      <c r="K32" s="63" t="str">
         <f>IF('Drug Information'!L31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L32" s="65" t="str">
+      <c r="L32" s="63" t="str">
         <f>IF('Drug Information'!M31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M32" s="65" t="str">
+      <c r="M32" s="63" t="str">
         <f>IF('Drug Information'!N31=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N32" s="65" t="str">
+      <c r="N32" s="63" t="str">
         <f>IF('Drug Information'!O31=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="51" t="str">
+      <c r="B33" s="50" t="str">
         <f>'Drug Information'!$B32</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C33" s="66" t="str">
+      <c r="C33" s="64" t="str">
         <f>IF('Drug Information'!D32=1,"",".")</f>
         <v/>
       </c>
-      <c r="D33" s="66" t="str">
+      <c r="D33" s="64" t="str">
         <f>IF('Drug Information'!E32=1,"",".")</f>
         <v/>
       </c>
-      <c r="E33" s="66" t="str">
+      <c r="E33" s="64" t="str">
         <f>IF('Drug Information'!F32=1,"",".")</f>
         <v/>
       </c>
-      <c r="F33" s="66" t="str">
+      <c r="F33" s="64" t="str">
         <f>IF('Drug Information'!G32=1,"",".")</f>
         <v/>
       </c>
-      <c r="G33" s="66" t="str">
+      <c r="G33" s="64" t="str">
         <f>IF('Drug Information'!H32=1,"",".")</f>
         <v/>
       </c>
-      <c r="H33" s="66" t="str">
+      <c r="H33" s="64" t="str">
         <f>IF('Drug Information'!I32=1,"",".")</f>
         <v/>
       </c>
-      <c r="I33" s="66" t="str">
+      <c r="I33" s="64" t="str">
         <f>IF('Drug Information'!J32=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J33" s="66" t="str">
+      <c r="J33" s="64" t="str">
         <f>IF('Drug Information'!K32=1,"",".")</f>
         <v/>
       </c>
-      <c r="K33" s="66" t="str">
+      <c r="K33" s="64" t="str">
         <f>IF('Drug Information'!L32=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L33" s="66" t="str">
+      <c r="L33" s="64" t="str">
         <f>IF('Drug Information'!M32=1,"",".")</f>
         <v/>
       </c>
-      <c r="M33" s="66" t="str">
+      <c r="M33" s="64" t="str">
         <f>IF('Drug Information'!N32=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N33" s="66" t="str">
+      <c r="N33" s="64" t="str">
         <f>IF('Drug Information'!O32=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="52" t="str">
+      <c r="B34" s="51" t="str">
         <f>'Drug Information'!$B33</f>
         <v>Metronidazole</v>
       </c>
-      <c r="C34" s="67" t="str">
+      <c r="C34" s="65" t="str">
         <f>IF('Drug Information'!D33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D34" s="67" t="str">
+      <c r="D34" s="65" t="str">
         <f>IF('Drug Information'!E33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E34" s="67" t="str">
+      <c r="E34" s="65" t="str">
         <f>IF('Drug Information'!F33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F34" s="67" t="str">
+      <c r="F34" s="65" t="str">
         <f>IF('Drug Information'!G33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G34" s="67" t="str">
+      <c r="G34" s="65" t="str">
         <f>IF('Drug Information'!H33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H34" s="67" t="str">
+      <c r="H34" s="65" t="str">
         <f>IF('Drug Information'!I33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I34" s="67" t="str">
+      <c r="I34" s="65" t="str">
         <f>IF('Drug Information'!J33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J34" s="67" t="str">
+      <c r="J34" s="65" t="str">
         <f>IF('Drug Information'!K33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K34" s="67" t="str">
+      <c r="K34" s="65" t="str">
         <f>IF('Drug Information'!L33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L34" s="67" t="str">
+      <c r="L34" s="65" t="str">
         <f>IF('Drug Information'!M33=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M34" s="67" t="str">
+      <c r="M34" s="65" t="str">
         <f>IF('Drug Information'!N33=1,"",".")</f>
         <v/>
       </c>
-      <c r="N34" s="67" t="str">
+      <c r="N34" s="65" t="str">
         <f>IF('Drug Information'!O33=1,"",".")</f>
         <v>.</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="129" t="s">
+      <c r="A35" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="129"/>
-      <c r="C35" s="129"/>
-      <c r="D35" s="129"/>
-      <c r="E35" s="129"/>
-      <c r="F35" s="129"/>
-      <c r="G35" s="129"/>
-      <c r="H35" s="129"/>
-      <c r="I35" s="129"/>
-      <c r="J35" s="129"/>
-      <c r="K35" s="129"/>
-      <c r="L35" s="129"/>
-      <c r="M35" s="129"/>
-      <c r="N35" s="129"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="127"/>
+      <c r="D35" s="127"/>
+      <c r="E35" s="127"/>
+      <c r="F35" s="127"/>
+      <c r="G35" s="127"/>
+      <c r="H35" s="127"/>
+      <c r="I35" s="127"/>
+      <c r="J35" s="127"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="127"/>
+      <c r="M35" s="127"/>
+      <c r="N35" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4878,19 +4875,19 @@
     <mergeCell ref="A35:N35"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="A26:A28"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B8 C3:N34">
+  <conditionalFormatting sqref="B3:B11 C3:N34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"."</formula>
     </cfRule>
@@ -4935,23 +4932,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="81" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="69" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="95" t="s">
+      <c r="K1" s="68"/>
+      <c r="L1" s="93" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -4992,7 +4989,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="96"/>
+      <c r="L2" s="94"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5022,11 +5019,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="70" t="str">
         <f>'Drug Information'!$B5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="73"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5043,12 +5040,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="72" t="str">
+      <c r="D5" s="70" t="str">
         <f>'Drug Information'!$B7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="73"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5065,14 +5062,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="75" t="str">
-        <f>'Drug Information'!$B8</f>
+      <c r="C6" s="73" t="str">
+        <f>'Drug Information'!$B11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="77"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="75"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5085,59 +5082,59 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="75" t="str">
-        <f>'Drug Information'!$B11</f>
+      <c r="C7" s="73" t="str">
+        <f>'Drug Information'!$B14</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="77"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="75"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="10" t="str">
-        <f>'Drug Information'!$B11</f>
+        <f>'Drug Information'!$B14</f>
         <v>Cefoxitin</v>
       </c>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="69" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="75" t="str">
-        <f>'Drug Information'!$B12</f>
+      <c r="C8" s="73" t="str">
+        <f>'Drug Information'!$B15</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="77"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="75"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="75" t="str">
-        <f>'Drug Information'!$B12</f>
+      <c r="I8" s="73" t="str">
+        <f>'Drug Information'!$B15</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="90"/>
-      <c r="K8" s="77"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="75"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="75" t="str">
-        <f>'Drug Information'!$B13</f>
+      <c r="D9" s="73" t="str">
+        <f>'Drug Information'!$B16</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -5149,125 +5146,125 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="91" t="str">
-        <f>'Drug Information'!$B14</f>
+      <c r="C10" s="89" t="str">
+        <f>'Drug Information'!$B17</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="77"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="75"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="69" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="78" t="str">
-        <f>'Drug Information'!$B15</f>
+      <c r="C11" s="76" t="str">
+        <f>'Drug Information'!$B8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="80"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="11" t="str">
-        <f>'Drug Information'!$B15</f>
+        <f>'Drug Information'!$B8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="78" t="str">
-        <f>'Drug Information'!$B16</f>
+      <c r="C12" s="76" t="str">
+        <f>'Drug Information'!$B9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="11" t="str">
-        <f>'Drug Information'!$B16</f>
+        <f>'Drug Information'!$B9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="93" t="str">
-        <f>'Drug Information'!$B17</f>
+      <c r="C13" s="91" t="str">
+        <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="94"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="92"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="93" t="str">
-        <f>'Drug Information'!$B17</f>
+      <c r="K13" s="91" t="str">
+        <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="94"/>
+      <c r="L13" s="92"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="69" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="104" t="str">
+      <c r="C14" s="102" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="106"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="104"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="104" t="str">
+      <c r="I14" s="102" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="106"/>
+      <c r="J14" s="103"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="104"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="104" t="str">
+      <c r="C15" s="102" t="str">
         <f>'Drug Information'!$B20</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="106"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="103"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="104"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -5277,20 +5274,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="107" t="s">
+      <c r="E16" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="109"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="107"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="69" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -5299,34 +5296,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="113" t="str">
+      <c r="E17" s="111" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="114"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114"/>
-      <c r="J17" s="114"/>
-      <c r="K17" s="115"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="113"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
+      <c r="A18" s="69"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="113" t="str">
+      <c r="C18" s="111" t="str">
         <f>'Drug Information'!$B23</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="117"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="115"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$B23</f>
@@ -5334,25 +5331,25 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="87" t="str">
+      <c r="C19" s="85" t="str">
         <f>'Drug Information'!$B24</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="89"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="87"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="87" t="str">
+      <c r="I19" s="85" t="str">
         <f>'Drug Information'!$B24</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="89"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="87"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -5361,14 +5358,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="120" t="str">
+      <c r="E20" s="118" t="str">
         <f>'Drug Information'!$B27</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="122"/>
-      <c r="I20" s="123"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="120"/>
+      <c r="I20" s="121"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -5378,12 +5375,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="97" t="str">
+      <c r="B21" s="95" t="str">
         <f>'Drug Information'!$B28</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="99"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -5402,11 +5399,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="118" t="str">
+      <c r="C22" s="116" t="str">
         <f>'Drug Information'!$B29</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="119"/>
+      <c r="D22" s="117"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -5427,13 +5424,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="124" t="str">
+      <c r="B23" s="122" t="str">
         <f>'Drug Information'!$B30</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="126"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="124"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -5453,12 +5450,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="100" t="str">
+      <c r="B24" s="98" t="str">
         <f>'Drug Information'!$B31</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="101"/>
-      <c r="D24" s="102"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="100"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -5473,15 +5470,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="110" t="str">
+      <c r="B25" s="108" t="str">
         <f>'Drug Information'!$B32</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="112"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="110"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -5514,21 +5511,21 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>

<commit_message>
Temporarily filter out drugs with no coverage data
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B59105-2310-41C5-A733-95C0818BB07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC587CC-B318-44CD-805A-75307F7CBC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1783,7 +1783,44 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
-  <autoFilter ref="B2:O39" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}"/>
+  <autoFilter ref="B2:O39" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Amikacin"/>
+        <filter val="Amoxicillin"/>
+        <filter val="Amoxicillin-Clavulanic Acid"/>
+        <filter val="Ampicillin"/>
+        <filter val="Ampicillin/Sulbactam"/>
+        <filter val="Azithromycin"/>
+        <filter val="Aztreonam"/>
+        <filter val="Benzylpenicillin"/>
+        <filter val="Cefalexin"/>
+        <filter val="Cefazolin"/>
+        <filter val="Cefepime"/>
+        <filter val="Cefoxitin"/>
+        <filter val="Ceftazidime"/>
+        <filter val="Ceftriaxone"/>
+        <filter val="Cephotetan"/>
+        <filter val="Ciprofloxacin"/>
+        <filter val="Clindamycin"/>
+        <filter val="Doxycycline"/>
+        <filter val="Ertapenem"/>
+        <filter val="Flucloxacillin"/>
+        <filter val="Gentamicin"/>
+        <filter val="Imipenem"/>
+        <filter val="Levofloxacin"/>
+        <filter val="Meropenem"/>
+        <filter val="Metronidazole"/>
+        <filter val="Moxifloxacin"/>
+        <filter val="Naficillin"/>
+        <filter val="Oxacillin"/>
+        <filter val="Piperacillin-Tazobactam"/>
+        <filter val="Tobramycin"/>
+        <filter val="Trimethoprim/Sulfamethoxazole"/>
+        <filter val="Vancomycin"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="3">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
@@ -2906,7 +2943,7 @@
         <v>Cefalexin</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="str" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B14)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
@@ -3092,7 +3129,7 @@
         <v>Cefoxitin</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="138" t="str" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B17)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>3rd-gen cephalosporin</v>
@@ -3340,7 +3377,7 @@
         <v>Cefepime</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="135" t="str" cm="1">
         <f t="array" aca="1" ref="A21" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B21)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>5th-gen cephalosporin</v>
@@ -4270,7 +4307,7 @@
         <v>Vancomycin</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="str" cm="1">
         <f t="array" aca="1" ref="A36" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B36)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Lipopeptides</v>
@@ -4332,7 +4369,7 @@
         <v>Daptomycin</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44" t="str" cm="1">
         <f t="array" aca="1" ref="A37" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B37)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Oxazolidinones</v>

</xml_diff>

<commit_message>
Add github action to generate PDF and JPG automatically from XLSX
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CFBA1C-3DFF-4106-BAD0-B611BB3439BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB76C799-DB27-4D40-9703-8F926C722B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="original antibiogram" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$N$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$O$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'original antibiogram'!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -822,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -995,6 +995,294 @@
     <xf numFmtId="0" fontId="10" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1004,9 +1292,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1025,15 +1310,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,15 +1328,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,276 +1336,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1346,7 +1343,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="33">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1356,102 +1353,6 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1757,6 +1658,72 @@
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -1782,7 +1749,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B2:O39" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}">
     <filterColumn colId="0">
       <filters>
@@ -1822,43 +1789,43 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="29">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FC9C8C68-530C-4012-80B1-959161B27B76}" name="MRSA" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{FC9C8C68-530C-4012-80B1-959161B27B76}" name="MRSA" dataDxfId="28">
       <calculatedColumnFormula>IF('Drug Information'!C2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FBBC04D6-A577-454C-9CA5-71A9E5B59BE9}" name="MSSA" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{FBBC04D6-A577-454C-9CA5-71A9E5B59BE9}" name="MSSA" dataDxfId="27">
       <calculatedColumnFormula>IF('Drug Information'!D2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FE6DE44F-9CCB-4B75-91DD-689C40EFDD60}" name="Streptococci" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{FE6DE44F-9CCB-4B75-91DD-689C40EFDD60}" name="Streptococci" dataDxfId="26">
       <calculatedColumnFormula>IF('Drug Information'!E2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{050D08FE-B7BA-4BA2-9308-9602383C097B}" name="E. coli" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{050D08FE-B7BA-4BA2-9308-9602383C097B}" name="E. coli" dataDxfId="25">
       <calculatedColumnFormula>IF('Drug Information'!F2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0056F4D3-DB47-4738-9938-DDEB05F402A0}" name="P. mirabilis" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{0056F4D3-DB47-4738-9938-DDEB05F402A0}" name="P. mirabilis" dataDxfId="24">
       <calculatedColumnFormula>IF('Drug Information'!G2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61CA5D48-A78B-422A-A1CB-1B458E5C3C92}" name="Klebsiella" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{61CA5D48-A78B-422A-A1CB-1B458E5C3C92}" name="Klebsiella" dataDxfId="23">
       <calculatedColumnFormula>IF('Drug Information'!H2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6157DD55-5AAB-4974-B118-40237915EB0E}" name="Pseudomonas" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{6157DD55-5AAB-4974-B118-40237915EB0E}" name="Pseudomonas" dataDxfId="22">
       <calculatedColumnFormula>IF('Drug Information'!I2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{81D75E20-E7E3-4FBF-9379-ED66BEC6D631}" name="ESCAPPM" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{81D75E20-E7E3-4FBF-9379-ED66BEC6D631}" name="ESCAPPM" dataDxfId="21">
       <calculatedColumnFormula>IF('Drug Information'!J2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58146AC7-0BAA-4A64-8334-7BA8D5AD4463}" name="N. gonorrhoeae" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{58146AC7-0BAA-4A64-8334-7BA8D5AD4463}" name="N. gonorrhoeae" dataDxfId="20">
       <calculatedColumnFormula>IF('Drug Information'!K2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="19">
       <calculatedColumnFormula>IF('Drug Information'!L2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="???" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="???" dataDxfId="18">
       <calculatedColumnFormula>IF('Drug Information'!M2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="6">
+    <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="17">
       <calculatedColumnFormula>IF('Drug Information'!N2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{4A3A98C8-EB5C-429F-9790-93036600FBEE}" name="Drug Name "/>
@@ -1868,23 +1835,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:N38" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:N38" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:N38" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Drug Class" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Drug Class" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2159,9 +2126,9 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J5" sqref="J5"/>
+      <selection pane="topRight" activeCell="O41" sqref="A1:O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2147,7 @@
     <col min="12" max="12" width="18.75" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.75" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.875" style="142" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.875" style="64" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="42.5" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.875" style="2" bestFit="1" customWidth="1"/>
@@ -2188,26 +2155,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="120" t="s">
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="121" t="s">
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="121"/>
+      <c r="L1" s="106"/>
       <c r="M1" s="33" t="s">
         <v>6</v>
       </c>
@@ -2217,8 +2184,8 @@
       <c r="O1" s="47"/>
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="123"/>
-      <c r="B2" s="144" t="s">
+      <c r="A2" s="100"/>
+      <c r="B2" s="66" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -2257,16 +2224,16 @@
       <c r="N2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="157" t="s">
+      <c r="O2" s="79" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="124" t="str" cm="1">
+      <c r="A3" s="60" t="str" cm="1">
         <f t="array" aca="1" ref="A3" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B3)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Penicillin</v>
       </c>
-      <c r="B3" s="145" t="str">
+      <c r="B3" s="67" t="str">
         <f>'Drug Information'!$A2</f>
         <v>Benzylpenicillin</v>
       </c>
@@ -2318,17 +2285,17 @@
         <f>IF('Drug Information'!N2=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O3" s="158" t="str">
+      <c r="O3" s="80" t="str">
         <f>'Drug Information'!$A2</f>
         <v>Benzylpenicillin</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="125" t="str" cm="1">
+      <c r="A4" s="109" t="str" cm="1">
         <f t="array" aca="1" ref="A4" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B4)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B4" s="145" t="str">
+      <c r="B4" s="67" t="str">
         <f>'Drug Information'!$A3</f>
         <v>Naficillin</v>
       </c>
@@ -2380,17 +2347,17 @@
         <f>IF('Drug Information'!N3=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O4" s="158" t="str">
+      <c r="O4" s="80" t="str">
         <f>'Drug Information'!$A3</f>
         <v>Naficillin</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="126" t="str" cm="1">
+      <c r="A5" s="110" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B5)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B5" s="145" t="str">
+      <c r="B5" s="67" t="str">
         <f>'Drug Information'!$A4</f>
         <v>Oxacillin</v>
       </c>
@@ -2442,17 +2409,17 @@
         <f>IF('Drug Information'!N4=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O5" s="158" t="str">
+      <c r="O5" s="80" t="str">
         <f>'Drug Information'!$A4</f>
         <v>Oxacillin</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="127" t="str" cm="1">
+      <c r="A6" s="111" t="str" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B6)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B6" s="145" t="str">
+      <c r="B6" s="67" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
@@ -2504,17 +2471,17 @@
         <f>IF('Drug Information'!N5=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O6" s="158" t="str">
+      <c r="O6" s="80" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="125" t="str" cm="1">
+      <c r="A7" s="109" t="str" cm="1">
         <f t="array" aca="1" ref="A7" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B7)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins</v>
       </c>
-      <c r="B7" s="145" t="str">
+      <c r="B7" s="67" t="str">
         <f>'Drug Information'!$A6</f>
         <v>Ampicillin</v>
       </c>
@@ -2566,17 +2533,17 @@
         <f>IF('Drug Information'!N6=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O7" s="158" t="str">
+      <c r="O7" s="80" t="str">
         <f>'Drug Information'!$A6</f>
         <v>Ampicillin</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127" t="str" cm="1">
+      <c r="A8" s="111" t="str" cm="1">
         <f t="array" aca="1" ref="A8" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B8)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins</v>
       </c>
-      <c r="B8" s="145" t="str">
+      <c r="B8" s="67" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
@@ -2628,17 +2595,17 @@
         <f>IF('Drug Information'!N7=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O8" s="158" t="str">
+      <c r="O8" s="80" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="128" t="str" cm="1">
+      <c r="A9" s="103" t="str" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B9)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B9" s="146" t="str">
+      <c r="B9" s="68" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
@@ -2690,17 +2657,17 @@
         <f>IF('Drug Information'!N8=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O9" s="159" t="str">
+      <c r="O9" s="81" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="128" t="str" cm="1">
+      <c r="A10" s="103" t="str" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B10)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B10" s="146" t="str">
+      <c r="B10" s="68" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
@@ -2752,17 +2719,17 @@
         <f>IF('Drug Information'!N9=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O10" s="159" t="str">
+      <c r="O10" s="81" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="128" t="str" cm="1">
+      <c r="A11" s="103" t="str" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B11)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B11" s="146" t="str">
+      <c r="B11" s="68" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
@@ -2814,637 +2781,637 @@
         <f>IF('Drug Information'!N10=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O11" s="159" t="str">
+      <c r="O11" s="81" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="134" t="str" cm="1">
+      <c r="A12" s="107" t="str" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B12)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>1st-gen cephalosporin</v>
       </c>
-      <c r="B12" s="147" t="str">
+      <c r="B12" s="69" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="C12" s="136" t="str">
+      <c r="C12" s="62" t="str">
         <f>IF('Drug Information'!C11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D12" s="136" t="str">
+      <c r="D12" s="62" t="str">
         <f>IF('Drug Information'!D11=1,"",".")</f>
         <v/>
       </c>
-      <c r="E12" s="136" t="str">
+      <c r="E12" s="62" t="str">
         <f>IF('Drug Information'!E11=1,"",".")</f>
         <v/>
       </c>
-      <c r="F12" s="136" t="str">
+      <c r="F12" s="62" t="str">
         <f>IF('Drug Information'!F11=1,"",".")</f>
         <v/>
       </c>
-      <c r="G12" s="136" t="str">
+      <c r="G12" s="62" t="str">
         <f>IF('Drug Information'!G11=1,"",".")</f>
         <v/>
       </c>
-      <c r="H12" s="136" t="str">
+      <c r="H12" s="62" t="str">
         <f>IF('Drug Information'!H11=1,"",".")</f>
         <v/>
       </c>
-      <c r="I12" s="136" t="str">
+      <c r="I12" s="62" t="str">
         <f>IF('Drug Information'!I11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J12" s="136" t="str">
+      <c r="J12" s="62" t="str">
         <f>IF('Drug Information'!J11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K12" s="136" t="str">
+      <c r="K12" s="62" t="str">
         <f>IF('Drug Information'!K11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L12" s="136" t="str">
+      <c r="L12" s="62" t="str">
         <f>IF('Drug Information'!L11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M12" s="136" t="str">
+      <c r="M12" s="62" t="str">
         <f>IF('Drug Information'!M11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N12" s="136" t="str">
+      <c r="N12" s="62" t="str">
         <f>IF('Drug Information'!N11=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O12" s="160" t="str">
+      <c r="O12" s="82" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="137" t="str" cm="1">
+      <c r="A13" s="108" t="str" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B13)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>1st-gen cephalosporin</v>
       </c>
-      <c r="B13" s="147" t="str">
+      <c r="B13" s="69" t="str">
         <f>'Drug Information'!$A12</f>
         <v>Cefalexin</v>
       </c>
-      <c r="C13" s="136" t="str">
+      <c r="C13" s="62" t="str">
         <f>IF('Drug Information'!C12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D13" s="136" t="str">
+      <c r="D13" s="62" t="str">
         <f>IF('Drug Information'!D12=1,"",".")</f>
         <v/>
       </c>
-      <c r="E13" s="136" t="str">
+      <c r="E13" s="62" t="str">
         <f>IF('Drug Information'!E12=1,"",".")</f>
         <v/>
       </c>
-      <c r="F13" s="136" t="str">
+      <c r="F13" s="62" t="str">
         <f>IF('Drug Information'!F12=1,"",".")</f>
         <v/>
       </c>
-      <c r="G13" s="136" t="str">
+      <c r="G13" s="62" t="str">
         <f>IF('Drug Information'!G12=1,"",".")</f>
         <v/>
       </c>
-      <c r="H13" s="136" t="str">
+      <c r="H13" s="62" t="str">
         <f>IF('Drug Information'!H12=1,"",".")</f>
         <v/>
       </c>
-      <c r="I13" s="136" t="str">
+      <c r="I13" s="62" t="str">
         <f>IF('Drug Information'!I12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J13" s="136" t="str">
+      <c r="J13" s="62" t="str">
         <f>IF('Drug Information'!J12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K13" s="136" t="str">
+      <c r="K13" s="62" t="str">
         <f>IF('Drug Information'!K12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L13" s="136" t="str">
+      <c r="L13" s="62" t="str">
         <f>IF('Drug Information'!L12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M13" s="136" t="str">
+      <c r="M13" s="62" t="str">
         <f>IF('Drug Information'!M12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N13" s="136" t="str">
+      <c r="N13" s="62" t="str">
         <f>IF('Drug Information'!N12=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O13" s="160" t="str">
+      <c r="O13" s="82" t="str">
         <f>'Drug Information'!$A12</f>
         <v>Cefalexin</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="138" t="str" cm="1">
+      <c r="A14" s="95" t="str" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B14)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B14" s="147" t="str">
+      <c r="B14" s="69" t="str">
         <f>'Drug Information'!$A13</f>
         <v>Cefuroxime</v>
       </c>
-      <c r="C14" s="136" t="str">
+      <c r="C14" s="62" t="str">
         <f>IF('Drug Information'!C13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D14" s="136" t="str">
+      <c r="D14" s="62" t="str">
         <f>IF('Drug Information'!D13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E14" s="136" t="str">
+      <c r="E14" s="62" t="str">
         <f>IF('Drug Information'!E13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F14" s="136" t="str">
+      <c r="F14" s="62" t="str">
         <f>IF('Drug Information'!F13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G14" s="136" t="str">
+      <c r="G14" s="62" t="str">
         <f>IF('Drug Information'!G13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H14" s="136" t="str">
+      <c r="H14" s="62" t="str">
         <f>IF('Drug Information'!H13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I14" s="136" t="str">
+      <c r="I14" s="62" t="str">
         <f>IF('Drug Information'!I13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J14" s="136" t="str">
+      <c r="J14" s="62" t="str">
         <f>IF('Drug Information'!J13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K14" s="136" t="str">
+      <c r="K14" s="62" t="str">
         <f>IF('Drug Information'!K13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L14" s="136" t="str">
+      <c r="L14" s="62" t="str">
         <f>IF('Drug Information'!L13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M14" s="136" t="str">
+      <c r="M14" s="62" t="str">
         <f>IF('Drug Information'!M13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N14" s="136" t="str">
+      <c r="N14" s="62" t="str">
         <f>IF('Drug Information'!N13=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O14" s="160" t="str">
+      <c r="O14" s="82" t="str">
         <f>'Drug Information'!$A13</f>
         <v>Cefuroxime</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="139" t="str" cm="1">
+      <c r="A15" s="96" t="str" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B15)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B15" s="147" t="str">
+      <c r="B15" s="69" t="str">
         <f>'Drug Information'!$A14</f>
         <v>Cephotetan</v>
       </c>
-      <c r="C15" s="136" t="str">
+      <c r="C15" s="62" t="str">
         <f>IF('Drug Information'!C14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D15" s="136" t="str">
+      <c r="D15" s="62" t="str">
         <f>IF('Drug Information'!D14=1,"",".")</f>
         <v/>
       </c>
-      <c r="E15" s="136" t="str">
+      <c r="E15" s="62" t="str">
         <f>IF('Drug Information'!E14=1,"",".")</f>
         <v/>
       </c>
-      <c r="F15" s="136" t="str">
+      <c r="F15" s="62" t="str">
         <f>IF('Drug Information'!F14=1,"",".")</f>
         <v/>
       </c>
-      <c r="G15" s="136" t="str">
+      <c r="G15" s="62" t="str">
         <f>IF('Drug Information'!G14=1,"",".")</f>
         <v/>
       </c>
-      <c r="H15" s="136" t="str">
+      <c r="H15" s="62" t="str">
         <f>IF('Drug Information'!H14=1,"",".")</f>
         <v/>
       </c>
-      <c r="I15" s="136" t="str">
+      <c r="I15" s="62" t="str">
         <f>IF('Drug Information'!I14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J15" s="136" t="str">
+      <c r="J15" s="62" t="str">
         <f>IF('Drug Information'!J14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K15" s="136" t="str">
+      <c r="K15" s="62" t="str">
         <f>IF('Drug Information'!K14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L15" s="136" t="str">
+      <c r="L15" s="62" t="str">
         <f>IF('Drug Information'!L14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M15" s="136" t="str">
+      <c r="M15" s="62" t="str">
         <f>IF('Drug Information'!M14=1,"",".")</f>
         <v/>
       </c>
-      <c r="N15" s="136" t="str">
+      <c r="N15" s="62" t="str">
         <f>IF('Drug Information'!N14=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O15" s="160" t="str">
+      <c r="O15" s="82" t="str">
         <f>'Drug Information'!$A14</f>
         <v>Cephotetan</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="140" t="str" cm="1">
+      <c r="A16" s="97" t="str" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B16)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B16" s="147" t="str">
+      <c r="B16" s="69" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="C16" s="136" t="str">
+      <c r="C16" s="62" t="str">
         <f>IF('Drug Information'!C15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D16" s="136" t="str">
+      <c r="D16" s="62" t="str">
         <f>IF('Drug Information'!D15=1,"",".")</f>
         <v/>
       </c>
-      <c r="E16" s="136" t="str">
+      <c r="E16" s="62" t="str">
         <f>IF('Drug Information'!E15=1,"",".")</f>
         <v/>
       </c>
-      <c r="F16" s="136" t="str">
+      <c r="F16" s="62" t="str">
         <f>IF('Drug Information'!F15=1,"",".")</f>
         <v/>
       </c>
-      <c r="G16" s="136" t="str">
+      <c r="G16" s="62" t="str">
         <f>IF('Drug Information'!G15=1,"",".")</f>
         <v/>
       </c>
-      <c r="H16" s="136" t="str">
+      <c r="H16" s="62" t="str">
         <f>IF('Drug Information'!H15=1,"",".")</f>
         <v/>
       </c>
-      <c r="I16" s="136" t="str">
+      <c r="I16" s="62" t="str">
         <f>IF('Drug Information'!I15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J16" s="136" t="str">
+      <c r="J16" s="62" t="str">
         <f>IF('Drug Information'!J15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K16" s="136" t="str">
+      <c r="K16" s="62" t="str">
         <f>IF('Drug Information'!K15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L16" s="136" t="str">
+      <c r="L16" s="62" t="str">
         <f>IF('Drug Information'!L15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M16" s="136" t="str">
+      <c r="M16" s="62" t="str">
         <f>IF('Drug Information'!M15=1,"",".")</f>
         <v/>
       </c>
-      <c r="N16" s="136" t="str">
+      <c r="N16" s="62" t="str">
         <f>IF('Drug Information'!N15=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O16" s="160" t="str">
+      <c r="O16" s="82" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="138" t="str" cm="1">
+      <c r="A17" s="95" t="str" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B17)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B17" s="147" t="str">
+      <c r="B17" s="69" t="str">
         <f>'Drug Information'!$A16</f>
         <v>Cefotaxime</v>
       </c>
-      <c r="C17" s="136" t="str">
+      <c r="C17" s="62" t="str">
         <f>IF('Drug Information'!C16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D17" s="136" t="str">
+      <c r="D17" s="62" t="str">
         <f>IF('Drug Information'!D16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E17" s="136" t="str">
+      <c r="E17" s="62" t="str">
         <f>IF('Drug Information'!E16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F17" s="136" t="str">
+      <c r="F17" s="62" t="str">
         <f>IF('Drug Information'!F16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G17" s="136" t="str">
+      <c r="G17" s="62" t="str">
         <f>IF('Drug Information'!G16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H17" s="136" t="str">
+      <c r="H17" s="62" t="str">
         <f>IF('Drug Information'!H16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I17" s="136" t="str">
+      <c r="I17" s="62" t="str">
         <f>IF('Drug Information'!I16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J17" s="136" t="str">
+      <c r="J17" s="62" t="str">
         <f>IF('Drug Information'!J16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K17" s="136" t="str">
+      <c r="K17" s="62" t="str">
         <f>IF('Drug Information'!K16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L17" s="136" t="str">
+      <c r="L17" s="62" t="str">
         <f>IF('Drug Information'!L16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M17" s="136" t="str">
+      <c r="M17" s="62" t="str">
         <f>IF('Drug Information'!M16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N17" s="136" t="str">
+      <c r="N17" s="62" t="str">
         <f>IF('Drug Information'!N16=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O17" s="160" t="str">
+      <c r="O17" s="82" t="str">
         <f>'Drug Information'!$A16</f>
         <v>Cefotaxime</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="139" t="str" cm="1">
+      <c r="A18" s="96" t="str" cm="1">
         <f t="array" aca="1" ref="A18" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B18)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B18" s="147" t="str">
+      <c r="B18" s="69" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="C18" s="136" t="str">
+      <c r="C18" s="62" t="str">
         <f>IF('Drug Information'!C17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D18" s="136" t="str">
+      <c r="D18" s="62" t="str">
         <f>IF('Drug Information'!D17=1,"",".")</f>
         <v/>
       </c>
-      <c r="E18" s="136" t="str">
+      <c r="E18" s="62" t="str">
         <f>IF('Drug Information'!E17=1,"",".")</f>
         <v/>
       </c>
-      <c r="F18" s="136" t="str">
+      <c r="F18" s="62" t="str">
         <f>IF('Drug Information'!F17=1,"",".")</f>
         <v/>
       </c>
-      <c r="G18" s="136" t="str">
+      <c r="G18" s="62" t="str">
         <f>IF('Drug Information'!G17=1,"",".")</f>
         <v/>
       </c>
-      <c r="H18" s="136" t="str">
+      <c r="H18" s="62" t="str">
         <f>IF('Drug Information'!H17=1,"",".")</f>
         <v/>
       </c>
-      <c r="I18" s="136" t="str">
+      <c r="I18" s="62" t="str">
         <f>IF('Drug Information'!I17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J18" s="136" t="str">
+      <c r="J18" s="62" t="str">
         <f>IF('Drug Information'!J17=1,"",".")</f>
         <v/>
       </c>
-      <c r="K18" s="136" t="str">
+      <c r="K18" s="62" t="str">
         <f>IF('Drug Information'!K17=1,"",".")</f>
         <v/>
       </c>
-      <c r="L18" s="136" t="str">
+      <c r="L18" s="62" t="str">
         <f>IF('Drug Information'!L17=1,"",".")</f>
         <v/>
       </c>
-      <c r="M18" s="136" t="str">
+      <c r="M18" s="62" t="str">
         <f>IF('Drug Information'!M17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N18" s="136" t="str">
+      <c r="N18" s="62" t="str">
         <f>IF('Drug Information'!N17=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O18" s="160" t="str">
+      <c r="O18" s="82" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="140" t="str" cm="1">
+      <c r="A19" s="97" t="str" cm="1">
         <f t="array" aca="1" ref="A19" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B19)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>4th-gen cephalosporin</v>
       </c>
-      <c r="B19" s="147" t="str">
+      <c r="B19" s="69" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="C19" s="136" t="str">
+      <c r="C19" s="62" t="str">
         <f>IF('Drug Information'!C18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D19" s="136" t="str">
+      <c r="D19" s="62" t="str">
         <f>IF('Drug Information'!D18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E19" s="136" t="str">
+      <c r="E19" s="62" t="str">
         <f>IF('Drug Information'!E18=1,"",".")</f>
         <v/>
       </c>
-      <c r="F19" s="136" t="str">
+      <c r="F19" s="62" t="str">
         <f>IF('Drug Information'!F18=1,"",".")</f>
         <v/>
       </c>
-      <c r="G19" s="136" t="str">
+      <c r="G19" s="62" t="str">
         <f>IF('Drug Information'!G18=1,"",".")</f>
         <v/>
       </c>
-      <c r="H19" s="136" t="str">
+      <c r="H19" s="62" t="str">
         <f>IF('Drug Information'!H18=1,"",".")</f>
         <v/>
       </c>
-      <c r="I19" s="136" t="str">
+      <c r="I19" s="62" t="str">
         <f>IF('Drug Information'!I18=1,"",".")</f>
         <v/>
       </c>
-      <c r="J19" s="136" t="str">
+      <c r="J19" s="62" t="str">
         <f>IF('Drug Information'!J18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K19" s="136" t="str">
+      <c r="K19" s="62" t="str">
         <f>IF('Drug Information'!K18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L19" s="136" t="str">
+      <c r="L19" s="62" t="str">
         <f>IF('Drug Information'!L18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M19" s="136" t="str">
+      <c r="M19" s="62" t="str">
         <f>IF('Drug Information'!M18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N19" s="136" t="str">
+      <c r="N19" s="62" t="str">
         <f>IF('Drug Information'!N18=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O19" s="160" t="str">
+      <c r="O19" s="82" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="135" t="str" cm="1">
+      <c r="A20" s="61" t="str" cm="1">
         <f t="array" aca="1" ref="A20" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B20)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>4th-gen cephalosporin</v>
       </c>
-      <c r="B20" s="147" t="str">
+      <c r="B20" s="69" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="C20" s="136" t="str">
+      <c r="C20" s="62" t="str">
         <f>IF('Drug Information'!C19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D20" s="136" t="str">
+      <c r="D20" s="62" t="str">
         <f>IF('Drug Information'!D19=1,"",".")</f>
         <v/>
       </c>
-      <c r="E20" s="136" t="str">
+      <c r="E20" s="62" t="str">
         <f>IF('Drug Information'!E19=1,"",".")</f>
         <v/>
       </c>
-      <c r="F20" s="136" t="str">
+      <c r="F20" s="62" t="str">
         <f>IF('Drug Information'!F19=1,"",".")</f>
         <v/>
       </c>
-      <c r="G20" s="136" t="str">
+      <c r="G20" s="62" t="str">
         <f>IF('Drug Information'!G19=1,"",".")</f>
         <v/>
       </c>
-      <c r="H20" s="136" t="str">
+      <c r="H20" s="62" t="str">
         <f>IF('Drug Information'!H19=1,"",".")</f>
         <v/>
       </c>
-      <c r="I20" s="136" t="str">
+      <c r="I20" s="62" t="str">
         <f>IF('Drug Information'!I19=1,"",".")</f>
         <v/>
       </c>
-      <c r="J20" s="136" t="str">
+      <c r="J20" s="62" t="str">
         <f>IF('Drug Information'!J19=1,"",".")</f>
         <v/>
       </c>
-      <c r="K20" s="136" t="str">
+      <c r="K20" s="62" t="str">
         <f>IF('Drug Information'!K19=1,"",".")</f>
         <v/>
       </c>
-      <c r="L20" s="136" t="str">
+      <c r="L20" s="62" t="str">
         <f>IF('Drug Information'!L19=1,"",".")</f>
         <v/>
       </c>
-      <c r="M20" s="136" t="str">
+      <c r="M20" s="62" t="str">
         <f>IF('Drug Information'!M19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N20" s="136" t="str">
+      <c r="N20" s="62" t="str">
         <f>IF('Drug Information'!N19=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O20" s="160" t="str">
+      <c r="O20" s="82" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="135" t="str" cm="1">
+      <c r="A21" s="61" t="str" cm="1">
         <f t="array" aca="1" ref="A21" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B21)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>5th-gen cephalosporin</v>
       </c>
-      <c r="B21" s="147" t="str">
+      <c r="B21" s="69" t="str">
         <f>'Drug Information'!$A20</f>
         <v>Ceftaroline</v>
       </c>
-      <c r="C21" s="136" t="str">
+      <c r="C21" s="62" t="str">
         <f>IF('Drug Information'!C20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D21" s="136" t="str">
+      <c r="D21" s="62" t="str">
         <f>IF('Drug Information'!D20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E21" s="136" t="str">
+      <c r="E21" s="62" t="str">
         <f>IF('Drug Information'!E20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F21" s="136" t="str">
+      <c r="F21" s="62" t="str">
         <f>IF('Drug Information'!F20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G21" s="136" t="str">
+      <c r="G21" s="62" t="str">
         <f>IF('Drug Information'!G20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H21" s="136" t="str">
+      <c r="H21" s="62" t="str">
         <f>IF('Drug Information'!H20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I21" s="136" t="str">
+      <c r="I21" s="62" t="str">
         <f>IF('Drug Information'!I20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J21" s="136" t="str">
+      <c r="J21" s="62" t="str">
         <f>IF('Drug Information'!J20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K21" s="136" t="str">
+      <c r="K21" s="62" t="str">
         <f>IF('Drug Information'!K20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L21" s="136" t="str">
+      <c r="L21" s="62" t="str">
         <f>IF('Drug Information'!L20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M21" s="136" t="str">
+      <c r="M21" s="62" t="str">
         <f>IF('Drug Information'!M20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N21" s="136" t="str">
+      <c r="N21" s="62" t="str">
         <f>IF('Drug Information'!N20=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O21" s="160" t="str">
+      <c r="O21" s="82" t="str">
         <f>'Drug Information'!$A20</f>
         <v>Ceftaroline</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="129" t="str" cm="1">
+      <c r="A22" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A22" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B22)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B22" s="148" t="str">
+      <c r="B22" s="70" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
@@ -3496,17 +3463,17 @@
         <f>IF('Drug Information'!N21=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O22" s="161" t="str">
+      <c r="O22" s="83" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="129" t="str" cm="1">
+      <c r="A23" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A23" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B23)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B23" s="148" t="str">
+      <c r="B23" s="70" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Imipenem</v>
       </c>
@@ -3558,17 +3525,17 @@
         <f>IF('Drug Information'!N22=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O23" s="161" t="str">
+      <c r="O23" s="83" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Imipenem</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="129" t="str" cm="1">
+      <c r="A24" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A24" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B24)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B24" s="148" t="str">
+      <c r="B24" s="70" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
@@ -3620,7 +3587,7 @@
         <f>IF('Drug Information'!N23=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O24" s="161" t="str">
+      <c r="O24" s="83" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
@@ -3630,7 +3597,7 @@
         <f t="array" aca="1" ref="A25" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B25)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Monobactams</v>
       </c>
-      <c r="B25" s="149" t="str">
+      <c r="B25" s="71" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Aztreonam</v>
       </c>
@@ -3682,17 +3649,17 @@
         <f>IF('Drug Information'!N24=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O25" s="162" t="str">
+      <c r="O25" s="84" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Aztreonam</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="130" t="str" cm="1">
+      <c r="A26" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A26" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B26)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B26" s="150" t="str">
+      <c r="B26" s="72" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
@@ -3744,17 +3711,17 @@
         <f>IF('Drug Information'!N25=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O26" s="163" t="str">
+      <c r="O26" s="85" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="130" t="str" cm="1">
+      <c r="A27" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A27" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B27)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B27" s="150" t="str">
+      <c r="B27" s="72" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
@@ -3806,17 +3773,17 @@
         <f>IF('Drug Information'!N26=1,"",".")</f>
         <v/>
       </c>
-      <c r="O27" s="163" t="str">
+      <c r="O27" s="85" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="130" t="str" cm="1">
+      <c r="A28" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B28)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B28" s="150" t="str">
+      <c r="B28" s="72" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
@@ -3868,17 +3835,17 @@
         <f>IF('Drug Information'!N27=1,"",".")</f>
         <v/>
       </c>
-      <c r="O28" s="163" t="str">
+      <c r="O28" s="85" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="131" t="str" cm="1">
+      <c r="A29" s="112" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B29)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B29" s="151" t="str">
+      <c r="B29" s="73" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Gentamicin</v>
       </c>
@@ -3930,17 +3897,17 @@
         <f>IF('Drug Information'!N28=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O29" s="164" t="str">
+      <c r="O29" s="86" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Gentamicin</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="132" t="str" cm="1">
+      <c r="A30" s="113" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B30)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B30" s="151" t="str">
+      <c r="B30" s="73" t="str">
         <f>'Drug Information'!$A29</f>
         <v>Tobramycin</v>
       </c>
@@ -3992,17 +3959,17 @@
         <f>IF('Drug Information'!N29=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O30" s="164" t="str">
+      <c r="O30" s="86" t="str">
         <f>'Drug Information'!$A29</f>
         <v>Tobramycin</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="133" t="str" cm="1">
+      <c r="A31" s="114" t="str" cm="1">
         <f t="array" aca="1" ref="A31" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B31)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B31" s="151" t="str">
+      <c r="B31" s="73" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
@@ -4054,7 +4021,7 @@
         <f>IF('Drug Information'!N30=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O31" s="164" t="str">
+      <c r="O31" s="86" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
@@ -4064,7 +4031,7 @@
         <f t="array" aca="1" ref="A32" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B32)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Macrolides</v>
       </c>
-      <c r="B32" s="152" t="str">
+      <c r="B32" s="74" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
@@ -4116,7 +4083,7 @@
         <f>IF('Drug Information'!N31=1,"",".")</f>
         <v/>
       </c>
-      <c r="O32" s="165" t="str">
+      <c r="O32" s="87" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
@@ -4126,7 +4093,7 @@
         <f t="array" aca="1" ref="A33" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B33)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Lincosamide</v>
       </c>
-      <c r="B33" s="153" t="str">
+      <c r="B33" s="75" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
@@ -4178,7 +4145,7 @@
         <f>IF('Drug Information'!N32=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O33" s="166" t="str">
+      <c r="O33" s="88" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
@@ -4188,7 +4155,7 @@
         <f t="array" aca="1" ref="A34" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B34)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Tetracyclines</v>
       </c>
-      <c r="B34" s="154" t="str">
+      <c r="B34" s="76" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
@@ -4240,7 +4207,7 @@
         <f>IF('Drug Information'!N33=1,"",".")</f>
         <v/>
       </c>
-      <c r="O34" s="167" t="str">
+      <c r="O34" s="89" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
@@ -4250,7 +4217,7 @@
         <f t="array" aca="1" ref="A35" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B35)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Glycopeptides</v>
       </c>
-      <c r="B35" s="155" t="str">
+      <c r="B35" s="77" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
@@ -4302,7 +4269,7 @@
         <f>IF('Drug Information'!N34=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O35" s="168" t="str">
+      <c r="O35" s="90" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
@@ -4312,7 +4279,7 @@
         <f t="array" aca="1" ref="A36" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B36)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Lipopeptides</v>
       </c>
-      <c r="B36" s="155" t="str">
+      <c r="B36" s="77" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Daptomycin</v>
       </c>
@@ -4364,7 +4331,7 @@
         <f>IF('Drug Information'!N35=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O36" s="168" t="str">
+      <c r="O36" s="90" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Daptomycin</v>
       </c>
@@ -4374,66 +4341,66 @@
         <f t="array" aca="1" ref="A37" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B37)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Oxazolidinones</v>
       </c>
-      <c r="B37" s="155" t="str">
+      <c r="B37" s="77" t="str">
         <f>'Drug Information'!$A36</f>
         <v>Linezolid</v>
       </c>
-      <c r="C37" s="173" t="str">
+      <c r="C37" s="58" t="str">
         <f>IF('Drug Information'!C36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D37" s="173" t="str">
+      <c r="D37" s="58" t="str">
         <f>IF('Drug Information'!D36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E37" s="173" t="str">
+      <c r="E37" s="58" t="str">
         <f>IF('Drug Information'!E36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F37" s="173" t="str">
+      <c r="F37" s="58" t="str">
         <f>IF('Drug Information'!F36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G37" s="173" t="str">
+      <c r="G37" s="58" t="str">
         <f>IF('Drug Information'!G36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H37" s="173" t="str">
+      <c r="H37" s="58" t="str">
         <f>IF('Drug Information'!H36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I37" s="173" t="str">
+      <c r="I37" s="58" t="str">
         <f>IF('Drug Information'!I36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J37" s="173" t="str">
+      <c r="J37" s="58" t="str">
         <f>IF('Drug Information'!J36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K37" s="173" t="str">
+      <c r="K37" s="58" t="str">
         <f>IF('Drug Information'!K36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L37" s="173" t="str">
+      <c r="L37" s="58" t="str">
         <f>IF('Drug Information'!L36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M37" s="173" t="str">
+      <c r="M37" s="58" t="str">
         <f>IF('Drug Information'!M36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="N37" s="173" t="str">
+      <c r="N37" s="58" t="str">
         <f>IF('Drug Information'!N36=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O37" s="168"/>
+      <c r="O37" s="90"/>
     </row>
     <row r="38" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B38)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Antimetabolite</v>
       </c>
-      <c r="B38" s="156" t="str">
+      <c r="B38" s="78" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
@@ -4485,7 +4452,7 @@
         <f>IF('Drug Information'!N37=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O38" s="169" t="str">
+      <c r="O38" s="91" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
@@ -4495,101 +4462,101 @@
         <f t="array" aca="1" ref="A39" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B39)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Nitroimidazoles</v>
       </c>
-      <c r="B39" s="170" t="str">
+      <c r="B39" s="92" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Metronidazole</v>
       </c>
-      <c r="C39" s="143" t="str">
+      <c r="C39" s="65" t="str">
         <f>IF('Drug Information'!C38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="D39" s="143" t="str">
+      <c r="D39" s="65" t="str">
         <f>IF('Drug Information'!D38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="E39" s="143" t="str">
+      <c r="E39" s="65" t="str">
         <f>IF('Drug Information'!E38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="F39" s="143" t="str">
+      <c r="F39" s="65" t="str">
         <f>IF('Drug Information'!F38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="G39" s="143" t="str">
+      <c r="G39" s="65" t="str">
         <f>IF('Drug Information'!G38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="H39" s="143" t="str">
+      <c r="H39" s="65" t="str">
         <f>IF('Drug Information'!H38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="I39" s="143" t="str">
+      <c r="I39" s="65" t="str">
         <f>IF('Drug Information'!I38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="J39" s="143" t="str">
+      <c r="J39" s="65" t="str">
         <f>IF('Drug Information'!J38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="K39" s="143" t="str">
+      <c r="K39" s="65" t="str">
         <f>IF('Drug Information'!K38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="L39" s="143" t="str">
+      <c r="L39" s="65" t="str">
         <f>IF('Drug Information'!L38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="M39" s="143" t="str">
+      <c r="M39" s="65" t="str">
         <f>IF('Drug Information'!M38=1,"",".")</f>
         <v/>
       </c>
-      <c r="N39" s="143" t="str">
+      <c r="N39" s="65" t="str">
         <f>IF('Drug Information'!N38=1,"",".")</f>
         <v>.</v>
       </c>
-      <c r="O39" s="171" t="str">
+      <c r="O39" s="93" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Metronidazole</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="174" t="s">
+      <c r="A40" s="98" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="174"/>
-      <c r="C40" s="174"/>
-      <c r="D40" s="174"/>
-      <c r="E40" s="174"/>
-      <c r="F40" s="174"/>
-      <c r="G40" s="174"/>
-      <c r="H40" s="174"/>
-      <c r="I40" s="174"/>
-      <c r="J40" s="174"/>
-      <c r="K40" s="174"/>
-      <c r="L40" s="174"/>
-      <c r="M40" s="174"/>
-      <c r="N40" s="174"/>
-      <c r="O40" s="174"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="172"/>
-      <c r="C42" s="172"/>
-      <c r="D42" s="172"/>
-      <c r="E42" s="172"/>
-      <c r="F42" s="172"/>
-      <c r="G42" s="172"/>
-      <c r="H42" s="172"/>
-      <c r="I42" s="172"/>
-      <c r="J42" s="172"/>
-      <c r="K42" s="172"/>
-      <c r="L42" s="172"/>
-      <c r="M42" s="172"/>
-      <c r="N42" s="172"/>
-      <c r="O42" s="172"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="94"/>
+      <c r="I42" s="94"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="94"/>
+      <c r="L42" s="94"/>
+      <c r="M42" s="94"/>
+      <c r="N42" s="94"/>
+      <c r="O42" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4614,7 +4581,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="42" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -5008,24 +4975,24 @@
       <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="141"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="141"/>
-      <c r="K13" s="141"/>
-      <c r="L13" s="141"/>
-      <c r="M13" s="141"/>
-      <c r="N13" s="141"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -5092,24 +5059,24 @@
       <c r="N15" s="31"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="141"/>
-      <c r="K16" s="141"/>
-      <c r="L16" s="141"/>
-      <c r="M16" s="141"/>
-      <c r="N16" s="141"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
@@ -5216,24 +5183,24 @@
       <c r="N19" s="31"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="141" t="s">
+      <c r="A20" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="141" t="s">
+      <c r="B20" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="141"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="141"/>
-      <c r="N20" s="141"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
@@ -5708,44 +5675,44 @@
       <c r="N34" s="31"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="141" t="s">
+      <c r="A35" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="141" t="s">
+      <c r="B35" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="141"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="141"/>
-      <c r="N35" s="141"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="141" t="s">
+      <c r="A36" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="141" t="s">
+      <c r="B36" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="141"/>
-      <c r="D36" s="141"/>
-      <c r="E36" s="141"/>
-      <c r="F36" s="141"/>
-      <c r="G36" s="141"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="141"/>
-      <c r="M36" s="141"/>
-      <c r="N36" s="141"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="63"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
@@ -5848,23 +5815,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="73" t="s">
+      <c r="C1" s="169"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="165" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="61" t="s">
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="87" t="s">
+      <c r="K1" s="158"/>
+      <c r="L1" s="139" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5905,7 +5872,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="88"/>
+      <c r="L2" s="140"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5935,11 +5902,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="64" t="str">
+      <c r="C4" s="159" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="160"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5956,12 +5923,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="64" t="str">
+      <c r="D5" s="159" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="65"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="160"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5978,14 +5945,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="67" t="str">
+      <c r="C6" s="162" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="69"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5998,14 +5965,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="67" t="str">
+      <c r="C7" s="162" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="69"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -6017,40 +5984,40 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="118" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="67" t="str">
+      <c r="C8" s="162" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="69"/>
+      <c r="D8" s="171"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="67" t="str">
+      <c r="I8" s="162" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="171"/>
+      <c r="K8" s="164"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
+      <c r="A9" s="118"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="67" t="str">
+      <c r="D9" s="162" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="69"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="164"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -6062,34 +6029,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="83" t="str">
+      <c r="C10" s="172" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="69"/>
+      <c r="D10" s="173"/>
+      <c r="E10" s="173"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="164"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="118" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="70" t="str">
+      <c r="C11" s="133" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6101,16 +6068,16 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
+      <c r="A12" s="118"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="70" t="str">
+      <c r="C12" s="133" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="135"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6122,65 +6089,65 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="85" t="str">
+      <c r="C13" s="147" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="86"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="149"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="85" t="str">
+      <c r="K13" s="147" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="86"/>
+      <c r="L13" s="149"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="118" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="96" t="str">
+      <c r="C14" s="150" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="98"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="152"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="96" t="str">
+      <c r="I14" s="150" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="97"/>
-      <c r="K14" s="97"/>
-      <c r="L14" s="98"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="151"/>
+      <c r="L14" s="152"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="96" t="str">
+      <c r="C15" s="150" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="98"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="152"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6190,20 +6157,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="99" t="s">
+      <c r="E16" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="101"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="155"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="118" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -6212,34 +6179,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="105" t="str">
+      <c r="E17" s="119" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="107"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="121"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="63"/>
+      <c r="A18" s="118"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="105" t="str">
+      <c r="C18" s="119" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
-      <c r="K18" s="109"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="123"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6247,25 +6214,25 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="63"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="79" t="str">
+      <c r="C19" s="124" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="81"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="126"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="79" t="str">
+      <c r="I19" s="124" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="81"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="125"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="126"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6274,14 +6241,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="112" t="str">
+      <c r="E20" s="129" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="113"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="114"/>
-      <c r="I20" s="115"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="131"/>
+      <c r="I20" s="132"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6291,12 +6258,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="89" t="str">
+      <c r="B21" s="141" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="143"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6315,11 +6282,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="110" t="str">
+      <c r="C22" s="127" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="111"/>
+      <c r="D22" s="128"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6340,13 +6307,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="116" t="str">
+      <c r="B23" s="136" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="117"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="118"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="138"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6366,12 +6333,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="92" t="str">
+      <c r="B24" s="144" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="94"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="146"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6386,15 +6353,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="102" t="str">
+      <c r="B25" s="115" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="103"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
-      <c r="G25" s="104"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="117"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6427,43 +6394,24 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="156"/>
+      <c r="D27" s="156"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="156"/>
+      <c r="I27" s="156"/>
+      <c r="J27" s="156"/>
+      <c r="K27" s="156"/>
+      <c r="L27" s="156"/>
+      <c r="M27" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6480,6 +6428,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test change to XLSX
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB76C799-DB27-4D40-9703-8F926C722B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72183C7-AEBD-483C-B8E7-F8FC922425F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,10 +305,10 @@
     <t xml:space="preserve">Drug Name </t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Oxazolidinones</t>
+  </si>
+  <si>
+    <t>????</t>
   </si>
 </sst>
 </file>
@@ -1160,31 +1160,61 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1196,40 +1226,19 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,15 +1265,9 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1283,58 +1286,55 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1822,7 +1822,7 @@
     <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="19">
       <calculatedColumnFormula>IF('Drug Information'!L2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="???" dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="????" dataDxfId="18">
       <calculatedColumnFormula>IF('Drug Information'!M2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="17">
@@ -2128,7 +2128,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O41" sqref="A1:O41"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2219,7 +2219,7 @@
         <v>44</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N2" s="38" t="s">
         <v>46</v>
@@ -5699,7 +5699,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="63"/>
       <c r="D36" s="63"/>
@@ -5815,23 +5815,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="165" t="s">
+      <c r="C1" s="132"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="157" t="s">
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="158"/>
-      <c r="L1" s="139" t="s">
+      <c r="K1" s="117"/>
+      <c r="L1" s="142" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5872,7 +5872,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="140"/>
+      <c r="L2" s="143"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5902,11 +5902,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="159" t="str">
+      <c r="C4" s="119" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="160"/>
+      <c r="D4" s="120"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5923,12 +5923,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="159" t="str">
+      <c r="D5" s="119" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="161"/>
-      <c r="F5" s="160"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5945,14 +5945,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="162" t="str">
+      <c r="C6" s="122" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="124"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5965,14 +5965,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="162" t="str">
+      <c r="C7" s="122" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="164"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="124"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -5988,21 +5988,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="162" t="str">
+      <c r="C8" s="122" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="164"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="162" t="str">
+      <c r="I8" s="122" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="171"/>
-      <c r="K8" s="164"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="124"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -6010,14 +6010,14 @@
       <c r="A9" s="118"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="162" t="str">
+      <c r="D9" s="122" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="164"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="124"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -6029,18 +6029,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="172" t="str">
+      <c r="C10" s="138" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="164"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="124"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -6049,14 +6049,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="133" t="str">
+      <c r="C11" s="125" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="127"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6070,14 +6070,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="118"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="133" t="str">
+      <c r="C12" s="125" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="127"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6091,22 +6091,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="118"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="147" t="str">
+      <c r="C13" s="140" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="148"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="149"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="150"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="150"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="141"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="147" t="str">
+      <c r="K13" s="140" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="149"/>
+      <c r="L13" s="141"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6114,40 +6114,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="150" t="str">
+      <c r="C14" s="151" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="151"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="152"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="153"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="150" t="str">
+      <c r="I14" s="151" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="151"/>
-      <c r="K14" s="151"/>
-      <c r="L14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="153"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="118"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="150" t="str">
+      <c r="C15" s="151" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="151"/>
-      <c r="L15" s="152"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="153"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6157,15 +6157,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="153" t="s">
+      <c r="E16" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="156"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -6179,34 +6179,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="119" t="str">
+      <c r="E17" s="160" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="121"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
+      <c r="J17" s="161"/>
+      <c r="K17" s="162"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="118"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="119" t="str">
+      <c r="C18" s="160" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122"/>
-      <c r="K18" s="123"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
+      <c r="H18" s="161"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6216,23 +6216,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="118"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="124" t="str">
+      <c r="C19" s="134" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="126"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="136"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="124" t="str">
+      <c r="I19" s="134" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="125"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="126"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="136"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6241,14 +6241,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="129" t="str">
+      <c r="E20" s="167" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="131"/>
-      <c r="I20" s="132"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
+      <c r="H20" s="169"/>
+      <c r="I20" s="170"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6258,12 +6258,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="141" t="str">
+      <c r="B21" s="144" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="143"/>
+      <c r="C21" s="145"/>
+      <c r="D21" s="146"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6282,11 +6282,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="127" t="str">
+      <c r="C22" s="165" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="128"/>
+      <c r="D22" s="166"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6307,13 +6307,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="136" t="str">
+      <c r="B23" s="171" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="137"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="173"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6333,12 +6333,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="144" t="str">
+      <c r="B24" s="147" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="145"/>
-      <c r="D24" s="146"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="149"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6353,15 +6353,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="115" t="str">
+      <c r="B25" s="157" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="116"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="117"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="159"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6394,24 +6394,43 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="156" t="s">
+      <c r="A27" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="156"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="156"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="156"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="156"/>
-      <c r="J27" s="156"/>
-      <c r="K27" s="156"/>
-      <c r="L27" s="156"/>
-      <c r="M27" s="156"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6428,25 +6447,6 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Bacteria Information worksheet
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72183C7-AEBD-483C-B8E7-F8FC922425F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA1D4B4-1715-4D91-9238-A96913C8E16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="3" r:id="rId1"/>
     <sheet name="Drug Information" sheetId="2" r:id="rId2"/>
-    <sheet name="original antibiogram" sheetId="1" r:id="rId3"/>
+    <sheet name="Bacteria Information" sheetId="4" r:id="rId3"/>
+    <sheet name="original antibiogram" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$O$41</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'original antibiogram'!$A$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'original antibiogram'!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -309,6 +310,12 @@
   </si>
   <si>
     <t>????</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Bacterium</t>
   </si>
 </sst>
 </file>
@@ -1160,6 +1167,129 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1169,9 +1299,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,15 +1317,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1217,15 +1335,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1233,108 +1342,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1343,7 +1350,130 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="74">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1749,7 +1879,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="B2:O39" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}">
     <filterColumn colId="0">
       <filters>
@@ -1789,43 +1919,43 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="70">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FC9C8C68-530C-4012-80B1-959161B27B76}" name="MRSA" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{FC9C8C68-530C-4012-80B1-959161B27B76}" name="MRSA" dataDxfId="69">
       <calculatedColumnFormula>IF('Drug Information'!C2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FBBC04D6-A577-454C-9CA5-71A9E5B59BE9}" name="MSSA" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{FBBC04D6-A577-454C-9CA5-71A9E5B59BE9}" name="MSSA" dataDxfId="68">
       <calculatedColumnFormula>IF('Drug Information'!D2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FE6DE44F-9CCB-4B75-91DD-689C40EFDD60}" name="Streptococci" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{FE6DE44F-9CCB-4B75-91DD-689C40EFDD60}" name="Streptococci" dataDxfId="67">
       <calculatedColumnFormula>IF('Drug Information'!E2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{050D08FE-B7BA-4BA2-9308-9602383C097B}" name="E. coli" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{050D08FE-B7BA-4BA2-9308-9602383C097B}" name="E. coli" dataDxfId="66">
       <calculatedColumnFormula>IF('Drug Information'!F2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0056F4D3-DB47-4738-9938-DDEB05F402A0}" name="P. mirabilis" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{0056F4D3-DB47-4738-9938-DDEB05F402A0}" name="P. mirabilis" dataDxfId="65">
       <calculatedColumnFormula>IF('Drug Information'!G2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61CA5D48-A78B-422A-A1CB-1B458E5C3C92}" name="Klebsiella" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{61CA5D48-A78B-422A-A1CB-1B458E5C3C92}" name="Klebsiella" dataDxfId="64">
       <calculatedColumnFormula>IF('Drug Information'!H2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6157DD55-5AAB-4974-B118-40237915EB0E}" name="Pseudomonas" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{6157DD55-5AAB-4974-B118-40237915EB0E}" name="Pseudomonas" dataDxfId="63">
       <calculatedColumnFormula>IF('Drug Information'!I2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{81D75E20-E7E3-4FBF-9379-ED66BEC6D631}" name="ESCAPPM" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{81D75E20-E7E3-4FBF-9379-ED66BEC6D631}" name="ESCAPPM" dataDxfId="62">
       <calculatedColumnFormula>IF('Drug Information'!J2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58146AC7-0BAA-4A64-8334-7BA8D5AD4463}" name="N. gonorrhoeae" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{58146AC7-0BAA-4A64-8334-7BA8D5AD4463}" name="N. gonorrhoeae" dataDxfId="61">
       <calculatedColumnFormula>IF('Drug Information'!K2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="60">
       <calculatedColumnFormula>IF('Drug Information'!L2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="????" dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="????" dataDxfId="59">
       <calculatedColumnFormula>IF('Drug Information'!M2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="17">
+    <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="58">
       <calculatedColumnFormula>IF('Drug Information'!N2=1,"",".")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{4A3A98C8-EB5C-429F-9790-93036600FBEE}" name="Drug Name "/>
@@ -1835,25 +1965,73 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:N38" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:N38" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="A1:N38" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Drug Class" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Drug Class" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{26BC0B44-2CDD-434A-BE07-8094FD178840}" name="MRSA" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{30A05DE7-E027-4093-81F3-B65078F70278}" name="MSSA" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{B7E03A89-8BD8-46A1-9CCD-C5FDC441C25E}" name="Streptococci" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{4F353AC3-6533-474C-84CB-43F3F2C7D417}" name="E. coli" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{F09E3FC5-B9E6-49B4-B130-38AD917A3F9B}" name="P. mirabilis" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{4A2FA046-CD73-42E3-9500-FD60FA60DAA0}" name="Klebsiella" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{3B345728-E21D-4469-94BD-DF694DC71D17}" name="Pseudomonas" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{09606F38-97F9-4841-8BE1-86E5FD1AC722}" name="ESCAPPM" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{E483C769-170B-4235-B986-875C365387E0}" name="N. gonorrhoeae" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{15D4CCF5-A762-4AFB-BF96-6F78203174D8}" name="N. meningitidis" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{B16ABED2-95DD-46CA-9890-2A863F981C12}" name="Anaerobes" dataDxfId="43"/>
+    <tableColumn id="15" xr3:uid="{9A229B65-C366-4ADD-A51B-85D87DDF2801}" name="Atypicals" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52A18D50-55BF-49E3-A021-8248F804D959}" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:AM13" xr:uid="{52A18D50-55BF-49E3-A021-8248F804D959}"/>
+  <tableColumns count="39">
+    <tableColumn id="1" xr3:uid="{E21DD9BE-77F0-493A-BEF9-0D5BAB602B55}" name="Group" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{C5B0734E-6F00-4374-8898-CC9B96551EB9}" name="Bacterium" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{9EA258EC-76BC-41DE-B7BF-2F0189A59A9B}" name="Benzylpenicillin" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{81F30855-8E50-44A3-83E5-FC5C86B3D9B1}" name="Naficillin" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{8C39ADC0-FA67-4928-BF39-E6A53C9235A1}" name="Oxacillin" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{F82694A7-FF12-47DE-AD72-0A14A3A841AB}" name="Flucloxacillin" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{0B14F92A-37A7-45E6-8B49-E902FFCAD015}" name="Ampicillin" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{40CE8248-0FDC-474D-A236-A40E7590F689}" name="Amoxicillin" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{98411FF7-B840-4E78-A8A2-31014EBD33AC}" name="Amoxicillin-Clavulanic Acid" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{37E13DB0-3F29-48A2-B5CC-0ED97F4BC8B4}" name="Ampicillin/Sulbactam" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{DE7D4547-1413-4E75-A005-4D03C5908199}" name="Piperacillin-Tazobactam" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{8EF8C70D-8733-4940-BED0-69EC3A8589CE}" name="Cefazolin" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{E6B6BF20-8866-4B4B-8361-B3C81245A48A}" name="Cefalexin" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{B3A61893-21A7-4F59-990B-4E0617421B1E}" name="Cefuroxime" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{802060EF-4A4D-4895-A01E-5B44C6EB3623}" name="Cephotetan" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{7697FC5A-491F-4699-A7A1-F9482BC05244}" name="Cefoxitin" dataDxfId="25"/>
+    <tableColumn id="17" xr3:uid="{76937F60-68C7-4C1F-A8BE-B9803814C10D}" name="Cefotaxime" dataDxfId="24"/>
+    <tableColumn id="18" xr3:uid="{06F9D453-1BFE-4CB9-9BF2-8787729F30B7}" name="Ceftriaxone" dataDxfId="23"/>
+    <tableColumn id="19" xr3:uid="{F5AC8ACE-55B4-4566-9598-8CDE9D0D481A}" name="Ceftazidime" dataDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{540D357D-F9C6-451B-B9C1-C1E8A9B44B5C}" name="Cefepime" dataDxfId="21"/>
+    <tableColumn id="21" xr3:uid="{D588F0CE-1624-4B78-B00C-C7FD626EB494}" name="Ceftaroline" dataDxfId="20"/>
+    <tableColumn id="22" xr3:uid="{CFB60770-77F5-424E-A416-DA72F9CACFE3}" name="Ertapenem" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{0476BCDB-5C9A-4D41-8B16-26FC0779AF54}" name="Imipenem" dataDxfId="18"/>
+    <tableColumn id="24" xr3:uid="{A2AD478E-D3DB-4785-8421-BAFDF020555E}" name="Meropenem" dataDxfId="17"/>
+    <tableColumn id="25" xr3:uid="{E5B3A4D6-615B-4734-A542-839D4AAD24CD}" name="Aztreonam" dataDxfId="16"/>
+    <tableColumn id="26" xr3:uid="{FFC6B52C-27F0-48C7-910C-D822F7E7167C}" name="Ciprofloxacin" dataDxfId="15"/>
+    <tableColumn id="27" xr3:uid="{6E7BCB30-CFCC-4DAC-8F05-D74A95340A59}" name="Levofloxacin" dataDxfId="14"/>
+    <tableColumn id="28" xr3:uid="{B9D3A201-9687-4146-A29E-D37876F46631}" name="Moxifloxacin" dataDxfId="13"/>
+    <tableColumn id="29" xr3:uid="{72488A87-C429-4EBA-BB2A-6FCFE04F2498}" name="Gentamicin" dataDxfId="12"/>
+    <tableColumn id="30" xr3:uid="{5DED8E2E-0AA6-453A-81D9-49681C4A83AF}" name="Tobramycin" dataDxfId="11"/>
+    <tableColumn id="31" xr3:uid="{B4F1EE4C-925A-4A9F-9D9E-640A74F73B8F}" name="Amikacin" dataDxfId="10"/>
+    <tableColumn id="32" xr3:uid="{50656037-DD40-4527-89D1-2F741CDFE35C}" name="Azithromycin" dataDxfId="9"/>
+    <tableColumn id="33" xr3:uid="{3E7300E8-67E3-4B2C-B18F-0248121972FC}" name="Clindamycin" dataDxfId="8"/>
+    <tableColumn id="34" xr3:uid="{0762475D-529C-4A84-A91C-5C809A1AC7A7}" name="Doxycycline" dataDxfId="7"/>
+    <tableColumn id="35" xr3:uid="{4ECB7A4C-386B-480A-80AE-D2D428A30F0F}" name="Vancomycin" dataDxfId="6"/>
+    <tableColumn id="36" xr3:uid="{8D2166CD-1907-4165-B598-4DFCF471ABEB}" name="Daptomycin" dataDxfId="5"/>
+    <tableColumn id="37" xr3:uid="{8EF1C304-61CD-4250-96FE-753777AE5BFF}" name="Linezolid" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{6B46FDFD-F2BE-4CCD-ADC3-E165AFC203A6}" name="Trimethoprim/Sulfamethoxazole" dataDxfId="3"/>
+    <tableColumn id="39" xr3:uid="{A20123C8-B4B0-4323-A01A-76D2DA39FE80}" name="Metronidazole" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2126,9 +2304,9 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M2" sqref="M2"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4576,7 +4754,7 @@
     <mergeCell ref="A29:A31"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N39">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4596,7 +4774,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5781,6 +5959,836 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F097ADC-FAEF-4873-942A-675C7470FE68}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AM13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.875" style="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.125" style="64" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.625" style="64" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="64" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.625" style="64" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.75" style="64" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.75" style="64" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" style="64" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.75" style="64" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.625" style="64" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13" style="64" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.75" style="64" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13" style="64" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="13.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.375" style="64" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.25" style="64" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE1" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF1" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI1" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ1" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK1" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" s="64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="64">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="64">
+        <v>1</v>
+      </c>
+      <c r="E3" s="64">
+        <v>1</v>
+      </c>
+      <c r="F3" s="64">
+        <v>1</v>
+      </c>
+      <c r="I3" s="64">
+        <v>1</v>
+      </c>
+      <c r="J3" s="64">
+        <v>1</v>
+      </c>
+      <c r="K3" s="64">
+        <v>1</v>
+      </c>
+      <c r="L3" s="64">
+        <v>1</v>
+      </c>
+      <c r="M3" s="64">
+        <v>1</v>
+      </c>
+      <c r="O3" s="64">
+        <v>1</v>
+      </c>
+      <c r="P3" s="64">
+        <v>1</v>
+      </c>
+      <c r="R3" s="64">
+        <v>1</v>
+      </c>
+      <c r="T3" s="64">
+        <v>1</v>
+      </c>
+      <c r="V3" s="64">
+        <v>1</v>
+      </c>
+      <c r="W3" s="64">
+        <v>1</v>
+      </c>
+      <c r="X3" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="64">
+        <v>1</v>
+      </c>
+      <c r="D4" s="64">
+        <v>1</v>
+      </c>
+      <c r="E4" s="64">
+        <v>1</v>
+      </c>
+      <c r="F4" s="64">
+        <v>1</v>
+      </c>
+      <c r="G4" s="64">
+        <v>1</v>
+      </c>
+      <c r="H4" s="64">
+        <v>1</v>
+      </c>
+      <c r="I4" s="64">
+        <v>1</v>
+      </c>
+      <c r="J4" s="64">
+        <v>1</v>
+      </c>
+      <c r="K4" s="64">
+        <v>1</v>
+      </c>
+      <c r="L4" s="64">
+        <v>1</v>
+      </c>
+      <c r="M4" s="64">
+        <v>1</v>
+      </c>
+      <c r="O4" s="64">
+        <v>1</v>
+      </c>
+      <c r="P4" s="64">
+        <v>1</v>
+      </c>
+      <c r="R4" s="64">
+        <v>1</v>
+      </c>
+      <c r="S4" s="64">
+        <v>1</v>
+      </c>
+      <c r="T4" s="64">
+        <v>1</v>
+      </c>
+      <c r="V4" s="64">
+        <v>1</v>
+      </c>
+      <c r="W4" s="64">
+        <v>1</v>
+      </c>
+      <c r="X4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="64">
+        <v>1</v>
+      </c>
+      <c r="H5" s="64">
+        <v>1</v>
+      </c>
+      <c r="I5" s="64">
+        <v>1</v>
+      </c>
+      <c r="J5" s="64">
+        <v>1</v>
+      </c>
+      <c r="K5" s="64">
+        <v>1</v>
+      </c>
+      <c r="L5" s="64">
+        <v>1</v>
+      </c>
+      <c r="M5" s="64">
+        <v>1</v>
+      </c>
+      <c r="O5" s="64">
+        <v>1</v>
+      </c>
+      <c r="P5" s="64">
+        <v>1</v>
+      </c>
+      <c r="R5" s="64">
+        <v>1</v>
+      </c>
+      <c r="S5" s="64">
+        <v>1</v>
+      </c>
+      <c r="T5" s="64">
+        <v>1</v>
+      </c>
+      <c r="V5" s="64">
+        <v>1</v>
+      </c>
+      <c r="W5" s="64">
+        <v>1</v>
+      </c>
+      <c r="X5" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="64">
+        <v>1</v>
+      </c>
+      <c r="H6" s="64">
+        <v>1</v>
+      </c>
+      <c r="I6" s="64">
+        <v>1</v>
+      </c>
+      <c r="J6" s="64">
+        <v>1</v>
+      </c>
+      <c r="K6" s="64">
+        <v>1</v>
+      </c>
+      <c r="L6" s="64">
+        <v>1</v>
+      </c>
+      <c r="M6" s="64">
+        <v>1</v>
+      </c>
+      <c r="O6" s="64">
+        <v>1</v>
+      </c>
+      <c r="P6" s="64">
+        <v>1</v>
+      </c>
+      <c r="R6" s="64">
+        <v>1</v>
+      </c>
+      <c r="S6" s="64">
+        <v>1</v>
+      </c>
+      <c r="T6" s="64">
+        <v>1</v>
+      </c>
+      <c r="V6" s="64">
+        <v>1</v>
+      </c>
+      <c r="W6" s="64">
+        <v>1</v>
+      </c>
+      <c r="X6" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="64">
+        <v>1</v>
+      </c>
+      <c r="J7" s="64">
+        <v>1</v>
+      </c>
+      <c r="K7" s="64">
+        <v>1</v>
+      </c>
+      <c r="L7" s="64">
+        <v>1</v>
+      </c>
+      <c r="M7" s="64">
+        <v>1</v>
+      </c>
+      <c r="O7" s="64">
+        <v>1</v>
+      </c>
+      <c r="P7" s="64">
+        <v>1</v>
+      </c>
+      <c r="R7" s="64">
+        <v>1</v>
+      </c>
+      <c r="S7" s="64">
+        <v>1</v>
+      </c>
+      <c r="T7" s="64">
+        <v>1</v>
+      </c>
+      <c r="V7" s="64">
+        <v>1</v>
+      </c>
+      <c r="W7" s="64">
+        <v>1</v>
+      </c>
+      <c r="X7" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="64">
+        <v>1</v>
+      </c>
+      <c r="S8" s="64">
+        <v>1</v>
+      </c>
+      <c r="T8" s="64">
+        <v>1</v>
+      </c>
+      <c r="W8" s="64">
+        <v>1</v>
+      </c>
+      <c r="X8" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="64">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="64">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="64">
+        <v>1</v>
+      </c>
+      <c r="R9" s="64">
+        <v>1</v>
+      </c>
+      <c r="T9" s="64">
+        <v>1</v>
+      </c>
+      <c r="V9" s="64">
+        <v>1</v>
+      </c>
+      <c r="W9" s="64">
+        <v>1</v>
+      </c>
+      <c r="X9" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="64">
+        <v>1</v>
+      </c>
+      <c r="T10" s="64">
+        <v>1</v>
+      </c>
+      <c r="V10" s="64">
+        <v>1</v>
+      </c>
+      <c r="W10" s="64">
+        <v>1</v>
+      </c>
+      <c r="X10" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="64">
+        <v>1</v>
+      </c>
+      <c r="H11" s="64">
+        <v>1</v>
+      </c>
+      <c r="K11" s="64">
+        <v>1</v>
+      </c>
+      <c r="R11" s="64">
+        <v>1</v>
+      </c>
+      <c r="T11" s="64">
+        <v>1</v>
+      </c>
+      <c r="V11" s="64">
+        <v>1</v>
+      </c>
+      <c r="W11" s="64">
+        <v>1</v>
+      </c>
+      <c r="X11" s="64">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="64">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="64">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL11" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="64">
+        <v>1</v>
+      </c>
+      <c r="J12" s="64">
+        <v>1</v>
+      </c>
+      <c r="K12" s="64">
+        <v>1</v>
+      </c>
+      <c r="O12" s="64">
+        <v>1</v>
+      </c>
+      <c r="P12" s="64">
+        <v>1</v>
+      </c>
+      <c r="V12" s="64">
+        <v>1</v>
+      </c>
+      <c r="W12" s="64">
+        <v>1</v>
+      </c>
+      <c r="X12" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="64">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" s="64">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="64">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="64">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="64">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -5815,23 +6823,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="128" t="s">
+      <c r="C1" s="169"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="165" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="116" t="s">
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="117"/>
-      <c r="L1" s="142" t="s">
+      <c r="K1" s="158"/>
+      <c r="L1" s="139" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5872,7 +6880,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="143"/>
+      <c r="L2" s="140"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5902,11 +6910,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="119" t="str">
+      <c r="C4" s="159" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="120"/>
+      <c r="D4" s="160"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5923,12 +6931,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="119" t="str">
+      <c r="D5" s="159" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="121"/>
-      <c r="F5" s="120"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="160"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5945,14 +6953,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="122" t="str">
+      <c r="C6" s="162" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="124"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5965,14 +6973,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="122" t="str">
+      <c r="C7" s="162" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="124"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -5988,21 +6996,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="122" t="str">
+      <c r="C8" s="162" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="124"/>
+      <c r="D8" s="171"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="122" t="str">
+      <c r="I8" s="162" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="137"/>
-      <c r="K8" s="124"/>
+      <c r="J8" s="171"/>
+      <c r="K8" s="164"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -6010,14 +7018,14 @@
       <c r="A9" s="118"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="122" t="str">
+      <c r="D9" s="162" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="124"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="164"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -6029,18 +7037,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="138" t="str">
+      <c r="C10" s="172" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="139"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="137"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="124"/>
+      <c r="D10" s="173"/>
+      <c r="E10" s="173"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="164"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -6049,14 +7057,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="125" t="str">
+      <c r="C11" s="133" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="127"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6070,14 +7078,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="118"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="125" t="str">
+      <c r="C12" s="133" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="127"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="135"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6091,22 +7099,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="118"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="140" t="str">
+      <c r="C13" s="147" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="141"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="149"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="140" t="str">
+      <c r="K13" s="147" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="141"/>
+      <c r="L13" s="149"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6114,40 +7122,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="151" t="str">
+      <c r="C14" s="150" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="152"/>
-      <c r="E14" s="152"/>
-      <c r="F14" s="152"/>
-      <c r="G14" s="153"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="152"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="151" t="str">
+      <c r="I14" s="150" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="152"/>
-      <c r="K14" s="152"/>
-      <c r="L14" s="153"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="151"/>
+      <c r="L14" s="152"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="118"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="151" t="str">
+      <c r="C15" s="150" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="152"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="152"/>
-      <c r="J15" s="152"/>
-      <c r="K15" s="152"/>
-      <c r="L15" s="153"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="152"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6157,15 +7165,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="155"/>
-      <c r="G16" s="155"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="155"/>
-      <c r="J16" s="155"/>
-      <c r="K16" s="156"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="155"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -6179,34 +7187,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="160" t="str">
+      <c r="E17" s="119" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="162"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="121"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="118"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="160" t="str">
+      <c r="C18" s="119" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="161"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-      <c r="G18" s="161"/>
-      <c r="H18" s="161"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="164"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="123"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6216,23 +7224,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="118"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="134" t="str">
+      <c r="C19" s="124" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="136"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="126"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="134" t="str">
+      <c r="I19" s="124" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="136"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="125"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="126"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6241,14 +7249,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="167" t="str">
+      <c r="E20" s="129" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="170"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="131"/>
+      <c r="I20" s="132"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6258,12 +7266,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="144" t="str">
+      <c r="B21" s="141" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="145"/>
-      <c r="D21" s="146"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="143"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6282,11 +7290,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="165" t="str">
+      <c r="C22" s="127" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="166"/>
+      <c r="D22" s="128"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6307,13 +7315,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="171" t="str">
+      <c r="B23" s="136" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="172"/>
-      <c r="D23" s="172"/>
-      <c r="E23" s="173"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="138"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6333,12 +7341,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="147" t="str">
+      <c r="B24" s="144" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="148"/>
-      <c r="D24" s="149"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="146"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6353,15 +7361,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="157" t="str">
+      <c r="B25" s="115" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="159"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="117"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6394,43 +7402,24 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="115" t="s">
+      <c r="A27" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="115"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="115"/>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="156"/>
+      <c r="D27" s="156"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="156"/>
+      <c r="I27" s="156"/>
+      <c r="J27" s="156"/>
+      <c r="K27" s="156"/>
+      <c r="L27" s="156"/>
+      <c r="M27" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6447,6 +7436,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct errors in bacteria naming
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E279D67-257F-44B1-8BA6-01DA86FE4825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE3C320-406C-4537-B491-87D1C6182A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="3" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Gram negative bacilli</t>
+  </si>
+  <si>
+    <t>Gram negative cocci</t>
   </si>
 </sst>
 </file>
@@ -2066,7 +2072,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1:N1"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4533,7 +4539,7 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
@@ -4863,8 +4869,8 @@
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5212,7 +5218,7 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B5" s="64" t="s">
         <v>23</v>
@@ -5292,7 +5298,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B6" s="64" t="s">
         <v>22</v>
@@ -5369,7 +5375,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B7" s="64" t="s">
         <v>40</v>
@@ -5440,7 +5446,7 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B8" s="64" t="s">
         <v>4</v>
@@ -5481,7 +5487,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>5</v>
@@ -5531,7 +5537,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B10" s="64" t="s">
         <v>8</v>
@@ -5566,7 +5572,7 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B11" s="64" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Update coverage of Cefuroxime, Cefotaxime, Ceftaroline, Daptomycin, and Linezolid
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE3C320-406C-4537-B491-87D1C6182A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="3" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$O$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'original antibiogram'!$A$1:$M$27</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,14 +37,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -327,7 +321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -835,7 +829,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1173,31 +1167,61 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1209,40 +1233,19 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1269,15 +1272,9 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1296,59 +1293,59 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1357,16 +1354,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="62">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1504,7 +1491,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1523,7 +1509,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1542,7 +1527,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1561,7 +1545,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1632,6 +1615,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -1657,8 +1650,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="B2:O39" xr:uid="{D3A226D6-0154-404A-9404-A7E04AA3E622}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+  <autoFilter ref="B2:O39">
     <filterColumn colId="0">
       <filters>
         <filter val="Amikacin"/>
@@ -1697,105 +1690,105 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6F09EC5A-4B84-4EAD-A69B-652D3181E954}" name="Drug Name" dataDxfId="58">
+    <tableColumn id="1" name="Drug Name" dataDxfId="57">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FC9C8C68-530C-4012-80B1-959161B27B76}" name="MRSA" dataDxfId="57">
+    <tableColumn id="2" name="MRSA" dataDxfId="56">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FBBC04D6-A577-454C-9CA5-71A9E5B59BE9}" name="MSSA" dataDxfId="56">
+    <tableColumn id="3" name="MSSA" dataDxfId="55">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FE6DE44F-9CCB-4B75-91DD-689C40EFDD60}" name="Streptococci" dataDxfId="55">
+    <tableColumn id="4" name="Streptococci" dataDxfId="54">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{050D08FE-B7BA-4BA2-9308-9602383C097B}" name="E. coli" dataDxfId="54">
+    <tableColumn id="5" name="E. coli" dataDxfId="53">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0056F4D3-DB47-4738-9938-DDEB05F402A0}" name="P. mirabilis" dataDxfId="53">
+    <tableColumn id="6" name="P. mirabilis" dataDxfId="52">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61CA5D48-A78B-422A-A1CB-1B458E5C3C92}" name="Klebsiella" dataDxfId="52">
+    <tableColumn id="7" name="Klebsiella" dataDxfId="51">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6157DD55-5AAB-4974-B118-40237915EB0E}" name="Pseudomonas" dataDxfId="51">
+    <tableColumn id="8" name="Pseudomonas" dataDxfId="50">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{81D75E20-E7E3-4FBF-9379-ED66BEC6D631}" name="ESCAPPM" dataDxfId="50">
+    <tableColumn id="9" name="ESCAPPM" dataDxfId="49">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58146AC7-0BAA-4A64-8334-7BA8D5AD4463}" name="N. gonorrhoeae" dataDxfId="49">
+    <tableColumn id="10" name="N. gonorrhoeae" dataDxfId="48">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{ABFF55F7-1832-482A-9FA5-A335EB46FCD6}" name="N. meningitidis" dataDxfId="48">
+    <tableColumn id="11" name="N. meningitidis" dataDxfId="47">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2396FCAD-7999-4DB4-B260-245463F60D8D}" name="????" dataDxfId="47">
+    <tableColumn id="12" name="????" dataDxfId="46">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A5F9D043-95B7-46A3-BE9B-8FE40ABAFB54}" name="e.g. Mycoplasma" dataDxfId="46">
+    <tableColumn id="13" name="e.g. Mycoplasma" dataDxfId="45">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{4A3A98C8-EB5C-429F-9790-93036600FBEE}" name="Drug Name "/>
+    <tableColumn id="14" name="Drug Name "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <autoFilter ref="A1:B38" xr:uid="{A003E1BB-F418-4253-8616-E065F4FDC632}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A1:B38"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A2613E87-CAB7-4CC0-B9B9-53C34B8BCE6C}" name="Drug Name" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{B4BE1605-B374-4455-846C-4E6604A68083}" name="Drug Class" dataDxfId="42"/>
+    <tableColumn id="1" name="Drug Name" dataDxfId="42"/>
+    <tableColumn id="2" name="Drug Class" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52A18D50-55BF-49E3-A021-8248F804D959}" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:AM13" xr:uid="{52A18D50-55BF-49E3-A021-8248F804D959}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:AM13"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{E21DD9BE-77F0-493A-BEF9-0D5BAB602B55}" name="Group" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{C5B0734E-6F00-4374-8898-CC9B96551EB9}" name="Name" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{9EA258EC-76BC-41DE-B7BF-2F0189A59A9B}" name="Benzylpenicillin" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{81F30855-8E50-44A3-83E5-FC5C86B3D9B1}" name="Naficillin" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{8C39ADC0-FA67-4928-BF39-E6A53C9235A1}" name="Oxacillin" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{F82694A7-FF12-47DE-AD72-0A14A3A841AB}" name="Flucloxacillin" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{0B14F92A-37A7-45E6-8B49-E902FFCAD015}" name="Ampicillin" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{40CE8248-0FDC-474D-A236-A40E7590F689}" name="Amoxicillin" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{98411FF7-B840-4E78-A8A2-31014EBD33AC}" name="Amoxicillin-Clavulanic Acid" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{37E13DB0-3F29-48A2-B5CC-0ED97F4BC8B4}" name="Ampicillin/Sulbactam" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{DE7D4547-1413-4E75-A005-4D03C5908199}" name="Piperacillin-Tazobactam" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{8EF8C70D-8733-4940-BED0-69EC3A8589CE}" name="Cefazolin" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{E6B6BF20-8866-4B4B-8361-B3C81245A48A}" name="Cefalexin" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{B3A61893-21A7-4F59-990B-4E0617421B1E}" name="Cefuroxime" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{802060EF-4A4D-4895-A01E-5B44C6EB3623}" name="Cephotetan" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{7697FC5A-491F-4699-A7A1-F9482BC05244}" name="Cefoxitin" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{76937F60-68C7-4C1F-A8BE-B9803814C10D}" name="Cefotaxime" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{06F9D453-1BFE-4CB9-9BF2-8787729F30B7}" name="Ceftriaxone" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{F5AC8ACE-55B4-4566-9598-8CDE9D0D481A}" name="Ceftazidime" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{540D357D-F9C6-451B-B9C1-C1E8A9B44B5C}" name="Cefepime" dataDxfId="22"/>
-    <tableColumn id="21" xr3:uid="{D588F0CE-1624-4B78-B00C-C7FD626EB494}" name="Ceftaroline" dataDxfId="21"/>
-    <tableColumn id="22" xr3:uid="{CFB60770-77F5-424E-A416-DA72F9CACFE3}" name="Ertapenem" dataDxfId="20"/>
-    <tableColumn id="23" xr3:uid="{0476BCDB-5C9A-4D41-8B16-26FC0779AF54}" name="Imipenem" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{A2AD478E-D3DB-4785-8421-BAFDF020555E}" name="Meropenem" dataDxfId="18"/>
-    <tableColumn id="25" xr3:uid="{E5B3A4D6-615B-4734-A542-839D4AAD24CD}" name="Aztreonam" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{FFC6B52C-27F0-48C7-910C-D822F7E7167C}" name="Ciprofloxacin" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{6E7BCB30-CFCC-4DAC-8F05-D74A95340A59}" name="Levofloxacin" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{B9D3A201-9687-4146-A29E-D37876F46631}" name="Moxifloxacin" dataDxfId="14"/>
-    <tableColumn id="29" xr3:uid="{72488A87-C429-4EBA-BB2A-6FCFE04F2498}" name="Gentamicin" dataDxfId="13"/>
-    <tableColumn id="30" xr3:uid="{5DED8E2E-0AA6-453A-81D9-49681C4A83AF}" name="Tobramycin" dataDxfId="12"/>
-    <tableColumn id="31" xr3:uid="{B4F1EE4C-925A-4A9F-9D9E-640A74F73B8F}" name="Amikacin" dataDxfId="11"/>
-    <tableColumn id="32" xr3:uid="{50656037-DD40-4527-89D1-2F741CDFE35C}" name="Azithromycin" dataDxfId="10"/>
-    <tableColumn id="33" xr3:uid="{3E7300E8-67E3-4B2C-B18F-0248121972FC}" name="Clindamycin" dataDxfId="9"/>
-    <tableColumn id="34" xr3:uid="{0762475D-529C-4A84-A91C-5C809A1AC7A7}" name="Doxycycline" dataDxfId="8"/>
-    <tableColumn id="35" xr3:uid="{4ECB7A4C-386B-480A-80AE-D2D428A30F0F}" name="Vancomycin" dataDxfId="7"/>
-    <tableColumn id="36" xr3:uid="{8D2166CD-1907-4165-B598-4DFCF471ABEB}" name="Daptomycin" dataDxfId="6"/>
-    <tableColumn id="37" xr3:uid="{8EF1C304-61CD-4250-96FE-753777AE5BFF}" name="Linezolid" dataDxfId="5"/>
-    <tableColumn id="38" xr3:uid="{6B46FDFD-F2BE-4CCD-ADC3-E165AFC203A6}" name="Trimethoprim/Sulfamethoxazole" dataDxfId="4"/>
-    <tableColumn id="39" xr3:uid="{A20123C8-B4B0-4323-A01A-76D2DA39FE80}" name="Metronidazole" dataDxfId="3"/>
+    <tableColumn id="1" name="Group" dataDxfId="38"/>
+    <tableColumn id="2" name="Name" dataDxfId="37"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="36"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="35"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="34"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="33"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="32"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="31"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="30"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="29"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="28"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="27"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="26"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="25"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="24"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="23"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="22"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="21"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="20"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="19"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="18"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="17"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="16"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="15"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="14"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="13"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="12"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="11"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="10"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="9"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="8"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="7"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="6"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="5"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="4"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="3"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="2"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="1"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2056,14 +2049,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38DBB59-9153-4008-AD05-F81C07E1E687}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -4520,7 +4513,7 @@
     <mergeCell ref="A29:A31"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N39">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4533,14 +4526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5474896F-AAD3-451A-94EF-CDE00ADCB149}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4647,10 +4640,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="174" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="174" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4863,19 +4856,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F097ADC-FAEF-4873-942A-675C7470FE68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <pane xSplit="4260" ySplit="7875" topLeftCell="AA25" activePane="topRight"/>
+      <selection pane="topRight" activeCell="AK5" sqref="AK5"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.375" style="64" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.25" style="64" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.375" style="64" bestFit="1" customWidth="1"/>
@@ -5040,6 +5036,9 @@
       <c r="B2" s="64" t="s">
         <v>1</v>
       </c>
+      <c r="U2" s="64">
+        <v>1</v>
+      </c>
       <c r="AG2" s="64">
         <v>1</v>
       </c>
@@ -5047,6 +5046,12 @@
         <v>1</v>
       </c>
       <c r="AI2" s="64">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="64">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="64">
         <v>1</v>
       </c>
       <c r="AL2" s="64">
@@ -5084,18 +5089,27 @@
       <c r="M3" s="64">
         <v>1</v>
       </c>
+      <c r="N3" s="64">
+        <v>1</v>
+      </c>
       <c r="O3" s="64">
         <v>1</v>
       </c>
       <c r="P3" s="64">
         <v>1</v>
       </c>
+      <c r="Q3" s="64">
+        <v>1</v>
+      </c>
       <c r="R3" s="64">
         <v>1</v>
       </c>
       <c r="T3" s="64">
         <v>1</v>
       </c>
+      <c r="U3" s="64">
+        <v>1</v>
+      </c>
       <c r="V3" s="64">
         <v>1</v>
       </c>
@@ -5124,6 +5138,12 @@
         <v>1</v>
       </c>
       <c r="AI3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="64">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="64">
         <v>1</v>
       </c>
       <c r="AL3" s="64">
@@ -5170,12 +5190,18 @@
       <c r="M4" s="64">
         <v>1</v>
       </c>
+      <c r="N4" s="64">
+        <v>1</v>
+      </c>
       <c r="O4" s="64">
         <v>1</v>
       </c>
       <c r="P4" s="64">
         <v>1</v>
       </c>
+      <c r="Q4" s="64">
+        <v>1</v>
+      </c>
       <c r="R4" s="64">
         <v>1</v>
       </c>
@@ -5185,6 +5211,9 @@
       <c r="T4" s="64">
         <v>1</v>
       </c>
+      <c r="U4" s="64">
+        <v>1</v>
+      </c>
       <c r="V4" s="64">
         <v>1</v>
       </c>
@@ -5210,6 +5239,12 @@
         <v>1</v>
       </c>
       <c r="AI4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="64">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="64">
         <v>1</v>
       </c>
       <c r="AL4" s="64">
@@ -5244,12 +5279,18 @@
       <c r="M5" s="64">
         <v>1</v>
       </c>
+      <c r="N5" s="64">
+        <v>1</v>
+      </c>
       <c r="O5" s="64">
         <v>1</v>
       </c>
       <c r="P5" s="64">
         <v>1</v>
       </c>
+      <c r="Q5" s="64">
+        <v>1</v>
+      </c>
       <c r="R5" s="64">
         <v>1</v>
       </c>
@@ -5257,6 +5298,9 @@
         <v>1</v>
       </c>
       <c r="T5" s="64">
+        <v>1</v>
+      </c>
+      <c r="U5" s="64">
         <v>1</v>
       </c>
       <c r="V5" s="64">
@@ -5324,12 +5368,18 @@
       <c r="M6" s="64">
         <v>1</v>
       </c>
+      <c r="N6" s="64">
+        <v>1</v>
+      </c>
       <c r="O6" s="64">
         <v>1</v>
       </c>
       <c r="P6" s="64">
         <v>1</v>
       </c>
+      <c r="Q6" s="64">
+        <v>1</v>
+      </c>
       <c r="R6" s="64">
         <v>1</v>
       </c>
@@ -5337,6 +5387,9 @@
         <v>1</v>
       </c>
       <c r="T6" s="64">
+        <v>1</v>
+      </c>
+      <c r="U6" s="64">
         <v>1</v>
       </c>
       <c r="V6" s="64">
@@ -5395,12 +5448,18 @@
       <c r="M7" s="64">
         <v>1</v>
       </c>
+      <c r="N7" s="64">
+        <v>1</v>
+      </c>
       <c r="O7" s="64">
         <v>1</v>
       </c>
       <c r="P7" s="64">
         <v>1</v>
       </c>
+      <c r="Q7" s="64">
+        <v>1</v>
+      </c>
       <c r="R7" s="64">
         <v>1</v>
       </c>
@@ -5408,6 +5467,9 @@
         <v>1</v>
       </c>
       <c r="T7" s="64">
+        <v>1</v>
+      </c>
+      <c r="U7" s="64">
         <v>1</v>
       </c>
       <c r="V7" s="64">
@@ -5495,12 +5557,18 @@
       <c r="K9" s="64">
         <v>1</v>
       </c>
+      <c r="Q9" s="64">
+        <v>1</v>
+      </c>
       <c r="R9" s="64">
         <v>1</v>
       </c>
       <c r="T9" s="64">
         <v>1</v>
       </c>
+      <c r="U9" s="64">
+        <v>1</v>
+      </c>
       <c r="V9" s="64">
         <v>1</v>
       </c>
@@ -5529,6 +5597,12 @@
         <v>1</v>
       </c>
       <c r="AE9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="64">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="64">
         <v>1</v>
       </c>
       <c r="AL9" s="64">
@@ -5584,6 +5658,9 @@
         <v>1</v>
       </c>
       <c r="K11" s="64">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="64">
         <v>1</v>
       </c>
       <c r="R11" s="64">
@@ -5693,7 +5770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -5727,23 +5804,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="165" t="s">
+      <c r="C1" s="132"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="157" t="s">
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="158"/>
-      <c r="L1" s="139" t="s">
+      <c r="K1" s="117"/>
+      <c r="L1" s="142" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5784,7 +5861,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="140"/>
+      <c r="L2" s="143"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5814,11 +5891,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="159" t="str">
+      <c r="C4" s="119" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="160"/>
+      <c r="D4" s="120"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5835,12 +5912,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="159" t="str">
+      <c r="D5" s="119" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="161"/>
-      <c r="F5" s="160"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5857,14 +5934,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="162" t="str">
+      <c r="C6" s="122" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="124"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5877,14 +5954,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="162" t="str">
+      <c r="C7" s="122" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="164"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="124"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -5900,21 +5977,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="162" t="str">
+      <c r="C8" s="122" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="164"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="162" t="str">
+      <c r="I8" s="122" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="171"/>
-      <c r="K8" s="164"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="124"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -5922,14 +5999,14 @@
       <c r="A9" s="118"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="162" t="str">
+      <c r="D9" s="122" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="164"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="124"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -5941,18 +6018,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="172" t="str">
+      <c r="C10" s="138" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="164"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="124"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -5961,14 +6038,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="133" t="str">
+      <c r="C11" s="125" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="127"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -5982,14 +6059,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="118"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="133" t="str">
+      <c r="C12" s="125" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="127"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6003,22 +6080,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="118"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="147" t="str">
+      <c r="C13" s="140" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="148"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="149"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="150"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="150"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="141"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="147" t="str">
+      <c r="K13" s="140" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="149"/>
+      <c r="L13" s="141"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6026,40 +6103,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="150" t="str">
+      <c r="C14" s="151" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="151"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="152"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="153"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="150" t="str">
+      <c r="I14" s="151" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="151"/>
-      <c r="K14" s="151"/>
-      <c r="L14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="153"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="118"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="150" t="str">
+      <c r="C15" s="151" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="151"/>
-      <c r="L15" s="152"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="153"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6069,15 +6146,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="153" t="s">
+      <c r="E16" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="156"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -6091,34 +6168,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="119" t="str">
+      <c r="E17" s="160" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="121"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
+      <c r="J17" s="161"/>
+      <c r="K17" s="162"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="118"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="119" t="str">
+      <c r="C18" s="160" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122"/>
-      <c r="K18" s="123"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
+      <c r="H18" s="161"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6128,23 +6205,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="118"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="124" t="str">
+      <c r="C19" s="134" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="126"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="136"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="124" t="str">
+      <c r="I19" s="134" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="125"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="126"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="136"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6153,14 +6230,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="129" t="str">
+      <c r="E20" s="167" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="131"/>
-      <c r="I20" s="132"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
+      <c r="H20" s="169"/>
+      <c r="I20" s="170"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6170,12 +6247,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="141" t="str">
+      <c r="B21" s="144" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="143"/>
+      <c r="C21" s="145"/>
+      <c r="D21" s="146"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6194,11 +6271,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="127" t="str">
+      <c r="C22" s="165" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="128"/>
+      <c r="D22" s="166"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6219,13 +6296,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="136" t="str">
+      <c r="B23" s="171" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="137"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="173"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6245,12 +6322,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="144" t="str">
+      <c r="B24" s="147" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="145"/>
-      <c r="D24" s="146"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="149"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6265,15 +6342,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="115" t="str">
+      <c r="B25" s="157" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="116"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="117"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="159"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6306,24 +6383,43 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="156" t="s">
+      <c r="A27" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="156"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="156"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="156"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="156"/>
-      <c r="J27" s="156"/>
-      <c r="K27" s="156"/>
-      <c r="L27" s="156"/>
-      <c r="M27" s="156"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6340,25 +6436,6 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add anaerobe & atypical examples
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30415803-AAE2-4458-9F45-C6CD7BAA9230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="3" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$O$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'original antibiogram'!$A$1:$M$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,14 +43,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -59,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -316,12 +322,18 @@
   </si>
   <si>
     <t>Gram negative cocci</t>
+  </si>
+  <si>
+    <t>e.g. Bacteroides sp.</t>
+  </si>
+  <si>
+    <t>e.g. Mycoplasma sp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -823,7 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1158,6 +1170,129 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1167,9 +1302,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,15 +1320,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1215,15 +1338,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1232,114 +1346,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1348,6 +1354,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="62">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1609,16 +1625,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -1644,8 +1650,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
-  <autoFilter ref="B2:O39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B2:O39" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Amikacin"/>
@@ -1684,105 +1690,105 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="Drug Name" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Drug Name" dataDxfId="58">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="MRSA" dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MRSA" dataDxfId="57">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="MSSA" dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MSSA" dataDxfId="56">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Streptococci" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Streptococci" dataDxfId="55">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="E. coli" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E. coli" dataDxfId="54">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="P. mirabilis" dataDxfId="52">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="P. mirabilis" dataDxfId="53">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Klebsiella" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Klebsiella" dataDxfId="52">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Pseudomonas" dataDxfId="50">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Pseudomonas" dataDxfId="51">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="ESCAPPM" dataDxfId="49">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ESCAPPM" dataDxfId="50">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="N. gonorrhoeae" dataDxfId="48">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="N. gonorrhoeae" dataDxfId="49">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="N. meningitidis" dataDxfId="47">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="N. meningitidis" dataDxfId="48">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="????" dataDxfId="46">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="????" dataDxfId="47">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="e.g. Mycoplasma" dataDxfId="45">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="e.g. Mycoplasma" dataDxfId="46">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Drug Name "/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Drug Name "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A1:B38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Drug Name" dataDxfId="42"/>
-    <tableColumn id="2" name="Drug Class" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Drug Name" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Drug Class" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:AM13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:AM13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="39">
-    <tableColumn id="1" name="Group" dataDxfId="38"/>
-    <tableColumn id="2" name="Name" dataDxfId="37"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="36"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="35"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="34"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="33"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="32"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="31"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="30"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="29"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="28"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="27"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="26"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="25"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="24"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="23"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="22"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="21"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="20"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="19"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="18"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="17"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="16"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="15"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="14"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="13"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="12"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="11"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="10"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="9"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="8"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="7"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="6"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="5"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="4"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="3"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="2"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="1"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Group" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Benzylpenicillin" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Naficillin" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Oxacillin" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Flucloxacillin" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Ampicillin" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Amoxicillin" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Amoxicillin-Clavulanic Acid" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Ampicillin/Sulbactam" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Piperacillin-Tazobactam" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Cefazolin" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Cefalexin" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Cefuroxime" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Cephotetan" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Cefoxitin" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Cefotaxime" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ceftriaxone" dataDxfId="22"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Ceftazidime" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Cefepime" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Ceftaroline" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Ertapenem" dataDxfId="18"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="Imipenem" dataDxfId="17"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="Meropenem" dataDxfId="16"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Aztreonam" dataDxfId="15"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="Ciprofloxacin" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Levofloxacin" dataDxfId="13"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="Moxifloxacin" dataDxfId="12"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="Gentamicin" dataDxfId="11"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="Tobramycin" dataDxfId="10"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="Amikacin" dataDxfId="9"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0200-000020000000}" name="Azithromycin" dataDxfId="8"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0200-000021000000}" name="Clindamycin" dataDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0200-000022000000}" name="Doxycycline" dataDxfId="6"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0200-000023000000}" name="Vancomycin" dataDxfId="5"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0200-000024000000}" name="Daptomycin" dataDxfId="4"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0200-000025000000}" name="Linezolid" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0200-000026000000}" name="Trimethoprim/Sulfamethoxazole" dataDxfId="2"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0200-000027000000}" name="Metronidazole" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2043,14 +2049,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -4507,7 +4513,7 @@
     <mergeCell ref="A29:A31"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N39">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4520,13 +4526,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -4634,10 +4640,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="173" t="s">
+      <c r="A13" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="173" t="s">
+      <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4650,204 +4656,196 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="173" t="s">
+      <c r="A15" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="173" t="s">
+      <c r="B16" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="173" t="s">
+      <c r="A17" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="173" t="s">
+      <c r="B17" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="173" t="s">
+      <c r="A18" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="173" t="s">
+      <c r="B18" s="31" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="173" t="s">
+      <c r="A19" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="173" t="s">
+      <c r="B19" s="31" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="173" t="s">
+      <c r="A20" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="31" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="173" t="s">
+      <c r="A21" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="173" t="s">
+      <c r="B21" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="173" t="s">
+      <c r="A22" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="173" t="s">
+      <c r="B22" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="173" t="s">
+      <c r="A23" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="173" t="s">
+      <c r="B23" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="173" t="s">
+      <c r="A24" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="173" t="s">
+      <c r="B24" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="173" t="s">
+      <c r="A25" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="173" t="s">
+      <c r="B25" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="173" t="s">
+      <c r="A26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="173" t="s">
+      <c r="A27" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="173" t="s">
+      <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="173" t="s">
+      <c r="A28" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="173" t="s">
+      <c r="A29" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="173" t="s">
+      <c r="B29" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="173" t="s">
+      <c r="A30" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="173" t="s">
+      <c r="A31" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="173" t="s">
+      <c r="B31" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="173" t="s">
+      <c r="A32" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="173" t="s">
+      <c r="B32" s="31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="173" t="s">
+      <c r="A33" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="173" t="s">
+      <c r="B33" s="31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="173" t="s">
+      <c r="A34" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="173" t="s">
+      <c r="B34" s="31" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="173" t="s">
+      <c r="A35" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="173" t="s">
+      <c r="B35" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="173" t="s">
+      <c r="A36" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="173" t="s">
+      <c r="B36" s="31" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="173" t="s">
+      <c r="A37" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="173" t="s">
+      <c r="B37" s="31" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="173" t="s">
+      <c r="A38" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="173" t="s">
+      <c r="B38" s="31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="174"/>
-      <c r="B39" s="174"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="174"/>
-      <c r="B40" s="174"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4858,24 +4856,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="10320" ySplit="7875" topLeftCell="A25"/>
-      <selection activeCell="AF17" sqref="AF17"/>
+      <selection activeCell="C21" sqref="C21"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.375" style="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.25" style="63" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.375" style="63" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.125" style="63" bestFit="1" customWidth="1"/>
@@ -5708,7 +5706,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="I12" s="63">
         <v>1</v>
@@ -5749,7 +5747,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="AA13" s="63">
         <v>1</v>
@@ -5773,7 +5771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -5807,23 +5805,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="127" t="s">
+      <c r="C1" s="168"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="115" t="s">
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="116"/>
-      <c r="L1" s="141" t="s">
+      <c r="K1" s="157"/>
+      <c r="L1" s="138" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5864,7 +5862,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="142"/>
+      <c r="L2" s="139"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5894,11 +5892,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="118" t="str">
+      <c r="C4" s="158" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="119"/>
+      <c r="D4" s="159"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5915,12 +5913,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="118" t="str">
+      <c r="D5" s="158" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="120"/>
-      <c r="F5" s="119"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="159"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5937,14 +5935,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="121" t="str">
+      <c r="C6" s="161" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="123"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5957,14 +5955,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="121" t="str">
+      <c r="C7" s="161" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="123"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -5980,21 +5978,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="121" t="str">
+      <c r="C8" s="161" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="123"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="121" t="str">
+      <c r="I8" s="161" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="136"/>
-      <c r="K8" s="123"/>
+      <c r="J8" s="170"/>
+      <c r="K8" s="163"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -6002,14 +6000,14 @@
       <c r="A9" s="117"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="121" t="str">
+      <c r="D9" s="161" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="123"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="163"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -6021,18 +6019,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="137" t="str">
+      <c r="C10" s="171" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="136"/>
-      <c r="K10" s="123"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="170"/>
+      <c r="I10" s="170"/>
+      <c r="J10" s="170"/>
+      <c r="K10" s="163"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -6041,14 +6039,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="124" t="str">
+      <c r="C11" s="132" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="126"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="134"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6062,14 +6060,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="117"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="124" t="str">
+      <c r="C12" s="132" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
-      <c r="G12" s="126"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6083,22 +6081,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="117"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="139" t="str">
+      <c r="C13" s="146" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="149"/>
-      <c r="E13" s="149"/>
-      <c r="F13" s="149"/>
-      <c r="G13" s="149"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="140"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="148"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="139" t="str">
+      <c r="K13" s="146" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="140"/>
+      <c r="L13" s="148"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6106,40 +6104,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="150" t="str">
+      <c r="C14" s="149" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="151"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="152"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="151"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="150" t="str">
+      <c r="I14" s="149" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="151"/>
-      <c r="K14" s="151"/>
-      <c r="L14" s="152"/>
+      <c r="J14" s="150"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="151"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="117"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="150" t="str">
+      <c r="C15" s="149" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="151"/>
-      <c r="L15" s="152"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="150"/>
+      <c r="L15" s="151"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6149,15 +6147,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="153" t="s">
+      <c r="E16" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="155"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
+      <c r="K16" s="154"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -6171,34 +6169,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="159" t="str">
+      <c r="E17" s="118" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="161"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="120"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="117"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="159" t="str">
+      <c r="C18" s="118" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
-      <c r="G18" s="160"/>
-      <c r="H18" s="160"/>
-      <c r="I18" s="162"/>
-      <c r="J18" s="162"/>
-      <c r="K18" s="163"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="122"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6208,23 +6206,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="117"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="133" t="str">
+      <c r="C19" s="123" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="135"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="133" t="str">
+      <c r="I19" s="123" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="134"/>
-      <c r="K19" s="134"/>
-      <c r="L19" s="134"/>
-      <c r="M19" s="135"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="125"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6233,14 +6231,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="166" t="str">
+      <c r="E20" s="128" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="168"/>
-      <c r="I20" s="169"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="131"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6250,12 +6248,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="143" t="str">
+      <c r="B21" s="140" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="144"/>
-      <c r="D21" s="145"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="142"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6274,11 +6272,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="164" t="str">
+      <c r="C22" s="126" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="165"/>
+      <c r="D22" s="127"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6299,13 +6297,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="170" t="str">
+      <c r="B23" s="135" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="171"/>
-      <c r="D23" s="171"/>
-      <c r="E23" s="172"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6325,12 +6323,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="146" t="str">
+      <c r="B24" s="143" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="147"/>
-      <c r="D24" s="148"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="145"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6345,15 +6343,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="156" t="str">
+      <c r="B25" s="114" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="158"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="116"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6386,43 +6384,24 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="114" t="s">
+      <c r="A27" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
+      <c r="H27" s="155"/>
+      <c r="I27" s="155"/>
+      <c r="J27" s="155"/>
+      <c r="K27" s="155"/>
+      <c r="L27" s="155"/>
+      <c r="M27" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6439,6 +6418,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve information on organism coverage
Co-authored-by: nocalla <16230431+nocalla@users.noreply.github.com>
Co-authored-by: github-actions <github-actions@github.com>
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall\Docs\Pharmacy\antibiogram\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30415803-AAE2-4458-9F45-C6CD7BAA9230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiogram" sheetId="3" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Antibiogram!$A$1:$O$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'original antibiogram'!$A$1:$M$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,14 +43,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -59,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -316,12 +322,18 @@
   </si>
   <si>
     <t>Gram negative cocci</t>
+  </si>
+  <si>
+    <t>e.g. Bacteroides sp.</t>
+  </si>
+  <si>
+    <t>e.g. Mycoplasma sp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -416,7 +428,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,12 +546,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,7 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1011,9 +1017,6 @@
     <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1167,6 +1170,129 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1176,9 +1302,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1197,15 +1320,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1224,15 +1338,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1241,111 +1346,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1354,6 +1354,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="62">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1615,16 +1625,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -1650,8 +1650,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
-  <autoFilter ref="B2:O39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="B2:O39" totalsRowShown="0" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B2:O39" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Amikacin"/>
@@ -1690,105 +1690,105 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="Drug Name" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Drug Name" dataDxfId="58">
       <calculatedColumnFormula>'Drug Information'!$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="MRSA" dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MRSA" dataDxfId="57">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="MSSA" dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MSSA" dataDxfId="56">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Streptococci" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Streptococci" dataDxfId="55">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="E. coli" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E. coli" dataDxfId="54">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="P. mirabilis" dataDxfId="52">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="P. mirabilis" dataDxfId="53">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Klebsiella" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Klebsiella" dataDxfId="52">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Pseudomonas" dataDxfId="50">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Pseudomonas" dataDxfId="51">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="ESCAPPM" dataDxfId="49">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ESCAPPM" dataDxfId="50">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="N. gonorrhoeae" dataDxfId="48">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="N. gonorrhoeae" dataDxfId="49">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="N. meningitidis" dataDxfId="47">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="N. meningitidis" dataDxfId="48">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="????" dataDxfId="46">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="????" dataDxfId="47">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="e.g. Mycoplasma" dataDxfId="45">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="e.g. Mycoplasma" dataDxfId="46">
       <calculatedColumnFormula>IF('Drug Information'!#REF!=1,"",".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Drug Name "/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Drug Name "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A1:B38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Drug Name" dataDxfId="42"/>
-    <tableColumn id="2" name="Drug Class" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Drug Name" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Drug Class" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:AM13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:AM13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="39">
-    <tableColumn id="1" name="Group" dataDxfId="38"/>
-    <tableColumn id="2" name="Name" dataDxfId="37"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="36"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="35"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="34"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="33"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="32"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="31"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="30"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="29"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="28"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="27"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="26"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="25"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="24"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="23"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="22"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="21"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="20"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="19"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="18"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="17"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="16"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="15"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="14"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="13"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="12"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="11"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="10"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="9"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="8"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="7"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="6"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="5"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="4"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="3"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="2"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="1"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Group" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Benzylpenicillin" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Naficillin" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Oxacillin" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Flucloxacillin" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Ampicillin" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Amoxicillin" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Amoxicillin-Clavulanic Acid" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Ampicillin/Sulbactam" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Piperacillin-Tazobactam" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Cefazolin" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Cefalexin" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Cefuroxime" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Cephotetan" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Cefoxitin" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Cefotaxime" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ceftriaxone" dataDxfId="22"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Ceftazidime" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Cefepime" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Ceftaroline" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Ertapenem" dataDxfId="18"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="Imipenem" dataDxfId="17"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="Meropenem" dataDxfId="16"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Aztreonam" dataDxfId="15"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="Ciprofloxacin" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Levofloxacin" dataDxfId="13"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="Moxifloxacin" dataDxfId="12"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="Gentamicin" dataDxfId="11"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="Tobramycin" dataDxfId="10"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="Amikacin" dataDxfId="9"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0200-000020000000}" name="Azithromycin" dataDxfId="8"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0200-000021000000}" name="Clindamycin" dataDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0200-000022000000}" name="Doxycycline" dataDxfId="6"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0200-000023000000}" name="Vancomycin" dataDxfId="5"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0200-000024000000}" name="Daptomycin" dataDxfId="4"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0200-000025000000}" name="Linezolid" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0200-000026000000}" name="Trimethoprim/Sulfamethoxazole" dataDxfId="2"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0200-000027000000}" name="Metronidazole" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2049,14 +2049,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2084,7 +2084,7 @@
     <col min="12" max="12" width="18.75" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.75" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.875" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.875" style="63" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="42.5" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.875" style="2" bestFit="1" customWidth="1"/>
@@ -2092,26 +2092,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="105" t="s">
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="106" t="s">
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="106"/>
+      <c r="L1" s="105"/>
       <c r="M1" s="33" t="s">
         <v>6</v>
       </c>
@@ -2121,8 +2121,8 @@
       <c r="O1" s="47"/>
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="100"/>
-      <c r="B2" s="66" t="s">
+      <c r="A2" s="99"/>
+      <c r="B2" s="65" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -2161,7 +2161,7 @@
       <c r="N2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="79" t="s">
+      <c r="O2" s="78" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2170,7 +2170,7 @@
         <f t="array" aca="1" ref="A3" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B3)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Penicillin</v>
       </c>
-      <c r="B3" s="67" t="str">
+      <c r="B3" s="66" t="str">
         <f>'Drug Information'!$A2</f>
         <v>Benzylpenicillin</v>
       </c>
@@ -2222,17 +2222,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O3" s="80" t="str">
+      <c r="O3" s="79" t="str">
         <f>'Drug Information'!$A2</f>
         <v>Benzylpenicillin</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="109" t="str" cm="1">
+      <c r="A4" s="108" t="str" cm="1">
         <f t="array" aca="1" ref="A4" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B4)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B4" s="67" t="str">
+      <c r="B4" s="66" t="str">
         <f>'Drug Information'!$A3</f>
         <v>Naficillin</v>
       </c>
@@ -2284,17 +2284,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O4" s="80" t="str">
+      <c r="O4" s="79" t="str">
         <f>'Drug Information'!$A3</f>
         <v>Naficillin</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="110" t="str" cm="1">
+      <c r="A5" s="109" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B5)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B5" s="67" t="str">
+      <c r="B5" s="66" t="str">
         <f>'Drug Information'!$A4</f>
         <v>Oxacillin</v>
       </c>
@@ -2346,17 +2346,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O5" s="80" t="str">
+      <c r="O5" s="79" t="str">
         <f>'Drug Information'!$A4</f>
         <v>Oxacillin</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="111" t="str" cm="1">
+      <c r="A6" s="110" t="str" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B6)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Anti-staphylococcal penicillins</v>
       </c>
-      <c r="B6" s="67" t="str">
+      <c r="B6" s="66" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
@@ -2408,17 +2408,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O6" s="80" t="str">
+      <c r="O6" s="79" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="109" t="str" cm="1">
+      <c r="A7" s="108" t="str" cm="1">
         <f t="array" aca="1" ref="A7" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B7)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins</v>
       </c>
-      <c r="B7" s="67" t="str">
+      <c r="B7" s="66" t="str">
         <f>'Drug Information'!$A6</f>
         <v>Ampicillin</v>
       </c>
@@ -2470,17 +2470,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O7" s="80" t="str">
+      <c r="O7" s="79" t="str">
         <f>'Drug Information'!$A6</f>
         <v>Ampicillin</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="111" t="str" cm="1">
+      <c r="A8" s="110" t="str" cm="1">
         <f t="array" aca="1" ref="A8" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B8)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins</v>
       </c>
-      <c r="B8" s="67" t="str">
+      <c r="B8" s="66" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
@@ -2532,17 +2532,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O8" s="80" t="str">
+      <c r="O8" s="79" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="103" t="str" cm="1">
+      <c r="A9" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B9)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B9" s="68" t="str">
+      <c r="B9" s="67" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
@@ -2594,17 +2594,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O9" s="81" t="str">
+      <c r="O9" s="80" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="103" t="str" cm="1">
+      <c r="A10" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B10)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B10" s="68" t="str">
+      <c r="B10" s="67" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
@@ -2656,17 +2656,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O10" s="81" t="str">
+      <c r="O10" s="80" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="103" t="str" cm="1">
+      <c r="A11" s="102" t="str" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B11)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminopenicillins with beta-lactamase inhibitors</v>
       </c>
-      <c r="B11" s="68" t="str">
+      <c r="B11" s="67" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
@@ -2718,17 +2718,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O11" s="81" t="str">
+      <c r="O11" s="80" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="107" t="str" cm="1">
+      <c r="A12" s="106" t="str" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B12)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>1st-gen cephalosporin</v>
       </c>
-      <c r="B12" s="69" t="str">
+      <c r="B12" s="68" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
@@ -2780,17 +2780,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O12" s="82" t="str">
+      <c r="O12" s="81" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="108" t="str" cm="1">
+      <c r="A13" s="107" t="str" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B13)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>1st-gen cephalosporin</v>
       </c>
-      <c r="B13" s="69" t="str">
+      <c r="B13" s="68" t="str">
         <f>'Drug Information'!$A12</f>
         <v>Cefalexin</v>
       </c>
@@ -2842,17 +2842,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O13" s="82" t="str">
+      <c r="O13" s="81" t="str">
         <f>'Drug Information'!$A12</f>
         <v>Cefalexin</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="95" t="str" cm="1">
+      <c r="A14" s="94" t="str" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B14)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B14" s="69" t="str">
+      <c r="B14" s="68" t="str">
         <f>'Drug Information'!$A13</f>
         <v>Cefuroxime</v>
       </c>
@@ -2904,17 +2904,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O14" s="82" t="str">
+      <c r="O14" s="81" t="str">
         <f>'Drug Information'!$A13</f>
         <v>Cefuroxime</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="96" t="str" cm="1">
+      <c r="A15" s="95" t="str" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B15)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B15" s="69" t="str">
+      <c r="B15" s="68" t="str">
         <f>'Drug Information'!$A14</f>
         <v>Cephotetan</v>
       </c>
@@ -2966,17 +2966,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O15" s="82" t="str">
+      <c r="O15" s="81" t="str">
         <f>'Drug Information'!$A14</f>
         <v>Cephotetan</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="97" t="str" cm="1">
+      <c r="A16" s="96" t="str" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B16)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>2nd-gen cephalosporin</v>
       </c>
-      <c r="B16" s="69" t="str">
+      <c r="B16" s="68" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
@@ -3028,17 +3028,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O16" s="82" t="str">
+      <c r="O16" s="81" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="95" t="str" cm="1">
+      <c r="A17" s="94" t="str" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B17)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B17" s="69" t="str">
+      <c r="B17" s="68" t="str">
         <f>'Drug Information'!$A16</f>
         <v>Cefotaxime</v>
       </c>
@@ -3090,17 +3090,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O17" s="82" t="str">
+      <c r="O17" s="81" t="str">
         <f>'Drug Information'!$A16</f>
         <v>Cefotaxime</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="96" t="str" cm="1">
+      <c r="A18" s="95" t="str" cm="1">
         <f t="array" aca="1" ref="A18" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B18)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>3rd-gen cephalosporin</v>
       </c>
-      <c r="B18" s="69" t="str">
+      <c r="B18" s="68" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
@@ -3152,17 +3152,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O18" s="82" t="str">
+      <c r="O18" s="81" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="97" t="str" cm="1">
+      <c r="A19" s="96" t="str" cm="1">
         <f t="array" aca="1" ref="A19" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B19)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>4th-gen cephalosporin</v>
       </c>
-      <c r="B19" s="69" t="str">
+      <c r="B19" s="68" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
@@ -3214,7 +3214,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O19" s="82" t="str">
+      <c r="O19" s="81" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
@@ -3224,7 +3224,7 @@
         <f t="array" aca="1" ref="A20" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B20)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>4th-gen cephalosporin</v>
       </c>
-      <c r="B20" s="69" t="str">
+      <c r="B20" s="68" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
@@ -3276,7 +3276,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O20" s="82" t="str">
+      <c r="O20" s="81" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
@@ -3286,7 +3286,7 @@
         <f t="array" aca="1" ref="A21" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B21)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>5th-gen cephalosporin</v>
       </c>
-      <c r="B21" s="69" t="str">
+      <c r="B21" s="68" t="str">
         <f>'Drug Information'!$A20</f>
         <v>Ceftaroline</v>
       </c>
@@ -3338,17 +3338,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O21" s="82" t="str">
+      <c r="O21" s="81" t="str">
         <f>'Drug Information'!$A20</f>
         <v>Ceftaroline</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="101" t="str" cm="1">
+      <c r="A22" s="100" t="str" cm="1">
         <f t="array" aca="1" ref="A22" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B22)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B22" s="70" t="str">
+      <c r="B22" s="69" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
@@ -3400,17 +3400,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O22" s="83" t="str">
+      <c r="O22" s="82" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="101" t="str" cm="1">
+      <c r="A23" s="100" t="str" cm="1">
         <f t="array" aca="1" ref="A23" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B23)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B23" s="70" t="str">
+      <c r="B23" s="69" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Imipenem</v>
       </c>
@@ -3462,17 +3462,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O23" s="83" t="str">
+      <c r="O23" s="82" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Imipenem</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="101" t="str" cm="1">
+      <c r="A24" s="100" t="str" cm="1">
         <f t="array" aca="1" ref="A24" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B24)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Carbapenems</v>
       </c>
-      <c r="B24" s="70" t="str">
+      <c r="B24" s="69" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
@@ -3524,7 +3524,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O24" s="83" t="str">
+      <c r="O24" s="82" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
@@ -3534,7 +3534,7 @@
         <f t="array" aca="1" ref="A25" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B25)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Monobactams</v>
       </c>
-      <c r="B25" s="71" t="str">
+      <c r="B25" s="70" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Aztreonam</v>
       </c>
@@ -3586,17 +3586,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O25" s="84" t="str">
+      <c r="O25" s="83" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Aztreonam</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="102" t="str" cm="1">
+      <c r="A26" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A26" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B26)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B26" s="72" t="str">
+      <c r="B26" s="71" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
@@ -3648,17 +3648,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O26" s="85" t="str">
+      <c r="O26" s="84" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="102" t="str" cm="1">
+      <c r="A27" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A27" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B27)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B27" s="72" t="str">
+      <c r="B27" s="71" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
@@ -3710,17 +3710,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O27" s="85" t="str">
+      <c r="O27" s="84" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="102" t="str" cm="1">
+      <c r="A28" s="101" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B28)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Quinolones</v>
       </c>
-      <c r="B28" s="72" t="str">
+      <c r="B28" s="71" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
@@ -3772,17 +3772,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O28" s="85" t="str">
+      <c r="O28" s="84" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="112" t="str" cm="1">
+      <c r="A29" s="111" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B29)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B29" s="73" t="str">
+      <c r="B29" s="72" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Gentamicin</v>
       </c>
@@ -3834,17 +3834,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O29" s="86" t="str">
+      <c r="O29" s="85" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Gentamicin</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="113" t="str" cm="1">
+      <c r="A30" s="112" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B30)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B30" s="73" t="str">
+      <c r="B30" s="72" t="str">
         <f>'Drug Information'!$A29</f>
         <v>Tobramycin</v>
       </c>
@@ -3896,17 +3896,17 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O30" s="86" t="str">
+      <c r="O30" s="85" t="str">
         <f>'Drug Information'!$A29</f>
         <v>Tobramycin</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="114" t="str" cm="1">
+      <c r="A31" s="113" t="str" cm="1">
         <f t="array" aca="1" ref="A31" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B31)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Aminoglycosides</v>
       </c>
-      <c r="B31" s="73" t="str">
+      <c r="B31" s="72" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
@@ -3958,7 +3958,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O31" s="86" t="str">
+      <c r="O31" s="85" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
@@ -3968,7 +3968,7 @@
         <f t="array" aca="1" ref="A32" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B32)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Macrolides</v>
       </c>
-      <c r="B32" s="74" t="str">
+      <c r="B32" s="73" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
@@ -4020,7 +4020,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O32" s="87" t="str">
+      <c r="O32" s="86" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
@@ -4030,7 +4030,7 @@
         <f t="array" aca="1" ref="A33" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B33)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Lincosamide</v>
       </c>
-      <c r="B33" s="75" t="str">
+      <c r="B33" s="74" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
@@ -4082,7 +4082,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O33" s="88" t="str">
+      <c r="O33" s="87" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
@@ -4092,7 +4092,7 @@
         <f t="array" aca="1" ref="A34" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B34)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Tetracyclines</v>
       </c>
-      <c r="B34" s="76" t="str">
+      <c r="B34" s="75" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
@@ -4144,7 +4144,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O34" s="89" t="str">
+      <c r="O34" s="88" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
@@ -4154,7 +4154,7 @@
         <f t="array" aca="1" ref="A35" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B35)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Glycopeptides</v>
       </c>
-      <c r="B35" s="77" t="str">
+      <c r="B35" s="76" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
@@ -4206,7 +4206,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O35" s="90" t="str">
+      <c r="O35" s="89" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
@@ -4216,7 +4216,7 @@
         <f t="array" aca="1" ref="A36" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B36)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Lipopeptides</v>
       </c>
-      <c r="B36" s="77" t="str">
+      <c r="B36" s="76" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Daptomycin</v>
       </c>
@@ -4268,7 +4268,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O36" s="90" t="str">
+      <c r="O36" s="89" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Daptomycin</v>
       </c>
@@ -4278,7 +4278,7 @@
         <f t="array" aca="1" ref="A37" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B37)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Oxazolidinones</v>
       </c>
-      <c r="B37" s="77" t="str">
+      <c r="B37" s="76" t="str">
         <f>'Drug Information'!$A36</f>
         <v>Linezolid</v>
       </c>
@@ -4330,14 +4330,14 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O37" s="90"/>
+      <c r="O37" s="89"/>
     </row>
     <row r="38" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B38)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Antimetabolite</v>
       </c>
-      <c r="B38" s="78" t="str">
+      <c r="B38" s="77" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
@@ -4389,7 +4389,7 @@
         <f>IF('Drug Information'!#REF!=1,"",".")</f>
         <v>#REF!</v>
       </c>
-      <c r="O38" s="91" t="str">
+      <c r="O38" s="90" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
@@ -4399,101 +4399,101 @@
         <f t="array" aca="1" ref="A39" ca="1">VLOOKUP(INDIRECT("B"&amp;ROW(B39)), drug_info[[Drug Name]:[Drug Class]], 2, FALSE)</f>
         <v>Nitroimidazoles</v>
       </c>
-      <c r="B39" s="92" t="str">
+      <c r="B39" s="91" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Metronidazole</v>
       </c>
-      <c r="C39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N39" s="65" t="e">
-        <f>IF('Drug Information'!#REF!=1,"",".")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O39" s="93" t="str">
+      <c r="C39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N39" s="64" t="e">
+        <f>IF('Drug Information'!#REF!=1,"",".")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O39" s="92" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Metronidazole</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="98" t="s">
+      <c r="A40" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="98"/>
-      <c r="C40" s="98"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="98"/>
-      <c r="I40" s="98"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="98"/>
-      <c r="L40" s="98"/>
-      <c r="M40" s="98"/>
-      <c r="N40" s="98"/>
-      <c r="O40" s="98"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="97"/>
+      <c r="H40" s="97"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="97"/>
+      <c r="K40" s="97"/>
+      <c r="L40" s="97"/>
+      <c r="M40" s="97"/>
+      <c r="N40" s="97"/>
+      <c r="O40" s="97"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="94"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="94"/>
-      <c r="F42" s="94"/>
-      <c r="G42" s="94"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="94"/>
-      <c r="J42" s="94"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="94"/>
-      <c r="O42" s="94"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4513,7 +4513,7 @@
     <mergeCell ref="A29:A31"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N39">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"."</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4526,14 +4526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4640,10 +4640,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="174" t="s">
+      <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4664,10 +4664,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="31" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4696,10 +4696,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="31" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4816,18 +4816,18 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="31" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4856,908 +4856,909 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4260" ySplit="7875" topLeftCell="AA25" activePane="topRight"/>
-      <selection pane="topRight" activeCell="AK5" sqref="AK5"/>
+      <pane xSplit="10320" ySplit="7875" topLeftCell="A25"/>
+      <selection activeCell="C21" sqref="C21"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="64" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.125" style="64" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.625" style="64" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.875" style="64" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.625" style="64" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.75" style="64" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.75" style="64" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14" style="64" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.75" style="64" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.625" style="64" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13" style="64" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.75" style="64" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13" style="64" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="13.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.375" style="64" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31.25" style="64" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.5" style="64" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9" style="64"/>
+    <col min="1" max="1" width="18.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.125" style="63" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="63" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" style="63" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.75" style="63" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="13.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.375" style="63" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.25" style="63" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.5" style="63" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9" style="63"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="J1" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="64" t="s">
+      <c r="K1" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="64" t="s">
+      <c r="N1" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="64" t="s">
+      <c r="O1" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="Q1" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="64" t="s">
+      <c r="V1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="64" t="s">
+      <c r="W1" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="64" t="s">
+      <c r="X1" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="64" t="s">
+      <c r="Y1" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="64" t="s">
+      <c r="Z1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="64" t="s">
+      <c r="AA1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="64" t="s">
+      <c r="AC1" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="64" t="s">
+      <c r="AD1" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="64" t="s">
+      <c r="AE1" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="64" t="s">
+      <c r="AF1" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="64" t="s">
+      <c r="AG1" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" s="64" t="s">
+      <c r="AH1" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="AI1" s="64" t="s">
+      <c r="AI1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="64" t="s">
+      <c r="AJ1" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" s="64" t="s">
+      <c r="AK1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="AL1" s="64" t="s">
+      <c r="AL1" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="AM1" s="64" t="s">
+      <c r="AM1" s="63" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="64">
+      <c r="B2" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="64">
-        <v>1</v>
-      </c>
-      <c r="E3" s="64">
-        <v>1</v>
-      </c>
-      <c r="F3" s="64">
-        <v>1</v>
-      </c>
-      <c r="I3" s="64">
-        <v>1</v>
-      </c>
-      <c r="J3" s="64">
-        <v>1</v>
-      </c>
-      <c r="K3" s="64">
-        <v>1</v>
-      </c>
-      <c r="L3" s="64">
-        <v>1</v>
-      </c>
-      <c r="M3" s="64">
-        <v>1</v>
-      </c>
-      <c r="N3" s="64">
-        <v>1</v>
-      </c>
-      <c r="O3" s="64">
-        <v>1</v>
-      </c>
-      <c r="P3" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="64">
-        <v>1</v>
-      </c>
-      <c r="R3" s="64">
-        <v>1</v>
-      </c>
-      <c r="T3" s="64">
-        <v>1</v>
-      </c>
-      <c r="U3" s="64">
-        <v>1</v>
-      </c>
-      <c r="V3" s="64">
-        <v>1</v>
-      </c>
-      <c r="W3" s="64">
-        <v>1</v>
-      </c>
-      <c r="X3" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="64">
+      <c r="D3" s="63">
+        <v>1</v>
+      </c>
+      <c r="E3" s="63">
+        <v>1</v>
+      </c>
+      <c r="F3" s="63">
+        <v>1</v>
+      </c>
+      <c r="I3" s="63">
+        <v>1</v>
+      </c>
+      <c r="J3" s="63">
+        <v>1</v>
+      </c>
+      <c r="K3" s="63">
+        <v>1</v>
+      </c>
+      <c r="L3" s="63">
+        <v>1</v>
+      </c>
+      <c r="M3" s="63">
+        <v>1</v>
+      </c>
+      <c r="N3" s="63">
+        <v>1</v>
+      </c>
+      <c r="O3" s="63">
+        <v>1</v>
+      </c>
+      <c r="P3" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="63">
+        <v>1</v>
+      </c>
+      <c r="R3" s="63">
+        <v>1</v>
+      </c>
+      <c r="T3" s="63">
+        <v>1</v>
+      </c>
+      <c r="U3" s="63">
+        <v>1</v>
+      </c>
+      <c r="V3" s="63">
+        <v>1</v>
+      </c>
+      <c r="W3" s="63">
+        <v>1</v>
+      </c>
+      <c r="X3" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="64">
-        <v>1</v>
-      </c>
-      <c r="D4" s="64">
-        <v>1</v>
-      </c>
-      <c r="E4" s="64">
-        <v>1</v>
-      </c>
-      <c r="F4" s="64">
-        <v>1</v>
-      </c>
-      <c r="G4" s="64">
-        <v>1</v>
-      </c>
-      <c r="H4" s="64">
-        <v>1</v>
-      </c>
-      <c r="I4" s="64">
-        <v>1</v>
-      </c>
-      <c r="J4" s="64">
-        <v>1</v>
-      </c>
-      <c r="K4" s="64">
-        <v>1</v>
-      </c>
-      <c r="L4" s="64">
-        <v>1</v>
-      </c>
-      <c r="M4" s="64">
-        <v>1</v>
-      </c>
-      <c r="N4" s="64">
-        <v>1</v>
-      </c>
-      <c r="O4" s="64">
-        <v>1</v>
-      </c>
-      <c r="P4" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="64">
-        <v>1</v>
-      </c>
-      <c r="R4" s="64">
-        <v>1</v>
-      </c>
-      <c r="S4" s="64">
-        <v>1</v>
-      </c>
-      <c r="T4" s="64">
-        <v>1</v>
-      </c>
-      <c r="U4" s="64">
-        <v>1</v>
-      </c>
-      <c r="V4" s="64">
-        <v>1</v>
-      </c>
-      <c r="W4" s="64">
-        <v>1</v>
-      </c>
-      <c r="X4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="64">
+      <c r="C4" s="63">
+        <v>1</v>
+      </c>
+      <c r="D4" s="63">
+        <v>1</v>
+      </c>
+      <c r="E4" s="63">
+        <v>1</v>
+      </c>
+      <c r="F4" s="63">
+        <v>1</v>
+      </c>
+      <c r="G4" s="63">
+        <v>1</v>
+      </c>
+      <c r="H4" s="63">
+        <v>1</v>
+      </c>
+      <c r="I4" s="63">
+        <v>1</v>
+      </c>
+      <c r="J4" s="63">
+        <v>1</v>
+      </c>
+      <c r="K4" s="63">
+        <v>1</v>
+      </c>
+      <c r="L4" s="63">
+        <v>1</v>
+      </c>
+      <c r="M4" s="63">
+        <v>1</v>
+      </c>
+      <c r="N4" s="63">
+        <v>1</v>
+      </c>
+      <c r="O4" s="63">
+        <v>1</v>
+      </c>
+      <c r="P4" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="63">
+        <v>1</v>
+      </c>
+      <c r="R4" s="63">
+        <v>1</v>
+      </c>
+      <c r="S4" s="63">
+        <v>1</v>
+      </c>
+      <c r="T4" s="63">
+        <v>1</v>
+      </c>
+      <c r="U4" s="63">
+        <v>1</v>
+      </c>
+      <c r="V4" s="63">
+        <v>1</v>
+      </c>
+      <c r="W4" s="63">
+        <v>1</v>
+      </c>
+      <c r="X4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="64">
-        <v>1</v>
-      </c>
-      <c r="H5" s="64">
-        <v>1</v>
-      </c>
-      <c r="I5" s="64">
-        <v>1</v>
-      </c>
-      <c r="J5" s="64">
-        <v>1</v>
-      </c>
-      <c r="K5" s="64">
-        <v>1</v>
-      </c>
-      <c r="L5" s="64">
-        <v>1</v>
-      </c>
-      <c r="M5" s="64">
-        <v>1</v>
-      </c>
-      <c r="N5" s="64">
-        <v>1</v>
-      </c>
-      <c r="O5" s="64">
-        <v>1</v>
-      </c>
-      <c r="P5" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="64">
-        <v>1</v>
-      </c>
-      <c r="R5" s="64">
-        <v>1</v>
-      </c>
-      <c r="S5" s="64">
-        <v>1</v>
-      </c>
-      <c r="T5" s="64">
-        <v>1</v>
-      </c>
-      <c r="U5" s="64">
-        <v>1</v>
-      </c>
-      <c r="V5" s="64">
-        <v>1</v>
-      </c>
-      <c r="W5" s="64">
-        <v>1</v>
-      </c>
-      <c r="X5" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="64">
+      <c r="G5" s="63">
+        <v>1</v>
+      </c>
+      <c r="H5" s="63">
+        <v>1</v>
+      </c>
+      <c r="I5" s="63">
+        <v>1</v>
+      </c>
+      <c r="J5" s="63">
+        <v>1</v>
+      </c>
+      <c r="K5" s="63">
+        <v>1</v>
+      </c>
+      <c r="L5" s="63">
+        <v>1</v>
+      </c>
+      <c r="M5" s="63">
+        <v>1</v>
+      </c>
+      <c r="N5" s="63">
+        <v>1</v>
+      </c>
+      <c r="O5" s="63">
+        <v>1</v>
+      </c>
+      <c r="P5" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="63">
+        <v>1</v>
+      </c>
+      <c r="R5" s="63">
+        <v>1</v>
+      </c>
+      <c r="S5" s="63">
+        <v>1</v>
+      </c>
+      <c r="T5" s="63">
+        <v>1</v>
+      </c>
+      <c r="U5" s="63">
+        <v>1</v>
+      </c>
+      <c r="V5" s="63">
+        <v>1</v>
+      </c>
+      <c r="W5" s="63">
+        <v>1</v>
+      </c>
+      <c r="X5" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="64">
-        <v>1</v>
-      </c>
-      <c r="H6" s="64">
-        <v>1</v>
-      </c>
-      <c r="I6" s="64">
-        <v>1</v>
-      </c>
-      <c r="J6" s="64">
-        <v>1</v>
-      </c>
-      <c r="K6" s="64">
-        <v>1</v>
-      </c>
-      <c r="L6" s="64">
-        <v>1</v>
-      </c>
-      <c r="M6" s="64">
-        <v>1</v>
-      </c>
-      <c r="N6" s="64">
-        <v>1</v>
-      </c>
-      <c r="O6" s="64">
-        <v>1</v>
-      </c>
-      <c r="P6" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="64">
-        <v>1</v>
-      </c>
-      <c r="R6" s="64">
-        <v>1</v>
-      </c>
-      <c r="S6" s="64">
-        <v>1</v>
-      </c>
-      <c r="T6" s="64">
-        <v>1</v>
-      </c>
-      <c r="U6" s="64">
-        <v>1</v>
-      </c>
-      <c r="V6" s="64">
-        <v>1</v>
-      </c>
-      <c r="W6" s="64">
-        <v>1</v>
-      </c>
-      <c r="X6" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="64">
+      <c r="G6" s="63">
+        <v>1</v>
+      </c>
+      <c r="H6" s="63">
+        <v>1</v>
+      </c>
+      <c r="I6" s="63">
+        <v>1</v>
+      </c>
+      <c r="J6" s="63">
+        <v>1</v>
+      </c>
+      <c r="K6" s="63">
+        <v>1</v>
+      </c>
+      <c r="L6" s="63">
+        <v>1</v>
+      </c>
+      <c r="M6" s="63">
+        <v>1</v>
+      </c>
+      <c r="N6" s="63">
+        <v>1</v>
+      </c>
+      <c r="O6" s="63">
+        <v>1</v>
+      </c>
+      <c r="P6" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="63">
+        <v>1</v>
+      </c>
+      <c r="R6" s="63">
+        <v>1</v>
+      </c>
+      <c r="S6" s="63">
+        <v>1</v>
+      </c>
+      <c r="T6" s="63">
+        <v>1</v>
+      </c>
+      <c r="U6" s="63">
+        <v>1</v>
+      </c>
+      <c r="V6" s="63">
+        <v>1</v>
+      </c>
+      <c r="W6" s="63">
+        <v>1</v>
+      </c>
+      <c r="X6" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="64">
-        <v>1</v>
-      </c>
-      <c r="J7" s="64">
-        <v>1</v>
-      </c>
-      <c r="K7" s="64">
-        <v>1</v>
-      </c>
-      <c r="L7" s="64">
-        <v>1</v>
-      </c>
-      <c r="M7" s="64">
-        <v>1</v>
-      </c>
-      <c r="N7" s="64">
-        <v>1</v>
-      </c>
-      <c r="O7" s="64">
-        <v>1</v>
-      </c>
-      <c r="P7" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="64">
-        <v>1</v>
-      </c>
-      <c r="R7" s="64">
-        <v>1</v>
-      </c>
-      <c r="S7" s="64">
-        <v>1</v>
-      </c>
-      <c r="T7" s="64">
-        <v>1</v>
-      </c>
-      <c r="U7" s="64">
-        <v>1</v>
-      </c>
-      <c r="V7" s="64">
-        <v>1</v>
-      </c>
-      <c r="W7" s="64">
-        <v>1</v>
-      </c>
-      <c r="X7" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="64">
+      <c r="I7" s="63">
+        <v>1</v>
+      </c>
+      <c r="J7" s="63">
+        <v>1</v>
+      </c>
+      <c r="K7" s="63">
+        <v>1</v>
+      </c>
+      <c r="L7" s="63">
+        <v>1</v>
+      </c>
+      <c r="M7" s="63">
+        <v>1</v>
+      </c>
+      <c r="N7" s="63">
+        <v>1</v>
+      </c>
+      <c r="O7" s="63">
+        <v>1</v>
+      </c>
+      <c r="P7" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="63">
+        <v>1</v>
+      </c>
+      <c r="R7" s="63">
+        <v>1</v>
+      </c>
+      <c r="S7" s="63">
+        <v>1</v>
+      </c>
+      <c r="T7" s="63">
+        <v>1</v>
+      </c>
+      <c r="U7" s="63">
+        <v>1</v>
+      </c>
+      <c r="V7" s="63">
+        <v>1</v>
+      </c>
+      <c r="W7" s="63">
+        <v>1</v>
+      </c>
+      <c r="X7" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="64">
-        <v>1</v>
-      </c>
-      <c r="S8" s="64">
-        <v>1</v>
-      </c>
-      <c r="T8" s="64">
-        <v>1</v>
-      </c>
-      <c r="W8" s="64">
-        <v>1</v>
-      </c>
-      <c r="X8" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="64">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="64">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="64">
+      <c r="K8" s="63">
+        <v>1</v>
+      </c>
+      <c r="S8" s="63">
+        <v>1</v>
+      </c>
+      <c r="T8" s="63">
+        <v>1</v>
+      </c>
+      <c r="W8" s="63">
+        <v>1</v>
+      </c>
+      <c r="X8" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="64">
-        <v>1</v>
-      </c>
-      <c r="R9" s="64">
-        <v>1</v>
-      </c>
-      <c r="T9" s="64">
-        <v>1</v>
-      </c>
-      <c r="U9" s="64">
-        <v>1</v>
-      </c>
-      <c r="V9" s="64">
-        <v>1</v>
-      </c>
-      <c r="W9" s="64">
-        <v>1</v>
-      </c>
-      <c r="X9" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AJ9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AK9" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="64">
+      <c r="K9" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="63">
+        <v>1</v>
+      </c>
+      <c r="R9" s="63">
+        <v>1</v>
+      </c>
+      <c r="T9" s="63">
+        <v>1</v>
+      </c>
+      <c r="U9" s="63">
+        <v>1</v>
+      </c>
+      <c r="V9" s="63">
+        <v>1</v>
+      </c>
+      <c r="W9" s="63">
+        <v>1</v>
+      </c>
+      <c r="X9" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="64">
-        <v>1</v>
-      </c>
-      <c r="T10" s="64">
-        <v>1</v>
-      </c>
-      <c r="V10" s="64">
-        <v>1</v>
-      </c>
-      <c r="W10" s="64">
-        <v>1</v>
-      </c>
-      <c r="X10" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="64">
+      <c r="R10" s="63">
+        <v>1</v>
+      </c>
+      <c r="T10" s="63">
+        <v>1</v>
+      </c>
+      <c r="V10" s="63">
+        <v>1</v>
+      </c>
+      <c r="W10" s="63">
+        <v>1</v>
+      </c>
+      <c r="X10" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="64">
-        <v>1</v>
-      </c>
-      <c r="H11" s="64">
-        <v>1</v>
-      </c>
-      <c r="K11" s="64">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="64">
-        <v>1</v>
-      </c>
-      <c r="R11" s="64">
-        <v>1</v>
-      </c>
-      <c r="T11" s="64">
-        <v>1</v>
-      </c>
-      <c r="V11" s="64">
-        <v>1</v>
-      </c>
-      <c r="W11" s="64">
-        <v>1</v>
-      </c>
-      <c r="X11" s="64">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="64">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="64">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="64">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="64">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="64">
+      <c r="G11" s="63">
+        <v>1</v>
+      </c>
+      <c r="H11" s="63">
+        <v>1</v>
+      </c>
+      <c r="K11" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="63">
+        <v>1</v>
+      </c>
+      <c r="R11" s="63">
+        <v>1</v>
+      </c>
+      <c r="T11" s="63">
+        <v>1</v>
+      </c>
+      <c r="V11" s="63">
+        <v>1</v>
+      </c>
+      <c r="W11" s="63">
+        <v>1</v>
+      </c>
+      <c r="X11" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="63">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="63">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="63">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL11" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="64">
-        <v>1</v>
-      </c>
-      <c r="J12" s="64">
-        <v>1</v>
-      </c>
-      <c r="K12" s="64">
-        <v>1</v>
-      </c>
-      <c r="O12" s="64">
-        <v>1</v>
-      </c>
-      <c r="P12" s="64">
-        <v>1</v>
-      </c>
-      <c r="V12" s="64">
-        <v>1</v>
-      </c>
-      <c r="W12" s="64">
-        <v>1</v>
-      </c>
-      <c r="X12" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="64">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="64">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="64">
+      <c r="B12" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="63">
+        <v>1</v>
+      </c>
+      <c r="J12" s="63">
+        <v>1</v>
+      </c>
+      <c r="K12" s="63">
+        <v>1</v>
+      </c>
+      <c r="O12" s="63">
+        <v>1</v>
+      </c>
+      <c r="P12" s="63">
+        <v>1</v>
+      </c>
+      <c r="V12" s="63">
+        <v>1</v>
+      </c>
+      <c r="W12" s="63">
+        <v>1</v>
+      </c>
+      <c r="X12" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="63">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA13" s="64">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="64">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="64">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="64">
+      <c r="B13" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA13" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="63">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="63">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="63">
         <v>1</v>
       </c>
     </row>
@@ -5770,7 +5771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -5804,23 +5805,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="128" t="s">
+      <c r="C1" s="168"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="116" t="s">
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="117"/>
-      <c r="L1" s="142" t="s">
+      <c r="K1" s="157"/>
+      <c r="L1" s="138" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -5861,7 +5862,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="143"/>
+      <c r="L2" s="139"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -5891,11 +5892,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="119" t="str">
+      <c r="C4" s="158" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="120"/>
+      <c r="D4" s="159"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5912,12 +5913,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="119" t="str">
+      <c r="D5" s="158" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="121"/>
-      <c r="F5" s="120"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="159"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5934,14 +5935,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="122" t="str">
+      <c r="C6" s="161" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="124"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5954,14 +5955,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="122" t="str">
+      <c r="C7" s="161" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="124"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -5973,40 +5974,40 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="117" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="122" t="str">
+      <c r="C8" s="161" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="124"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="122" t="str">
+      <c r="I8" s="161" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="137"/>
-      <c r="K8" s="124"/>
+      <c r="J8" s="170"/>
+      <c r="K8" s="163"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="118"/>
+      <c r="A9" s="117"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="122" t="str">
+      <c r="D9" s="161" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="124"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="163"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -6018,34 +6019,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="138" t="str">
+      <c r="C10" s="171" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="139"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="137"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="124"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="170"/>
+      <c r="I10" s="170"/>
+      <c r="J10" s="170"/>
+      <c r="K10" s="163"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="117" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="125" t="str">
+      <c r="C11" s="132" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="127"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="134"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6057,16 +6058,16 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="118"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="125" t="str">
+      <c r="C12" s="132" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="127"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6078,65 +6079,65 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="118"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="140" t="str">
+      <c r="C13" s="146" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="141"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="148"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="140" t="str">
+      <c r="K13" s="146" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="141"/>
+      <c r="L13" s="148"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="117" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="151" t="str">
+      <c r="C14" s="149" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="152"/>
-      <c r="E14" s="152"/>
-      <c r="F14" s="152"/>
-      <c r="G14" s="153"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="151"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="151" t="str">
+      <c r="I14" s="149" t="str">
         <f>'Drug Information'!$A21</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="152"/>
-      <c r="K14" s="152"/>
-      <c r="L14" s="153"/>
+      <c r="J14" s="150"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="151"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="118"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="151" t="str">
+      <c r="C15" s="149" t="str">
         <f>'Drug Information'!$A23</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="152"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="152"/>
-      <c r="J15" s="152"/>
-      <c r="K15" s="152"/>
-      <c r="L15" s="153"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="150"/>
+      <c r="L15" s="151"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6146,20 +6147,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="155"/>
-      <c r="G16" s="155"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="155"/>
-      <c r="J16" s="155"/>
-      <c r="K16" s="156"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
+      <c r="K16" s="154"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="117" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -6168,34 +6169,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="160" t="str">
+      <c r="E17" s="118" t="str">
         <f>'Drug Information'!$A25</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="162"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="120"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="160" t="str">
+      <c r="C18" s="118" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="161"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-      <c r="G18" s="161"/>
-      <c r="H18" s="161"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="164"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="122"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A26</f>
@@ -6203,25 +6204,25 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="134" t="str">
+      <c r="C19" s="123" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="136"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="134" t="str">
+      <c r="I19" s="123" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="136"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="125"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -6230,14 +6231,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="167" t="str">
+      <c r="E20" s="128" t="str">
         <f>'Drug Information'!$A30</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="170"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="131"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -6247,12 +6248,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="144" t="str">
+      <c r="B21" s="140" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="145"/>
-      <c r="D21" s="146"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="142"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -6271,11 +6272,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="165" t="str">
+      <c r="C22" s="126" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="166"/>
+      <c r="D22" s="127"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -6296,13 +6297,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="171" t="str">
+      <c r="B23" s="135" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="172"/>
-      <c r="D23" s="172"/>
-      <c r="E23" s="173"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -6322,12 +6323,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="147" t="str">
+      <c r="B24" s="143" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="148"/>
-      <c r="D24" s="149"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="145"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -6342,15 +6343,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="157" t="str">
+      <c r="B25" s="114" t="str">
         <f>'Drug Information'!$A37</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="159"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="116"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -6383,43 +6384,24 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="115" t="s">
+      <c r="A27" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="115"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="115"/>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
+      <c r="H27" s="155"/>
+      <c r="I27" s="155"/>
+      <c r="J27" s="155"/>
+      <c r="K27" s="155"/>
+      <c r="L27" s="155"/>
+      <c r="M27" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -6436,6 +6418,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>